<commit_message>
ip cím számolás, kisebb változás PT-ben
2024.03.09
</commit_message>
<xml_diff>
--- a/IP_cim_kiosztas.xlsx
+++ b/IP_cim_kiosztas.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Üzemeltető\vizsgaremek\Uzemelteto_vizsgaremek_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Vizsgaremek\Uzemelteto_vizsgaremek_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F290C56D-F311-4D2E-B77F-69CBFACB9904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605B570A-93AC-4C07-A317-ACAF228F974C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5DEB228F-9A24-4144-85FF-8E6948A8BA71}"/>
+    <workbookView xWindow="3495" yWindow="4425" windowWidth="16860" windowHeight="15345" activeTab="3" xr2:uid="{5DEB228F-9A24-4144-85FF-8E6948A8BA71}"/>
   </bookViews>
   <sheets>
     <sheet name="Központi Iroda" sheetId="1" r:id="rId1"/>
     <sheet name="Áruház" sheetId="3" r:id="rId2"/>
     <sheet name="Raktár" sheetId="2" r:id="rId3"/>
+    <sheet name="Köztes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="265">
   <si>
     <t>Központi Iroda</t>
   </si>
@@ -536,12 +537,6 @@
     <t>Pozsony_S1</t>
   </si>
   <si>
-    <t>G0/2</t>
-  </si>
-  <si>
-    <t>G0/6</t>
-  </si>
-  <si>
     <t>Pozsony_S2</t>
   </si>
   <si>
@@ -720,13 +715,127 @@
   </si>
   <si>
     <t>192.168.0.77</t>
+  </si>
+  <si>
+    <t>192.168.5.67</t>
+  </si>
+  <si>
+    <t>192.168.5.68</t>
+  </si>
+  <si>
+    <t>192.168.5.69</t>
+  </si>
+  <si>
+    <t>192.168.5.70</t>
+  </si>
+  <si>
+    <t>192.168.5.71</t>
+  </si>
+  <si>
+    <t>192.168.5.72</t>
+  </si>
+  <si>
+    <t>192.168.5.73</t>
+  </si>
+  <si>
+    <t>192.168.5.74</t>
+  </si>
+  <si>
+    <t>192.168.5.75</t>
+  </si>
+  <si>
+    <t>192.168.5.3</t>
+  </si>
+  <si>
+    <t>192.168.5.4</t>
+  </si>
+  <si>
+    <t>192.168.5.5</t>
+  </si>
+  <si>
+    <t>192.168.5.6</t>
+  </si>
+  <si>
+    <t>192.168.5.7</t>
+  </si>
+  <si>
+    <t>192.168.5.8</t>
+  </si>
+  <si>
+    <t>192.168.5.9</t>
+  </si>
+  <si>
+    <t>192.168.5.10</t>
+  </si>
+  <si>
+    <t>192.168.5.11</t>
+  </si>
+  <si>
+    <t>192.168.5.12</t>
+  </si>
+  <si>
+    <t>192.168.5.13</t>
+  </si>
+  <si>
+    <t>Port0 (nem aktív)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Köztes</t>
+  </si>
+  <si>
+    <t>Gyor_R0</t>
+  </si>
+  <si>
+    <t>130.10.10.0</t>
+  </si>
+  <si>
+    <t>/30</t>
+  </si>
+  <si>
+    <t>255.255.255.252</t>
+  </si>
+  <si>
+    <t>130.10.10.1 - 130.10.10.2</t>
+  </si>
+  <si>
+    <t>130.10.10.3</t>
+  </si>
+  <si>
+    <t>130.10.10.4</t>
+  </si>
+  <si>
+    <t>130.10.10.5 - 130.10.10.6</t>
+  </si>
+  <si>
+    <t>130.10.10.7</t>
+  </si>
+  <si>
+    <t>130.10.10.8</t>
+  </si>
+  <si>
+    <t>130.10.10.9 - 130.10.10.10</t>
+  </si>
+  <si>
+    <t>130.10.10.11</t>
+  </si>
+  <si>
+    <t>130.10.10.5</t>
+  </si>
+  <si>
+    <t>255.255.255.255.252</t>
+  </si>
+  <si>
+    <t>130.10.10.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -828,8 +937,46 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -868,12 +1015,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF7C80"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -903,7 +1044,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="62">
     <border>
       <left/>
       <right/>
@@ -1506,21 +1647,180 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -1533,7 +1833,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1635,99 +1935,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1735,24 +1977,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1767,39 +1991,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1807,185 +1998,488 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1995,8 +2489,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9933"/>
+      <color rgb="FFFF6600"/>
+      <color rgb="FFFF9966"/>
+      <color rgb="FFFF5050"/>
       <color rgb="FFFFFFFF"/>
-      <color rgb="FFFF9933"/>
       <color rgb="FF00FF00"/>
       <color rgb="FF33CCFF"/>
       <color rgb="FFFF7C80"/>
@@ -2337,19 +2834,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
     </row>
     <row r="2" spans="1:18" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="44" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2363,30 +2860,30 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="95"/>
-      <c r="B3" s="97"/>
-      <c r="C3" s="98" t="s">
+      <c r="A3" s="61"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="99"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="87"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:18" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="100"/>
-      <c r="B5" s="88"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="90"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="54"/>
       <c r="E5" s="3"/>
       <c r="J5" s="24" t="s">
         <v>36</v>
@@ -2417,8 +2914,8 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="100"/>
-      <c r="B6" s="87"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="3"/>
@@ -2451,10 +2948,10 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="100"/>
-      <c r="B7" s="88"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="90"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="54"/>
       <c r="E7" s="3"/>
       <c r="J7" s="25" t="s">
         <v>55</v>
@@ -2485,10 +2982,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="86"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="90"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="54"/>
       <c r="E8" s="3"/>
       <c r="J8" s="25" t="s">
         <v>56</v>
@@ -2519,10 +3016,10 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="85" t="s">
+      <c r="A9" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="87"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -2555,74 +3052,74 @@
       </c>
     </row>
     <row r="10" spans="1:18" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="86"/>
-      <c r="B10" s="88"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:18" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="85" t="s">
+      <c r="A11" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="87"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:18" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="86"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="90"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="54"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:18" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="87"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:18" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="86"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="90"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="54"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:18" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="85" t="s">
+      <c r="A15" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="87"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:18" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="86"/>
-      <c r="B16" s="88"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="90"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="54"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="85" t="s">
+      <c r="A17" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="87"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="86"/>
-      <c r="B18" s="91"/>
-      <c r="C18" s="92"/>
-      <c r="D18" s="93"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="59"/>
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2816,14 +3313,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
@@ -2840,6 +3329,14 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2850,17 +3347,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B769BC50-9623-4726-8971-E5FD68E08F76}">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" style="23" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" customWidth="1"/>
@@ -2875,47 +3372,47 @@
     <col min="19" max="19" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="109" t="s">
+    <row r="1" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="74" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-    </row>
-    <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+    </row>
+    <row r="2" spans="1:19" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="148" t="s">
+      <c r="G2" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="149"/>
-      <c r="I2" s="148" t="s">
+      <c r="H2" s="78"/>
+      <c r="I2" s="77" t="s">
         <v>161</v>
       </c>
-      <c r="J2" s="149"/>
+      <c r="J2" s="78"/>
       <c r="L2" s="20" t="s">
         <v>36</v>
       </c>
@@ -2942,20 +3439,24 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="150" t="s">
+      <c r="A3" s="79" t="s">
         <v>162</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="44" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="80" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="153"/>
-      <c r="J3" s="154"/>
+      <c r="D3" s="81" t="s">
+        <v>262</v>
+      </c>
+      <c r="E3" s="81" t="s">
+        <v>253</v>
+      </c>
+      <c r="F3" s="80"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="84"/>
       <c r="L3" s="21" t="s">
         <v>110</v>
       </c>
@@ -2982,18 +3483,22 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="151"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="44" t="s">
+      <c r="A4" s="85"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86" t="s">
         <v>142</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="153"/>
-      <c r="H4" s="154"/>
-      <c r="I4" s="153"/>
-      <c r="J4" s="154"/>
+      <c r="D4" s="86" t="s">
+        <v>264</v>
+      </c>
+      <c r="E4" s="86" t="s">
+        <v>263</v>
+      </c>
+      <c r="F4" s="86"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="89"/>
       <c r="L4" s="21" t="s">
         <v>111</v>
       </c>
@@ -3019,25 +3524,23 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="152"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44" t="s">
+    <row r="5" spans="1:19" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="90"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="45" t="s">
-        <v>185</v>
-      </c>
-      <c r="E5" s="45" t="s">
+      <c r="D5" s="92" t="s">
+        <v>183</v>
+      </c>
+      <c r="E5" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="82" t="s">
-        <v>185</v>
-      </c>
-      <c r="G5" s="153"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="154"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="95"/>
       <c r="L5" s="21" t="s">
         <v>115</v>
       </c>
@@ -3064,26 +3567,26 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="155" t="s">
+      <c r="A6" s="96" t="s">
         <v>165</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="47" t="s">
+      <c r="B6" s="97"/>
+      <c r="C6" s="97" t="s">
         <v>143</v>
       </c>
-      <c r="D6" s="48" t="s">
-        <v>192</v>
-      </c>
-      <c r="E6" s="46" t="s">
+      <c r="D6" s="98" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="46" t="s">
-        <v>185</v>
-      </c>
-      <c r="G6" s="141"/>
-      <c r="H6" s="142"/>
-      <c r="I6" s="141"/>
-      <c r="J6" s="142"/>
+      <c r="F6" s="97" t="s">
+        <v>183</v>
+      </c>
+      <c r="G6" s="99"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="101"/>
       <c r="L6" s="21" t="s">
         <v>119</v>
       </c>
@@ -3109,25 +3612,25 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="156"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="47" t="s">
+    <row r="7" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="102"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103" t="s">
         <v>147</v>
       </c>
-      <c r="D7" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="E7" s="46" t="s">
+      <c r="D7" s="103" t="s">
+        <v>191</v>
+      </c>
+      <c r="E7" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="46" t="s">
-        <v>185</v>
-      </c>
-      <c r="G7" s="141"/>
-      <c r="H7" s="142"/>
-      <c r="I7" s="141"/>
-      <c r="J7" s="142"/>
+      <c r="F7" s="103" t="s">
+        <v>183</v>
+      </c>
+      <c r="G7" s="104"/>
+      <c r="H7" s="105"/>
+      <c r="I7" s="104"/>
+      <c r="J7" s="106"/>
       <c r="L7" s="21" t="s">
         <v>108</v>
       </c>
@@ -3154,26 +3657,26 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="143" t="s">
+      <c r="A8" s="107" t="s">
         <v>164</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="50" t="s">
+      <c r="B8" s="108"/>
+      <c r="C8" s="108" t="s">
         <v>143</v>
       </c>
-      <c r="D8" s="49" t="s">
-        <v>188</v>
-      </c>
-      <c r="E8" s="49" t="s">
+      <c r="D8" s="108" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="49" t="s">
-        <v>185</v>
-      </c>
-      <c r="G8" s="146"/>
-      <c r="H8" s="147"/>
-      <c r="I8" s="146"/>
-      <c r="J8" s="147"/>
+      <c r="F8" s="108" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="109"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="111"/>
       <c r="L8" s="21" t="s">
         <v>106</v>
       </c>
@@ -3199,548 +3702,758 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="144"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="50" t="s">
+    <row r="9" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="112"/>
+      <c r="B9" s="113"/>
+      <c r="C9" s="113" t="s">
         <v>147</v>
       </c>
-      <c r="D9" s="49" t="s">
-        <v>195</v>
-      </c>
-      <c r="E9" s="49" t="s">
+      <c r="D9" s="113" t="s">
+        <v>193</v>
+      </c>
+      <c r="E9" s="113" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="113" t="s">
+        <v>183</v>
+      </c>
+      <c r="G9" s="114"/>
+      <c r="H9" s="115"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="116"/>
+    </row>
+    <row r="10" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="117"/>
+      <c r="B10" s="118"/>
+      <c r="C10" s="118" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="118" t="s">
+        <v>188</v>
+      </c>
+      <c r="E10" s="118" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="118" t="s">
+        <v>183</v>
+      </c>
+      <c r="G10" s="119"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="119"/>
+      <c r="J10" s="121"/>
+    </row>
+    <row r="11" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="122" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="123"/>
+      <c r="C11" s="123" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" s="123" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="123" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="123" t="s">
+        <v>183</v>
+      </c>
+      <c r="G11" s="124"/>
+      <c r="H11" s="125"/>
+      <c r="I11" s="124"/>
+      <c r="J11" s="126"/>
+    </row>
+    <row r="12" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="127"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="128" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="128" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" s="128" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="128" t="s">
+        <v>183</v>
+      </c>
+      <c r="G12" s="129"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="129"/>
+      <c r="J12" s="131"/>
+    </row>
+    <row r="13" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="132"/>
+      <c r="B13" s="133"/>
+      <c r="C13" s="133" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="133" t="s">
         <v>185</v>
       </c>
-      <c r="G9" s="146"/>
-      <c r="H9" s="147"/>
-      <c r="I9" s="146"/>
-      <c r="J9" s="147"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="145"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="50" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10" s="50" t="s">
-        <v>190</v>
-      </c>
-      <c r="E10" s="50" t="s">
+      <c r="E13" s="133" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="49" t="s">
-        <v>185</v>
-      </c>
-      <c r="G10" s="146"/>
-      <c r="H10" s="147"/>
-      <c r="I10" s="146"/>
-      <c r="J10" s="147"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="157" t="s">
-        <v>163</v>
-      </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="D11" s="52" t="s">
-        <v>186</v>
-      </c>
-      <c r="E11" s="52" t="s">
+      <c r="F13" s="133" t="s">
+        <v>183</v>
+      </c>
+      <c r="G13" s="134"/>
+      <c r="H13" s="135"/>
+      <c r="I13" s="134"/>
+      <c r="J13" s="136"/>
+    </row>
+    <row r="14" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="137" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" s="138"/>
+      <c r="C14" s="138" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="138" t="s">
+        <v>192</v>
+      </c>
+      <c r="E14" s="138" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="138" t="s">
+        <v>183</v>
+      </c>
+      <c r="G14" s="139"/>
+      <c r="H14" s="139"/>
+      <c r="I14" s="139"/>
+      <c r="J14" s="139"/>
+    </row>
+    <row r="15" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="140"/>
+      <c r="B15" s="141"/>
+      <c r="C15" s="141" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="141" t="s">
+        <v>227</v>
+      </c>
+      <c r="E15" s="141" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="141" t="s">
+        <v>183</v>
+      </c>
+      <c r="G15" s="142"/>
+      <c r="H15" s="142"/>
+      <c r="I15" s="142"/>
+      <c r="J15" s="142"/>
+    </row>
+    <row r="16" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="140"/>
+      <c r="B16" s="141"/>
+      <c r="C16" s="141" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="141" t="s">
+        <v>228</v>
+      </c>
+      <c r="E16" s="141" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="143" t="s">
+        <v>183</v>
+      </c>
+      <c r="G16" s="142"/>
+      <c r="H16" s="142"/>
+      <c r="I16" s="142"/>
+      <c r="J16" s="142"/>
+    </row>
+    <row r="17" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="140"/>
+      <c r="B17" s="141"/>
+      <c r="C17" s="141" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="141" t="s">
+        <v>229</v>
+      </c>
+      <c r="E17" s="141" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="143" t="s">
+        <v>183</v>
+      </c>
+      <c r="G17" s="142"/>
+      <c r="H17" s="142"/>
+      <c r="I17" s="142"/>
+      <c r="J17" s="142"/>
+    </row>
+    <row r="18" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="140"/>
+      <c r="B18" s="141"/>
+      <c r="C18" s="141" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" s="141" t="s">
+        <v>230</v>
+      </c>
+      <c r="E18" s="141" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="143" t="s">
+        <v>183</v>
+      </c>
+      <c r="G18" s="142"/>
+      <c r="H18" s="142"/>
+      <c r="I18" s="142"/>
+      <c r="J18" s="142"/>
+    </row>
+    <row r="19" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="140"/>
+      <c r="B19" s="141"/>
+      <c r="C19" s="141" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" s="141" t="s">
+        <v>231</v>
+      </c>
+      <c r="E19" s="141" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="143" t="s">
+        <v>183</v>
+      </c>
+      <c r="G19" s="142"/>
+      <c r="H19" s="142"/>
+      <c r="I19" s="142"/>
+      <c r="J19" s="142"/>
+    </row>
+    <row r="20" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="140"/>
+      <c r="B20" s="141"/>
+      <c r="C20" s="141" t="s">
+        <v>154</v>
+      </c>
+      <c r="D20" s="141" t="s">
+        <v>232</v>
+      </c>
+      <c r="E20" s="141" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="143" t="s">
+        <v>183</v>
+      </c>
+      <c r="G20" s="142"/>
+      <c r="H20" s="142"/>
+      <c r="I20" s="142"/>
+      <c r="J20" s="142"/>
+    </row>
+    <row r="21" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="144"/>
+      <c r="B21" s="145"/>
+      <c r="C21" s="146" t="s">
+        <v>155</v>
+      </c>
+      <c r="D21" s="146" t="s">
+        <v>233</v>
+      </c>
+      <c r="E21" s="146" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="145" t="s">
+        <v>183</v>
+      </c>
+      <c r="G21" s="147"/>
+      <c r="H21" s="147"/>
+      <c r="I21" s="147"/>
+      <c r="J21" s="147"/>
+    </row>
+    <row r="22" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="148" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" s="149"/>
+      <c r="C22" s="150" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="149" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="149" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="149" t="s">
+        <v>183</v>
+      </c>
+      <c r="G22" s="151"/>
+      <c r="H22" s="152"/>
+      <c r="I22" s="151"/>
+      <c r="J22" s="153"/>
+    </row>
+    <row r="23" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="154"/>
+      <c r="B23" s="155"/>
+      <c r="C23" s="156" t="s">
+        <v>149</v>
+      </c>
+      <c r="D23" s="155" t="s">
+        <v>236</v>
+      </c>
+      <c r="E23" s="155" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="155" t="s">
+        <v>183</v>
+      </c>
+      <c r="G23" s="157"/>
+      <c r="H23" s="158"/>
+      <c r="I23" s="157"/>
+      <c r="J23" s="159"/>
+    </row>
+    <row r="24" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="154"/>
+      <c r="B24" s="155"/>
+      <c r="C24" s="156" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" s="155" t="s">
+        <v>237</v>
+      </c>
+      <c r="E24" s="155" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="155" t="s">
+        <v>183</v>
+      </c>
+      <c r="G24" s="157"/>
+      <c r="H24" s="158"/>
+      <c r="I24" s="157"/>
+      <c r="J24" s="159"/>
+    </row>
+    <row r="25" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="154"/>
+      <c r="B25" s="155"/>
+      <c r="C25" s="156" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="155" t="s">
+        <v>238</v>
+      </c>
+      <c r="E25" s="155" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="155" t="s">
+        <v>183</v>
+      </c>
+      <c r="G25" s="157"/>
+      <c r="H25" s="158"/>
+      <c r="I25" s="157"/>
+      <c r="J25" s="159"/>
+    </row>
+    <row r="26" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="154"/>
+      <c r="B26" s="155"/>
+      <c r="C26" s="156" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="155" t="s">
+        <v>239</v>
+      </c>
+      <c r="E26" s="155" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="155" t="s">
+        <v>183</v>
+      </c>
+      <c r="G26" s="157"/>
+      <c r="H26" s="158"/>
+      <c r="I26" s="157"/>
+      <c r="J26" s="159"/>
+    </row>
+    <row r="27" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="154"/>
+      <c r="B27" s="155"/>
+      <c r="C27" s="156" t="s">
+        <v>153</v>
+      </c>
+      <c r="D27" s="155" t="s">
+        <v>240</v>
+      </c>
+      <c r="E27" s="155" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="155" t="s">
+        <v>183</v>
+      </c>
+      <c r="G27" s="157"/>
+      <c r="H27" s="158"/>
+      <c r="I27" s="157"/>
+      <c r="J27" s="159"/>
+    </row>
+    <row r="28" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="160"/>
+      <c r="B28" s="161"/>
+      <c r="C28" s="162" t="s">
+        <v>154</v>
+      </c>
+      <c r="D28" s="161" t="s">
+        <v>241</v>
+      </c>
+      <c r="E28" s="161" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="161" t="s">
+        <v>183</v>
+      </c>
+      <c r="G28" s="163"/>
+      <c r="H28" s="164"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="165"/>
+    </row>
+    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="166" t="s">
+        <v>170</v>
+      </c>
+      <c r="B29" s="167"/>
+      <c r="C29" s="167" t="s">
+        <v>247</v>
+      </c>
+      <c r="D29" s="167" t="s">
+        <v>248</v>
+      </c>
+      <c r="E29" s="167" t="s">
+        <v>248</v>
+      </c>
+      <c r="F29" s="167" t="s">
+        <v>248</v>
+      </c>
+      <c r="G29" s="168"/>
+      <c r="H29" s="169"/>
+      <c r="I29" s="168"/>
+      <c r="J29" s="170"/>
+    </row>
+    <row r="30" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="171"/>
+      <c r="B30" s="172"/>
+      <c r="C30" s="173" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30" s="172" t="s">
+        <v>242</v>
+      </c>
+      <c r="E30" s="172" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="172" t="s">
+        <v>183</v>
+      </c>
+      <c r="G30" s="174"/>
+      <c r="H30" s="175"/>
+      <c r="I30" s="174"/>
+      <c r="J30" s="176"/>
+    </row>
+    <row r="31" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="177" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" s="178"/>
+      <c r="C31" s="179" t="s">
+        <v>157</v>
+      </c>
+      <c r="D31" s="178" t="s">
+        <v>189</v>
+      </c>
+      <c r="E31" s="178" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="52" t="s">
-        <v>185</v>
-      </c>
-      <c r="G11" s="137"/>
-      <c r="H11" s="138"/>
-      <c r="I11" s="137"/>
-      <c r="J11" s="138"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="158"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="53" t="s">
-        <v>145</v>
-      </c>
-      <c r="D12" s="52" t="s">
-        <v>189</v>
-      </c>
-      <c r="E12" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="52" t="s">
-        <v>185</v>
-      </c>
-      <c r="G12" s="137"/>
-      <c r="H12" s="138"/>
-      <c r="I12" s="137"/>
-      <c r="J12" s="138"/>
-    </row>
-    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="159"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="54" t="s">
-        <v>146</v>
-      </c>
-      <c r="D13" s="54" t="s">
-        <v>187</v>
-      </c>
-      <c r="E13" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="51" t="s">
-        <v>185</v>
-      </c>
-      <c r="G13" s="139"/>
-      <c r="H13" s="140"/>
-      <c r="I13" s="139"/>
-      <c r="J13" s="140"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="111" t="s">
-        <v>166</v>
-      </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="56" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" s="55" t="s">
-        <v>194</v>
-      </c>
-      <c r="E14" s="55" t="s">
+      <c r="F31" s="178" t="s">
+        <v>183</v>
+      </c>
+      <c r="G31" s="180"/>
+      <c r="H31" s="181"/>
+      <c r="I31" s="180"/>
+      <c r="J31" s="182"/>
+    </row>
+    <row r="32" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="183" t="s">
+        <v>171</v>
+      </c>
+      <c r="B32" s="184" t="s">
+        <v>177</v>
+      </c>
+      <c r="C32" s="185" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" s="186" t="s">
+        <v>233</v>
+      </c>
+      <c r="E32" s="186" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="55" t="s">
-        <v>185</v>
-      </c>
-      <c r="G14" s="134"/>
-      <c r="H14" s="135"/>
-      <c r="I14" s="134"/>
-      <c r="J14" s="136"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="112"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="58" t="s">
-        <v>167</v>
-      </c>
-      <c r="D15" s="57" t="s">
-        <v>196</v>
-      </c>
-      <c r="E15" s="57" t="s">
+      <c r="F32" s="186" t="s">
+        <v>183</v>
+      </c>
+      <c r="G32" s="187"/>
+      <c r="H32" s="188"/>
+      <c r="I32" s="187"/>
+      <c r="J32" s="189"/>
+    </row>
+    <row r="33" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="190" t="s">
+        <v>172</v>
+      </c>
+      <c r="B33" s="191" t="s">
+        <v>177</v>
+      </c>
+      <c r="C33" s="192" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33" s="193" t="s">
+        <v>234</v>
+      </c>
+      <c r="E33" s="193" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="57" t="s">
-        <v>185</v>
-      </c>
-      <c r="G15" s="126"/>
-      <c r="H15" s="127"/>
-      <c r="I15" s="126"/>
-      <c r="J15" s="128"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="112"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="58" t="s">
-        <v>149</v>
-      </c>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="126"/>
-      <c r="H16" s="127"/>
-      <c r="I16" s="126"/>
-      <c r="J16" s="128"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="112"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="58" t="s">
-        <v>150</v>
-      </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="126"/>
-      <c r="H17" s="127"/>
-      <c r="I17" s="126"/>
-      <c r="J17" s="128"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="112"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="126"/>
-      <c r="H18" s="127"/>
-      <c r="I18" s="126"/>
-      <c r="J18" s="128"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="112"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="126"/>
-      <c r="H19" s="127"/>
-      <c r="I19" s="126"/>
-      <c r="J19" s="128"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="112"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="58" t="s">
-        <v>153</v>
-      </c>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="126"/>
-      <c r="H20" s="127"/>
-      <c r="I20" s="126"/>
-      <c r="J20" s="128"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="112"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="126"/>
-      <c r="H21" s="127"/>
-      <c r="I21" s="126"/>
-      <c r="J21" s="128"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="113"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="63" t="s">
-        <v>155</v>
-      </c>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="129"/>
-      <c r="H22" s="130"/>
-      <c r="I22" s="129"/>
-      <c r="J22" s="131"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="101" t="s">
-        <v>169</v>
-      </c>
-      <c r="B23" s="65"/>
-      <c r="C23" s="66" t="s">
-        <v>149</v>
-      </c>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="132"/>
-      <c r="H23" s="133"/>
-      <c r="I23" s="132"/>
-      <c r="J23" s="133"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="102"/>
-      <c r="B24" s="68"/>
-      <c r="C24" s="69" t="s">
-        <v>150</v>
-      </c>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="124"/>
-      <c r="H24" s="125"/>
-      <c r="I24" s="124"/>
-      <c r="J24" s="125"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="102"/>
-      <c r="B25" s="68"/>
-      <c r="C25" s="69" t="s">
-        <v>151</v>
-      </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="124"/>
-      <c r="H25" s="125"/>
-      <c r="I25" s="124"/>
-      <c r="J25" s="125"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="102"/>
-      <c r="B26" s="68"/>
-      <c r="C26" s="69" t="s">
-        <v>152</v>
-      </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="124"/>
-      <c r="H26" s="125"/>
-      <c r="I26" s="124"/>
-      <c r="J26" s="125"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="102"/>
-      <c r="B27" s="68"/>
-      <c r="C27" s="69" t="s">
-        <v>153</v>
-      </c>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="124"/>
-      <c r="H27" s="125"/>
-      <c r="I27" s="124"/>
-      <c r="J27" s="125"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="103"/>
-      <c r="B28" s="68"/>
-      <c r="C28" s="69" t="s">
-        <v>154</v>
-      </c>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="124"/>
-      <c r="H28" s="125"/>
-      <c r="I28" s="124"/>
-      <c r="J28" s="125"/>
-    </row>
-    <row r="29" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="105" t="s">
-        <v>172</v>
-      </c>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71" t="s">
-        <v>156</v>
-      </c>
-      <c r="D29" s="71"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="114"/>
-      <c r="H29" s="115"/>
-      <c r="I29" s="114"/>
-      <c r="J29" s="115"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="106"/>
-      <c r="B30" s="71"/>
-      <c r="C30" s="72" t="s">
-        <v>170</v>
-      </c>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="114"/>
-      <c r="H30" s="115"/>
-      <c r="I30" s="114"/>
-      <c r="J30" s="115"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="73" t="s">
-        <v>171</v>
-      </c>
-      <c r="B31" s="73"/>
-      <c r="C31" s="74" t="s">
+      <c r="F33" s="186" t="s">
+        <v>183</v>
+      </c>
+      <c r="G33" s="194"/>
+      <c r="H33" s="195"/>
+      <c r="I33" s="194"/>
+      <c r="J33" s="196"/>
+    </row>
+    <row r="34" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="197" t="s">
+        <v>173</v>
+      </c>
+      <c r="B34" s="191" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="198" t="s">
         <v>157</v>
       </c>
-      <c r="D31" s="73" t="s">
-        <v>191</v>
-      </c>
-      <c r="E31" s="73" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="G31" s="116"/>
-      <c r="H31" s="117"/>
-      <c r="I31" s="116"/>
-      <c r="J31" s="117"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="79" t="s">
-        <v>173</v>
-      </c>
-      <c r="B32" s="80" t="s">
+      <c r="D34" s="199" t="s">
+        <v>235</v>
+      </c>
+      <c r="E34" s="199" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="186" t="s">
+        <v>183</v>
+      </c>
+      <c r="G34" s="200"/>
+      <c r="H34" s="201"/>
+      <c r="I34" s="200"/>
+      <c r="J34" s="202"/>
+    </row>
+    <row r="35" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="203" t="s">
+        <v>174</v>
+      </c>
+      <c r="B35" s="204" t="s">
+        <v>178</v>
+      </c>
+      <c r="C35" s="205" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="204" t="s">
+        <v>242</v>
+      </c>
+      <c r="E35" s="204" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" s="204" t="s">
+        <v>183</v>
+      </c>
+      <c r="G35" s="206"/>
+      <c r="H35" s="206"/>
+      <c r="I35" s="206"/>
+      <c r="J35" s="207"/>
+    </row>
+    <row r="36" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="208" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" s="209" t="s">
+        <v>178</v>
+      </c>
+      <c r="C36" s="210" t="s">
+        <v>157</v>
+      </c>
+      <c r="D36" s="204" t="s">
+        <v>243</v>
+      </c>
+      <c r="E36" s="204" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" s="204" t="s">
+        <v>183</v>
+      </c>
+      <c r="G36" s="211"/>
+      <c r="H36" s="211"/>
+      <c r="I36" s="211"/>
+      <c r="J36" s="212"/>
+    </row>
+    <row r="37" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="213" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37" s="214" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" s="215" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" s="216" t="s">
+        <v>244</v>
+      </c>
+      <c r="E37" s="216" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" s="216" t="s">
+        <v>183</v>
+      </c>
+      <c r="G37" s="217"/>
+      <c r="H37" s="217"/>
+      <c r="I37" s="217"/>
+      <c r="J37" s="218"/>
+    </row>
+    <row r="38" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="155" t="s">
+        <v>181</v>
+      </c>
+      <c r="B38" s="155" t="s">
         <v>179</v>
       </c>
-      <c r="C32" s="81" t="s">
-        <v>157</v>
-      </c>
-      <c r="D32" s="79"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="79"/>
-      <c r="G32" s="122"/>
-      <c r="H32" s="123"/>
-      <c r="I32" s="122"/>
-      <c r="J32" s="123"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="79" t="s">
-        <v>174</v>
-      </c>
-      <c r="B33" s="80" t="s">
+      <c r="C38" s="155"/>
+      <c r="D38" s="155" t="s">
+        <v>245</v>
+      </c>
+      <c r="E38" s="155" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" s="155" t="s">
+        <v>183</v>
+      </c>
+      <c r="G38" s="219"/>
+      <c r="H38" s="219"/>
+      <c r="I38" s="219"/>
+      <c r="J38" s="219"/>
+    </row>
+    <row r="39" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="155" t="s">
+        <v>180</v>
+      </c>
+      <c r="B39" s="155" t="s">
         <v>179</v>
       </c>
-      <c r="C33" s="81" t="s">
-        <v>157</v>
-      </c>
-      <c r="D33" s="79"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="122"/>
-      <c r="H33" s="123"/>
-      <c r="I33" s="122"/>
-      <c r="J33" s="123"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="79" t="s">
-        <v>175</v>
-      </c>
-      <c r="B34" s="80" t="s">
-        <v>179</v>
-      </c>
-      <c r="C34" s="81" t="s">
-        <v>157</v>
-      </c>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="122"/>
-      <c r="H34" s="123"/>
-      <c r="I34" s="122"/>
-      <c r="J34" s="123"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="B35" s="76" t="s">
-        <v>180</v>
-      </c>
-      <c r="C35" s="77" t="s">
-        <v>157</v>
-      </c>
-      <c r="D35" s="75"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="118"/>
-      <c r="H35" s="119"/>
-      <c r="I35" s="118"/>
-      <c r="J35" s="119"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="75" t="s">
-        <v>177</v>
-      </c>
-      <c r="B36" s="76" t="s">
-        <v>180</v>
-      </c>
-      <c r="C36" s="77" t="s">
-        <v>157</v>
-      </c>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
-      <c r="F36" s="75"/>
-      <c r="G36" s="118"/>
-      <c r="H36" s="119"/>
-      <c r="I36" s="118"/>
-      <c r="J36" s="119"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="75" t="s">
-        <v>178</v>
-      </c>
-      <c r="B37" s="76" t="s">
-        <v>180</v>
-      </c>
-      <c r="C37" s="77" t="s">
-        <v>157</v>
-      </c>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="118"/>
-      <c r="H37" s="119"/>
-      <c r="I37" s="118"/>
-      <c r="J37" s="119"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="78" t="s">
+      <c r="C39" s="155"/>
+      <c r="D39" s="155" t="s">
+        <v>246</v>
+      </c>
+      <c r="E39" s="155" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" s="155" t="s">
         <v>183</v>
       </c>
-      <c r="B38" s="78" t="s">
-        <v>181</v>
-      </c>
-      <c r="C38" s="78"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="78"/>
-      <c r="F38" s="78"/>
-      <c r="G38" s="120"/>
-      <c r="H38" s="121"/>
-      <c r="I38" s="120"/>
-      <c r="J38" s="121"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="78" t="s">
+      <c r="G39" s="219"/>
+      <c r="H39" s="219"/>
+      <c r="I39" s="219"/>
+      <c r="J39" s="219"/>
+    </row>
+    <row r="40" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="220"/>
+      <c r="B40" s="221" t="s">
         <v>182</v>
       </c>
-      <c r="B39" s="78" t="s">
-        <v>181</v>
-      </c>
-      <c r="C39" s="78"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="78"/>
-      <c r="G39" s="120"/>
-      <c r="H39" s="121"/>
-      <c r="I39" s="120"/>
-      <c r="J39" s="121"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="107"/>
-      <c r="H40" s="108"/>
-      <c r="I40" s="107"/>
-      <c r="J40" s="108"/>
+      <c r="C40" s="221"/>
+      <c r="D40" s="221"/>
+      <c r="E40" s="221"/>
+      <c r="F40" s="221"/>
+      <c r="G40" s="222"/>
+      <c r="H40" s="223"/>
+      <c r="I40" s="222"/>
+      <c r="J40" s="224"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G41" s="104"/>
-      <c r="H41" s="104"/>
-      <c r="I41" s="104"/>
-      <c r="J41" s="104"/>
+      <c r="G41" s="72"/>
+      <c r="H41" s="72"/>
+      <c r="I41" s="72"/>
+      <c r="J41" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="88">
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
@@ -3757,79 +4470,8 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A14:A22"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
   </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3839,8 +4481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27F8DC3-BDE0-43F3-979D-2CCDC5541D2C}">
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F38"/>
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O21" sqref="N21:O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3864,14 +4506,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
@@ -3892,14 +4534,14 @@
       <c r="F2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="161" t="s">
+      <c r="G2" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="161"/>
-      <c r="I2" s="161" t="s">
+      <c r="H2" s="67"/>
+      <c r="I2" s="67" t="s">
         <v>161</v>
       </c>
-      <c r="J2" s="161"/>
+      <c r="J2" s="67"/>
       <c r="N2" t="s">
         <v>81</v>
       </c>
@@ -3912,7 +4554,7 @@
       <c r="U2" s="29"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="68" t="s">
         <v>125</v>
       </c>
       <c r="B3" s="34"/>
@@ -3922,37 +4564,37 @@
       <c r="D3" s="33"/>
       <c r="E3" s="33"/>
       <c r="F3" s="34"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="108"/>
-      <c r="N3" s="168" t="s">
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63"/>
+      <c r="N3" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="168" t="s">
+      <c r="O3" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="P3" s="168" t="s">
+      <c r="P3" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="168" t="s">
+      <c r="Q3" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="168" t="s">
+      <c r="R3" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="S3" s="168" t="s">
+      <c r="S3" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="T3" s="168" t="s">
+      <c r="T3" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="U3" s="168" t="s">
+      <c r="U3" s="43" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="160"/>
+      <c r="A4" s="68"/>
       <c r="B4" s="34"/>
       <c r="C4" s="32" t="s">
         <v>142</v>
@@ -3960,10 +4602,10 @@
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
       <c r="F4" s="34"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="108"/>
-      <c r="I4" s="107"/>
-      <c r="J4" s="108"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="63"/>
       <c r="N4" s="30" t="s">
         <v>82</v>
       </c>
@@ -3990,22 +4632,22 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="160"/>
+      <c r="A5" s="68"/>
       <c r="B5" s="34"/>
       <c r="C5" s="32" t="s">
         <v>143</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="34"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="108"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="63"/>
       <c r="N5" s="30" t="s">
         <v>86</v>
       </c>
@@ -4032,7 +4674,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="160" t="s">
+      <c r="A6" s="68" t="s">
         <v>126</v>
       </c>
       <c r="B6" s="34"/>
@@ -4040,18 +4682,18 @@
         <v>143</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G6" s="107"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="107"/>
-      <c r="J6" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G6" s="62"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="63"/>
       <c r="N6" s="30" t="s">
         <v>90</v>
       </c>
@@ -4078,24 +4720,24 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="160"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="34"/>
       <c r="C7" s="32" t="s">
         <v>147</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G7" s="107"/>
-      <c r="H7" s="108"/>
-      <c r="I7" s="107"/>
-      <c r="J7" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G7" s="62"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="63"/>
       <c r="N7" s="30" t="s">
         <v>94</v>
       </c>
@@ -4122,7 +4764,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="160" t="s">
+      <c r="A8" s="68" t="s">
         <v>127</v>
       </c>
       <c r="B8" s="34"/>
@@ -4130,18 +4772,18 @@
         <v>143</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E8" s="31" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G8" s="107"/>
-      <c r="H8" s="108"/>
-      <c r="I8" s="107"/>
-      <c r="J8" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G8" s="62"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="63"/>
       <c r="N8" s="37" t="s">
         <v>98</v>
       </c>
@@ -4168,24 +4810,24 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="160"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="34"/>
       <c r="C9" s="32" t="s">
         <v>147</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E9" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G9" s="107"/>
-      <c r="H9" s="108"/>
-      <c r="I9" s="107"/>
-      <c r="J9" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G9" s="62"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="63"/>
       <c r="L9" s="39"/>
       <c r="M9" s="40"/>
       <c r="N9" s="41" t="s">
@@ -4214,27 +4856,27 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="160"/>
+      <c r="A10" s="68"/>
       <c r="B10" s="34"/>
       <c r="C10" s="32" t="s">
         <v>148</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E10" s="31" t="s">
         <v>48</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G10" s="107"/>
-      <c r="H10" s="108"/>
-      <c r="I10" s="107"/>
-      <c r="J10" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="63"/>
     </row>
     <row r="11" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="160" t="s">
+      <c r="A11" s="68" t="s">
         <v>128</v>
       </c>
       <c r="B11" s="34"/>
@@ -4242,61 +4884,61 @@
         <v>144</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G11" s="107"/>
-      <c r="H11" s="108"/>
-      <c r="I11" s="107"/>
-      <c r="J11" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="63"/>
     </row>
     <row r="12" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="160"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="34"/>
       <c r="C12" s="32" t="s">
         <v>145</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E12" s="31" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G12" s="107"/>
-      <c r="H12" s="108"/>
-      <c r="I12" s="107"/>
-      <c r="J12" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G12" s="62"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="63"/>
     </row>
     <row r="13" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="160"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="34"/>
       <c r="C13" s="32" t="s">
         <v>146</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G13" s="107"/>
-      <c r="H13" s="108"/>
-      <c r="I13" s="107"/>
-      <c r="J13" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G13" s="62"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="63"/>
     </row>
     <row r="14" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="165" t="s">
+      <c r="A14" s="69" t="s">
         <v>129</v>
       </c>
       <c r="B14" s="34"/>
@@ -4304,141 +4946,141 @@
         <v>147</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G14" s="107"/>
-      <c r="H14" s="108"/>
-      <c r="I14" s="107"/>
-      <c r="J14" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G14" s="62"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="63"/>
     </row>
     <row r="15" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="166"/>
+      <c r="A15" s="70"/>
       <c r="B15" s="34"/>
       <c r="C15" s="32" t="s">
         <v>149</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G15" s="107"/>
-      <c r="H15" s="108"/>
-      <c r="I15" s="107"/>
-      <c r="J15" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="63"/>
     </row>
     <row r="16" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="166"/>
+      <c r="A16" s="70"/>
       <c r="B16" s="34"/>
       <c r="C16" s="32" t="s">
         <v>150</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G16" s="107"/>
-      <c r="H16" s="108"/>
-      <c r="I16" s="107"/>
-      <c r="J16" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G16" s="62"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="63"/>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="166"/>
+      <c r="A17" s="70"/>
       <c r="B17" s="34"/>
       <c r="C17" s="32" t="s">
         <v>151</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E17" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G17" s="107"/>
-      <c r="H17" s="108"/>
-      <c r="I17" s="107"/>
-      <c r="J17" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G17" s="62"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="63"/>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="166"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="34"/>
       <c r="C18" s="32" t="s">
         <v>152</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E18" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G18" s="107"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="107"/>
-      <c r="J18" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G18" s="62"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="63"/>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="166"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="34"/>
       <c r="C19" s="32" t="s">
         <v>153</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E19" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G19" s="107"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="107"/>
-      <c r="J19" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G19" s="62"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="63"/>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="167"/>
+      <c r="A20" s="71"/>
       <c r="B20" s="34"/>
       <c r="C20" s="32" t="s">
         <v>154</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E20" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G20" s="107"/>
-      <c r="H20" s="108"/>
-      <c r="I20" s="107"/>
-      <c r="J20" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G20" s="62"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="63"/>
     </row>
     <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="162" t="s">
+      <c r="A21" s="64" t="s">
         <v>130</v>
       </c>
       <c r="B21" s="36"/>
@@ -4446,158 +5088,158 @@
         <v>147</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E21" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G21" s="107"/>
-      <c r="H21" s="108"/>
-      <c r="I21" s="107"/>
-      <c r="J21" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G21" s="62"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="63"/>
     </row>
     <row r="22" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="163"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="36"/>
       <c r="C22" s="32" t="s">
         <v>149</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E22" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F22" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G22" s="107"/>
-      <c r="H22" s="108"/>
-      <c r="I22" s="107"/>
-      <c r="J22" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G22" s="62"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="63"/>
     </row>
     <row r="23" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="163"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="36"/>
       <c r="C23" s="32" t="s">
         <v>150</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E23" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G23" s="107"/>
-      <c r="H23" s="108"/>
-      <c r="I23" s="107"/>
-      <c r="J23" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G23" s="62"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="63"/>
     </row>
     <row r="24" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="163"/>
+      <c r="A24" s="65"/>
       <c r="B24" s="36"/>
       <c r="C24" s="32" t="s">
         <v>151</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E24" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G24" s="107"/>
-      <c r="H24" s="108"/>
-      <c r="I24" s="107"/>
-      <c r="J24" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G24" s="62"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="63"/>
     </row>
     <row r="25" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="163"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="36"/>
       <c r="C25" s="32" t="s">
         <v>152</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E25" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G25" s="107"/>
-      <c r="H25" s="108"/>
-      <c r="I25" s="107"/>
-      <c r="J25" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G25" s="62"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="63"/>
     </row>
     <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="163"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="36"/>
       <c r="C26" s="32" t="s">
         <v>153</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E26" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F26" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G26" s="107"/>
-      <c r="H26" s="108"/>
-      <c r="I26" s="107"/>
-      <c r="J26" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G26" s="62"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="63"/>
     </row>
     <row r="27" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="163"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="36"/>
       <c r="C27" s="32" t="s">
         <v>154</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E27" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F27" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G27" s="107"/>
-      <c r="H27" s="108"/>
-      <c r="I27" s="107"/>
-      <c r="J27" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G27" s="62"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="63"/>
     </row>
     <row r="28" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="164"/>
+      <c r="A28" s="66"/>
       <c r="B28" s="36"/>
       <c r="C28" s="32" t="s">
         <v>155</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E28" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F28" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G28" s="107"/>
-      <c r="H28" s="108"/>
-      <c r="I28" s="107"/>
-      <c r="J28" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G28" s="62"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="63"/>
     </row>
     <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -4608,18 +5250,18 @@
         <v>156</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E29" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F29" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G29" s="107"/>
-      <c r="H29" s="108"/>
-      <c r="I29" s="107"/>
-      <c r="J29" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G29" s="62"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="63"/>
     </row>
     <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -4630,18 +5272,18 @@
         <v>157</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E30" s="31" t="s">
         <v>48</v>
       </c>
       <c r="F30" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G30" s="107"/>
-      <c r="H30" s="108"/>
-      <c r="I30" s="107"/>
-      <c r="J30" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G30" s="62"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="63"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -4654,18 +5296,18 @@
         <v>157</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E31" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F31" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G31" s="107"/>
-      <c r="H31" s="108"/>
-      <c r="I31" s="107"/>
-      <c r="J31" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G31" s="62"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="63"/>
     </row>
     <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -4678,18 +5320,18 @@
         <v>157</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E32" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F32" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G32" s="107"/>
-      <c r="H32" s="108"/>
-      <c r="I32" s="107"/>
-      <c r="J32" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G32" s="62"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="63"/>
     </row>
     <row r="33" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
@@ -4702,18 +5344,18 @@
         <v>157</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E33" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F33" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G33" s="107"/>
-      <c r="H33" s="108"/>
-      <c r="I33" s="107"/>
-      <c r="J33" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G33" s="62"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="63"/>
     </row>
     <row r="34" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
@@ -4726,18 +5368,18 @@
         <v>157</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E34" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F34" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G34" s="107"/>
-      <c r="H34" s="108"/>
-      <c r="I34" s="107"/>
-      <c r="J34" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G34" s="62"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="63"/>
     </row>
     <row r="35" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -4750,18 +5392,18 @@
         <v>157</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E35" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G35" s="107"/>
-      <c r="H35" s="108"/>
-      <c r="I35" s="107"/>
-      <c r="J35" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G35" s="62"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="63"/>
     </row>
     <row r="36" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -4774,18 +5416,18 @@
         <v>157</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E36" s="31" t="s">
         <v>45</v>
       </c>
       <c r="F36" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G36" s="107"/>
-      <c r="H36" s="108"/>
-      <c r="I36" s="107"/>
-      <c r="J36" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G36" s="62"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="63"/>
     </row>
     <row r="37" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
@@ -4796,12 +5438,12 @@
       <c r="D37" s="31"/>
       <c r="E37" s="31"/>
       <c r="F37" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G37" s="107"/>
-      <c r="H37" s="108"/>
-      <c r="I37" s="107"/>
-      <c r="J37" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G37" s="62"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="63"/>
     </row>
     <row r="38" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -4812,12 +5454,12 @@
       <c r="D38" s="31"/>
       <c r="E38" s="31"/>
       <c r="F38" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="G38" s="107"/>
-      <c r="H38" s="108"/>
-      <c r="I38" s="107"/>
-      <c r="J38" s="108"/>
+        <v>195</v>
+      </c>
+      <c r="G38" s="62"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="63"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
@@ -4828,74 +5470,19 @@
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="107"/>
-      <c r="H39" s="108"/>
-      <c r="I39" s="107"/>
-      <c r="J39" s="108"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="63"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="A21:A28"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="G3:H3"/>
@@ -4912,15 +5499,219 @@
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:J38"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4B727F-DBFB-44AA-A62D-48CC65DAE88F}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="73" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4" s="22">
+        <v>2</v>
+      </c>
+      <c r="C4" s="22">
+        <v>2</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="22">
+        <v>2</v>
+      </c>
+      <c r="C5" s="22">
+        <v>2</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="22">
+        <v>2</v>
+      </c>
+      <c r="C6" s="22">
+        <v>2</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
pck ip cím beállítása+conflict feloldása
</commit_message>
<xml_diff>
--- a/IP_cim_kiosztas.xlsx
+++ b/IP_cim_kiosztas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Vizsgaremek\Uzemelteto_vizsgaremek_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Üzemeltető\vizsgaremek\Uzemelteto_vizsgaremek_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12152C03-47B6-4E35-AF7F-A2396B1DC724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9699B9D0-20B5-402C-A07C-5C44FD991BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="3585" windowWidth="16860" windowHeight="15345" activeTab="1" xr2:uid="{5DEB228F-9A24-4144-85FF-8E6948A8BA71}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21975" windowHeight="14130" activeTab="2" xr2:uid="{5DEB228F-9A24-4144-85FF-8E6948A8BA71}"/>
   </bookViews>
   <sheets>
     <sheet name="Központi Iroda" sheetId="1" r:id="rId1"/>
@@ -405,9 +405,6 @@
     <t xml:space="preserve"> Sopron_S2</t>
   </si>
   <si>
-    <t>Sopron_Access Point</t>
-  </si>
-  <si>
     <t>Sopron_server1</t>
   </si>
   <si>
@@ -947,6 +944,9 @@
   </si>
   <si>
     <t>Felügyeleti_VLAN_19</t>
+  </si>
+  <si>
+    <t>Sopron_Wireless Router</t>
   </si>
 </sst>
 </file>
@@ -2226,6 +2226,9 @@
     <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2259,52 +2262,154 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2331,12 +2436,6 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2355,161 +2454,59 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2526,6 +2523,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2537,9 +2540,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2549,12 +2549,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FFFF9933"/>
       <color rgb="FFFF6600"/>
       <color rgb="FFFF9966"/>
       <color rgb="FFFF5050"/>
       <color rgb="FFFFFFFF"/>
-      <color rgb="FF00FF00"/>
       <color rgb="FF33CCFF"/>
       <color rgb="FFFF7C80"/>
       <color rgb="FFD60093"/>
@@ -2895,19 +2895,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
     </row>
     <row r="2" spans="1:19" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="123" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="77" t="s">
@@ -2921,35 +2921,35 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="121"/>
-      <c r="B3" s="123"/>
-      <c r="C3" s="124" t="s">
+      <c r="A3" s="122"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="125"/>
+      <c r="D3" s="126"/>
       <c r="E3" s="79" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="116" t="s">
-        <v>237</v>
+      <c r="A4" s="117" t="s">
+        <v>236</v>
       </c>
       <c r="B4" s="80" t="s">
+        <v>250</v>
+      </c>
+      <c r="E4" s="76"/>
+    </row>
+    <row r="5" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="117"/>
+      <c r="B5" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E4" s="76"/>
-    </row>
-    <row r="5" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="116"/>
-      <c r="B5" s="1" t="s">
-        <v>252</v>
-      </c>
       <c r="C5" s="81" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E5" s="26"/>
       <c r="J5" s="16"/>
@@ -2963,15 +2963,15 @@
       <c r="R5" s="20"/>
     </row>
     <row r="6" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116"/>
+      <c r="A6" s="117"/>
       <c r="B6" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D6" s="81" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E6" s="26"/>
       <c r="J6" s="17"/>
@@ -2985,7 +2985,7 @@
       <c r="R6" s="16"/>
     </row>
     <row r="7" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="115" t="s">
+      <c r="A7" s="116" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="24"/>
@@ -3003,7 +3003,7 @@
       <c r="R7" s="16"/>
     </row>
     <row r="8" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="117"/>
+      <c r="A8" s="118"/>
       <c r="B8" s="24"/>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
@@ -3019,14 +3019,14 @@
       <c r="R8" s="16"/>
     </row>
     <row r="9" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="115" t="s">
+      <c r="A9" s="116" t="s">
+        <v>253</v>
+      </c>
+      <c r="B9" s="82" t="s">
         <v>254</v>
       </c>
-      <c r="B9" s="82" t="s">
+      <c r="C9" s="83" t="s">
         <v>255</v>
-      </c>
-      <c r="C9" s="83" t="s">
-        <v>256</v>
       </c>
       <c r="D9" s="83" t="s">
         <v>49</v>
@@ -3043,12 +3043,12 @@
       <c r="R9" s="16"/>
     </row>
     <row r="10" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="116"/>
+      <c r="A10" s="117"/>
       <c r="B10" s="82" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" s="83" t="s">
         <v>257</v>
-      </c>
-      <c r="C10" s="83" t="s">
-        <v>258</v>
       </c>
       <c r="D10" s="83" t="s">
         <v>49</v>
@@ -3056,12 +3056,12 @@
       <c r="E10" s="26"/>
     </row>
     <row r="11" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="116"/>
+      <c r="A11" s="117"/>
       <c r="B11" s="82" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" s="83" t="s">
         <v>259</v>
-      </c>
-      <c r="C11" s="83" t="s">
-        <v>260</v>
       </c>
       <c r="D11" s="83" t="s">
         <v>44</v>
@@ -3069,12 +3069,12 @@
       <c r="E11" s="26"/>
     </row>
     <row r="12" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="116"/>
+      <c r="A12" s="117"/>
       <c r="B12" s="82" t="s">
+        <v>260</v>
+      </c>
+      <c r="C12" s="83" t="s">
         <v>261</v>
-      </c>
-      <c r="C12" s="83" t="s">
-        <v>262</v>
       </c>
       <c r="D12" s="83" t="s">
         <v>44</v>
@@ -3108,16 +3108,16 @@
         <v>72</v>
       </c>
       <c r="S12" s="89" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="116"/>
+      <c r="A13" s="117"/>
       <c r="B13" s="82" t="s">
+        <v>262</v>
+      </c>
+      <c r="C13" s="83" t="s">
         <v>263</v>
-      </c>
-      <c r="C13" s="83" t="s">
-        <v>264</v>
       </c>
       <c r="D13" s="83" t="s">
         <v>44</v>
@@ -3151,11 +3151,11 @@
         <v>68</v>
       </c>
       <c r="S13" s="88" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="116"/>
+      <c r="A14" s="117"/>
       <c r="B14" s="82"/>
       <c r="C14" s="83"/>
       <c r="D14" s="83"/>
@@ -3188,11 +3188,11 @@
         <v>69</v>
       </c>
       <c r="S14" s="88" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="116"/>
+      <c r="A15" s="117"/>
       <c r="B15" s="82"/>
       <c r="C15" s="83"/>
       <c r="D15" s="83"/>
@@ -3225,11 +3225,11 @@
         <v>70</v>
       </c>
       <c r="S15" s="88" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="116"/>
+      <c r="A16" s="117"/>
       <c r="B16" s="82"/>
       <c r="C16" s="83"/>
       <c r="D16" s="83"/>
@@ -3262,25 +3262,25 @@
         <v>71</v>
       </c>
       <c r="S16" s="88" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="115" t="s">
+      <c r="A17" s="116" t="s">
+        <v>264</v>
+      </c>
+      <c r="B17" s="82" t="s">
+        <v>254</v>
+      </c>
+      <c r="C17" s="83" t="s">
         <v>265</v>
-      </c>
-      <c r="B17" s="82" t="s">
-        <v>255</v>
-      </c>
-      <c r="C17" s="83" t="s">
-        <v>266</v>
       </c>
       <c r="D17" s="83" t="s">
         <v>49</v>
       </c>
       <c r="E17" s="26"/>
       <c r="J17" s="90" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K17" s="90">
         <v>3</v>
@@ -3289,7 +3289,7 @@
         <v>6</v>
       </c>
       <c r="M17" s="88" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="N17" s="90" t="s">
         <v>43</v>
@@ -3298,25 +3298,25 @@
         <v>54</v>
       </c>
       <c r="P17" s="88" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q17" s="88" t="s">
         <v>278</v>
       </c>
-      <c r="Q17" s="88" t="s">
+      <c r="R17" s="88" t="s">
         <v>279</v>
       </c>
-      <c r="R17" s="88" t="s">
+      <c r="S17" s="88" t="s">
         <v>280</v>
       </c>
-      <c r="S17" s="88" t="s">
-        <v>281</v>
-      </c>
     </row>
     <row r="18" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="116"/>
+      <c r="A18" s="117"/>
       <c r="B18" s="82" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C18" s="83" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D18" s="83" t="s">
         <v>49</v>
@@ -3324,12 +3324,12 @@
       <c r="E18" s="26"/>
     </row>
     <row r="19" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="116"/>
+      <c r="A19" s="117"/>
       <c r="B19" s="82" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C19" s="83" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D19" s="83" t="s">
         <v>44</v>
@@ -3337,12 +3337,12 @@
       <c r="E19" s="26"/>
     </row>
     <row r="20" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="116"/>
+      <c r="A20" s="117"/>
       <c r="B20" s="82" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C20" s="83" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D20" s="83" t="s">
         <v>44</v>
@@ -3350,12 +3350,12 @@
       <c r="E20" s="26"/>
     </row>
     <row r="21" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="116"/>
+      <c r="A21" s="117"/>
       <c r="B21" s="82" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C21" s="83" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D21" s="83" t="s">
         <v>44</v>
@@ -3363,28 +3363,28 @@
       <c r="E21" s="26"/>
     </row>
     <row r="22" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="116"/>
+      <c r="A22" s="117"/>
       <c r="B22" s="82"/>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
       <c r="E22" s="26"/>
     </row>
     <row r="23" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="116"/>
+      <c r="A23" s="117"/>
       <c r="B23" s="82"/>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
       <c r="E23" s="26"/>
     </row>
     <row r="24" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="116"/>
+      <c r="A24" s="117"/>
       <c r="B24" s="82"/>
       <c r="C24" s="25"/>
       <c r="D24" s="25"/>
       <c r="E24" s="26"/>
     </row>
     <row r="25" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="115" t="s">
+      <c r="A25" s="116" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="24"/>
@@ -3393,7 +3393,7 @@
       <c r="E25" s="26"/>
     </row>
     <row r="26" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="117"/>
+      <c r="A26" s="118"/>
       <c r="B26" s="24"/>
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
@@ -3609,8 +3609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B769BC50-9623-4726-8971-E5FD68E08F76}">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3635,18 +3635,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="177" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="143"/>
-      <c r="I1" s="143"/>
-      <c r="J1" s="143"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="178"/>
     </row>
     <row r="2" spans="1:19" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
@@ -3667,14 +3667,14 @@
       <c r="F2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="194" t="s">
+      <c r="G2" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="195"/>
-      <c r="I2" s="194" t="s">
-        <v>152</v>
-      </c>
-      <c r="J2" s="195"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="127" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" s="128"/>
       <c r="L2" s="12" t="s">
         <v>32</v>
       </c>
@@ -3701,24 +3701,24 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="196" t="s">
-        <v>153</v>
+      <c r="A3" s="129" t="s">
+        <v>152</v>
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" s="114" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F3" s="37"/>
-      <c r="G3" s="199"/>
-      <c r="H3" s="200"/>
-      <c r="I3" s="199"/>
-      <c r="J3" s="201"/>
+      <c r="G3" s="132"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="134"/>
       <c r="L3" s="13" t="s">
         <v>105</v>
       </c>
@@ -3745,22 +3745,22 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="197"/>
+      <c r="A4" s="130"/>
       <c r="B4" s="39"/>
       <c r="C4" s="39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D4" s="113" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F4" s="39"/>
-      <c r="G4" s="202"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="202"/>
-      <c r="J4" s="204"/>
+      <c r="G4" s="135"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="135"/>
+      <c r="J4" s="137"/>
       <c r="L4" s="13" t="s">
         <v>106</v>
       </c>
@@ -3787,22 +3787,22 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="198"/>
+      <c r="A5" s="131"/>
       <c r="B5" s="40"/>
       <c r="C5" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E5" s="41" t="s">
         <v>49</v>
       </c>
       <c r="F5" s="40"/>
-      <c r="G5" s="205"/>
-      <c r="H5" s="206"/>
-      <c r="I5" s="205"/>
-      <c r="J5" s="207"/>
+      <c r="G5" s="138"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="138"/>
+      <c r="J5" s="140"/>
       <c r="L5" s="13" t="s">
         <v>110</v>
       </c>
@@ -3829,26 +3829,26 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="192" t="s">
-        <v>156</v>
+      <c r="A6" s="165" t="s">
+        <v>155</v>
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E6" s="42" t="s">
         <v>49</v>
       </c>
       <c r="F6" s="42" t="s">
-        <v>173</v>
-      </c>
-      <c r="G6" s="171"/>
-      <c r="H6" s="172"/>
-      <c r="I6" s="171"/>
-      <c r="J6" s="173"/>
+        <v>172</v>
+      </c>
+      <c r="G6" s="144"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="144"/>
+      <c r="J6" s="146"/>
       <c r="L6" s="13" t="s">
         <v>114</v>
       </c>
@@ -3875,24 +3875,24 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="193"/>
+      <c r="A7" s="166"/>
       <c r="B7" s="44"/>
       <c r="C7" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D7" s="44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E7" s="44" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>173</v>
-      </c>
-      <c r="G7" s="174"/>
-      <c r="H7" s="175"/>
-      <c r="I7" s="174"/>
-      <c r="J7" s="176"/>
+        <v>172</v>
+      </c>
+      <c r="G7" s="147"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="147"/>
+      <c r="J7" s="149"/>
       <c r="L7" s="97" t="s">
         <v>102</v>
       </c>
@@ -3919,28 +3919,28 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="177" t="s">
-        <v>155</v>
+      <c r="A8" s="150" t="s">
+        <v>154</v>
       </c>
       <c r="B8" s="45"/>
       <c r="C8" s="45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E8" s="45" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="G8" s="189"/>
-      <c r="H8" s="191"/>
-      <c r="I8" s="189"/>
-      <c r="J8" s="190"/>
+        <v>172</v>
+      </c>
+      <c r="G8" s="162"/>
+      <c r="H8" s="164"/>
+      <c r="I8" s="162"/>
+      <c r="J8" s="163"/>
       <c r="L8" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M8" s="14">
         <v>15</v>
@@ -3949,7 +3949,7 @@
         <v>30</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P8" s="14" t="s">
         <v>48</v>
@@ -3958,26 +3958,26 @@
         <v>49</v>
       </c>
       <c r="R8" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="S8" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="S8" s="14" t="s">
-        <v>302</v>
-      </c>
     </row>
     <row r="9" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="178"/>
+      <c r="A9" s="151"/>
       <c r="B9" s="46"/>
       <c r="C9" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E9" s="46" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G9" s="99"/>
       <c r="H9" s="100"/>
@@ -3985,19 +3985,19 @@
       <c r="J9" s="101"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="179"/>
+      <c r="A10" s="152"/>
       <c r="B10" s="47"/>
       <c r="C10" s="47" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D10" s="47" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E10" s="47" t="s">
         <v>44</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G10" s="102"/>
       <c r="H10" s="103"/>
@@ -4005,46 +4005,46 @@
       <c r="J10" s="104"/>
     </row>
     <row r="11" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="168" t="s">
-        <v>154</v>
+      <c r="A11" s="141" t="s">
+        <v>153</v>
       </c>
       <c r="B11" s="48"/>
       <c r="C11" s="48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D11" s="48" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E11" s="48" t="s">
         <v>49</v>
       </c>
       <c r="F11" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="G11" s="183"/>
-      <c r="H11" s="184"/>
-      <c r="I11" s="183"/>
-      <c r="J11" s="185"/>
+        <v>172</v>
+      </c>
+      <c r="G11" s="156"/>
+      <c r="H11" s="157"/>
+      <c r="I11" s="156"/>
+      <c r="J11" s="158"/>
     </row>
     <row r="12" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="169"/>
+      <c r="A12" s="142"/>
       <c r="B12" s="49"/>
       <c r="C12" s="49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E12" s="49" t="s">
         <v>49</v>
       </c>
       <c r="F12" s="49" t="s">
-        <v>173</v>
-      </c>
-      <c r="G12" s="186"/>
-      <c r="H12" s="187"/>
-      <c r="I12" s="186"/>
-      <c r="J12" s="188"/>
+        <v>172</v>
+      </c>
+      <c r="G12" s="159"/>
+      <c r="H12" s="160"/>
+      <c r="I12" s="159"/>
+      <c r="J12" s="161"/>
       <c r="L12" s="95"/>
       <c r="M12" s="95"/>
       <c r="N12" s="95"/>
@@ -4055,24 +4055,24 @@
       <c r="S12" s="95"/>
     </row>
     <row r="13" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="170"/>
+      <c r="A13" s="143"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D13" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E13" s="50" t="s">
         <v>49</v>
       </c>
       <c r="F13" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="G13" s="180"/>
-      <c r="H13" s="181"/>
-      <c r="I13" s="180"/>
-      <c r="J13" s="182"/>
+        <v>172</v>
+      </c>
+      <c r="G13" s="153"/>
+      <c r="H13" s="154"/>
+      <c r="I13" s="153"/>
+      <c r="J13" s="155"/>
       <c r="L13" s="96"/>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
@@ -4083,21 +4083,21 @@
       <c r="S13" s="21"/>
     </row>
     <row r="14" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="128" t="s">
-        <v>157</v>
+      <c r="A14" s="195" t="s">
+        <v>156</v>
       </c>
       <c r="B14" s="51"/>
       <c r="C14" s="51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E14" s="51" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G14" s="167"/>
       <c r="H14" s="167"/>
@@ -4113,24 +4113,24 @@
       <c r="S14" s="21"/>
     </row>
     <row r="15" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="129"/>
+      <c r="A15" s="196"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D15" s="52" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E15" s="52" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>173</v>
-      </c>
-      <c r="G15" s="158"/>
-      <c r="H15" s="158"/>
-      <c r="I15" s="158"/>
-      <c r="J15" s="158"/>
+        <v>172</v>
+      </c>
+      <c r="G15" s="168"/>
+      <c r="H15" s="168"/>
+      <c r="I15" s="168"/>
+      <c r="J15" s="168"/>
       <c r="L15" s="96"/>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
@@ -4141,24 +4141,24 @@
       <c r="S15" s="21"/>
     </row>
     <row r="16" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="129"/>
+      <c r="A16" s="196"/>
       <c r="B16" s="52"/>
       <c r="C16" s="52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D16" s="52" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E16" s="52" t="s">
         <v>41</v>
       </c>
       <c r="F16" s="53" t="s">
-        <v>173</v>
-      </c>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
+        <v>172</v>
+      </c>
+      <c r="G16" s="168"/>
+      <c r="H16" s="168"/>
+      <c r="I16" s="168"/>
+      <c r="J16" s="168"/>
       <c r="L16" s="96"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
@@ -4169,24 +4169,24 @@
       <c r="S16" s="21"/>
     </row>
     <row r="17" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="129"/>
+      <c r="A17" s="196"/>
       <c r="B17" s="52"/>
       <c r="C17" s="52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D17" s="52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E17" s="52" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="53" t="s">
-        <v>173</v>
-      </c>
-      <c r="G17" s="158"/>
-      <c r="H17" s="158"/>
-      <c r="I17" s="158"/>
-      <c r="J17" s="158"/>
+        <v>172</v>
+      </c>
+      <c r="G17" s="168"/>
+      <c r="H17" s="168"/>
+      <c r="I17" s="168"/>
+      <c r="J17" s="168"/>
       <c r="L17" s="96"/>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
@@ -4197,475 +4197,475 @@
       <c r="S17" s="21"/>
     </row>
     <row r="18" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="129"/>
+      <c r="A18" s="196"/>
       <c r="B18" s="52"/>
       <c r="C18" s="52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D18" s="52" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E18" s="52" t="s">
         <v>41</v>
       </c>
       <c r="F18" s="53" t="s">
-        <v>173</v>
-      </c>
-      <c r="G18" s="158"/>
-      <c r="H18" s="158"/>
-      <c r="I18" s="158"/>
-      <c r="J18" s="158"/>
+        <v>172</v>
+      </c>
+      <c r="G18" s="168"/>
+      <c r="H18" s="168"/>
+      <c r="I18" s="168"/>
+      <c r="J18" s="168"/>
     </row>
     <row r="19" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="129"/>
+      <c r="A19" s="196"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D19" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E19" s="52" t="s">
         <v>41</v>
       </c>
       <c r="F19" s="53" t="s">
-        <v>173</v>
-      </c>
-      <c r="G19" s="158"/>
-      <c r="H19" s="158"/>
-      <c r="I19" s="158"/>
-      <c r="J19" s="158"/>
+        <v>172</v>
+      </c>
+      <c r="G19" s="168"/>
+      <c r="H19" s="168"/>
+      <c r="I19" s="168"/>
+      <c r="J19" s="168"/>
     </row>
     <row r="20" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="129"/>
+      <c r="A20" s="196"/>
       <c r="B20" s="52"/>
       <c r="C20" s="52" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D20" s="52" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E20" s="52" t="s">
         <v>41</v>
       </c>
       <c r="F20" s="53" t="s">
-        <v>173</v>
-      </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="158"/>
-      <c r="J20" s="158"/>
+        <v>172</v>
+      </c>
+      <c r="G20" s="168"/>
+      <c r="H20" s="168"/>
+      <c r="I20" s="168"/>
+      <c r="J20" s="168"/>
     </row>
     <row r="21" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="130"/>
+      <c r="A21" s="197"/>
       <c r="B21" s="54"/>
       <c r="C21" s="55" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D21" s="55" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E21" s="55" t="s">
         <v>41</v>
       </c>
       <c r="F21" s="54" t="s">
-        <v>173</v>
-      </c>
-      <c r="G21" s="159"/>
-      <c r="H21" s="159"/>
-      <c r="I21" s="159"/>
-      <c r="J21" s="159"/>
+        <v>172</v>
+      </c>
+      <c r="G21" s="191"/>
+      <c r="H21" s="191"/>
+      <c r="I21" s="191"/>
+      <c r="J21" s="191"/>
     </row>
     <row r="22" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="163" t="s">
-        <v>158</v>
+      <c r="A22" s="169" t="s">
+        <v>157</v>
       </c>
       <c r="B22" s="56"/>
       <c r="C22" s="57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D22" s="56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E22" s="56" t="s">
         <v>41</v>
       </c>
       <c r="F22" s="56" t="s">
-        <v>173</v>
-      </c>
-      <c r="G22" s="160"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="160"/>
-      <c r="J22" s="166"/>
+        <v>172</v>
+      </c>
+      <c r="G22" s="175"/>
+      <c r="H22" s="192"/>
+      <c r="I22" s="175"/>
+      <c r="J22" s="176"/>
     </row>
     <row r="23" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="164"/>
+      <c r="A23" s="170"/>
       <c r="B23" s="58"/>
       <c r="C23" s="59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D23" s="58" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E23" s="58" t="s">
         <v>41</v>
       </c>
       <c r="F23" s="58" t="s">
-        <v>173</v>
-      </c>
-      <c r="G23" s="150"/>
-      <c r="H23" s="162"/>
-      <c r="I23" s="150"/>
-      <c r="J23" s="151"/>
+        <v>172</v>
+      </c>
+      <c r="G23" s="172"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="172"/>
+      <c r="J23" s="174"/>
     </row>
     <row r="24" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="164"/>
+      <c r="A24" s="170"/>
       <c r="B24" s="58"/>
       <c r="C24" s="59" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D24" s="58" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E24" s="58" t="s">
         <v>41</v>
       </c>
       <c r="F24" s="58" t="s">
-        <v>173</v>
-      </c>
-      <c r="G24" s="150"/>
-      <c r="H24" s="162"/>
-      <c r="I24" s="150"/>
-      <c r="J24" s="151"/>
+        <v>172</v>
+      </c>
+      <c r="G24" s="172"/>
+      <c r="H24" s="173"/>
+      <c r="I24" s="172"/>
+      <c r="J24" s="174"/>
     </row>
     <row r="25" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="164"/>
+      <c r="A25" s="170"/>
       <c r="B25" s="58"/>
       <c r="C25" s="59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D25" s="58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E25" s="58" t="s">
         <v>41</v>
       </c>
       <c r="F25" s="58" t="s">
-        <v>173</v>
-      </c>
-      <c r="G25" s="150"/>
-      <c r="H25" s="162"/>
-      <c r="I25" s="150"/>
-      <c r="J25" s="151"/>
+        <v>172</v>
+      </c>
+      <c r="G25" s="172"/>
+      <c r="H25" s="173"/>
+      <c r="I25" s="172"/>
+      <c r="J25" s="174"/>
     </row>
     <row r="26" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="164"/>
+      <c r="A26" s="170"/>
       <c r="B26" s="58"/>
       <c r="C26" s="59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D26" s="58" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E26" s="58" t="s">
         <v>41</v>
       </c>
       <c r="F26" s="58" t="s">
-        <v>173</v>
-      </c>
-      <c r="G26" s="150"/>
-      <c r="H26" s="162"/>
-      <c r="I26" s="150"/>
-      <c r="J26" s="151"/>
+        <v>172</v>
+      </c>
+      <c r="G26" s="172"/>
+      <c r="H26" s="173"/>
+      <c r="I26" s="172"/>
+      <c r="J26" s="174"/>
     </row>
     <row r="27" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="164"/>
+      <c r="A27" s="170"/>
       <c r="B27" s="58"/>
       <c r="C27" s="59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D27" s="58" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E27" s="58" t="s">
         <v>41</v>
       </c>
       <c r="F27" s="58" t="s">
-        <v>173</v>
-      </c>
-      <c r="G27" s="150"/>
-      <c r="H27" s="162"/>
-      <c r="I27" s="150"/>
-      <c r="J27" s="151"/>
+        <v>172</v>
+      </c>
+      <c r="G27" s="172"/>
+      <c r="H27" s="173"/>
+      <c r="I27" s="172"/>
+      <c r="J27" s="174"/>
     </row>
     <row r="28" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="165"/>
+      <c r="A28" s="171"/>
       <c r="B28" s="60"/>
       <c r="C28" s="61" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D28" s="60" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E28" s="60" t="s">
         <v>41</v>
       </c>
       <c r="F28" s="60" t="s">
-        <v>173</v>
-      </c>
-      <c r="G28" s="152"/>
-      <c r="H28" s="153"/>
-      <c r="I28" s="152"/>
-      <c r="J28" s="154"/>
+        <v>172</v>
+      </c>
+      <c r="G28" s="185"/>
+      <c r="H28" s="186"/>
+      <c r="I28" s="185"/>
+      <c r="J28" s="187"/>
     </row>
     <row r="29" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="131" t="s">
-        <v>161</v>
+      <c r="A29" s="198" t="s">
+        <v>160</v>
       </c>
       <c r="B29" s="62"/>
       <c r="C29" s="62" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D29" s="62" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F29" s="62" t="s">
-        <v>235</v>
-      </c>
-      <c r="G29" s="155"/>
-      <c r="H29" s="156"/>
-      <c r="I29" s="155"/>
-      <c r="J29" s="157"/>
+        <v>234</v>
+      </c>
+      <c r="G29" s="188"/>
+      <c r="H29" s="189"/>
+      <c r="I29" s="188"/>
+      <c r="J29" s="190"/>
     </row>
     <row r="30" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="132"/>
+      <c r="A30" s="199"/>
       <c r="B30" s="63"/>
       <c r="C30" s="64" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D30" s="63" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E30" s="63" t="s">
         <v>41</v>
       </c>
       <c r="F30" s="63" t="s">
-        <v>173</v>
-      </c>
-      <c r="G30" s="144"/>
-      <c r="H30" s="145"/>
-      <c r="I30" s="144"/>
-      <c r="J30" s="146"/>
+        <v>172</v>
+      </c>
+      <c r="G30" s="179"/>
+      <c r="H30" s="180"/>
+      <c r="I30" s="179"/>
+      <c r="J30" s="181"/>
     </row>
     <row r="31" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="105" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B31" s="106"/>
       <c r="C31" s="66" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D31" s="65" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E31" s="65" t="s">
         <v>49</v>
       </c>
       <c r="F31" s="65" t="s">
-        <v>173</v>
-      </c>
-      <c r="G31" s="147"/>
-      <c r="H31" s="148"/>
-      <c r="I31" s="147"/>
-      <c r="J31" s="149"/>
+        <v>172</v>
+      </c>
+      <c r="G31" s="182"/>
+      <c r="H31" s="183"/>
+      <c r="I31" s="182"/>
+      <c r="J31" s="184"/>
     </row>
     <row r="32" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B32" s="69" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C32" s="67" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D32" s="68" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E32" s="68" t="s">
         <v>41</v>
       </c>
       <c r="F32" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="G32" s="136"/>
-      <c r="H32" s="137"/>
-      <c r="I32" s="136"/>
-      <c r="J32" s="138"/>
+        <v>172</v>
+      </c>
+      <c r="G32" s="203"/>
+      <c r="H32" s="204"/>
+      <c r="I32" s="203"/>
+      <c r="J32" s="205"/>
     </row>
     <row r="33" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="69" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B33" s="69" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C33" s="67" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D33" s="68" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E33" s="69" t="s">
         <v>41</v>
       </c>
       <c r="F33" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="G33" s="139"/>
-      <c r="H33" s="140"/>
-      <c r="I33" s="139"/>
-      <c r="J33" s="141"/>
+        <v>172</v>
+      </c>
+      <c r="G33" s="206"/>
+      <c r="H33" s="207"/>
+      <c r="I33" s="206"/>
+      <c r="J33" s="208"/>
     </row>
     <row r="34" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="69" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B34" s="69" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C34" s="67" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D34" s="68" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E34" s="70" t="s">
         <v>41</v>
       </c>
       <c r="F34" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="G34" s="133"/>
-      <c r="H34" s="134"/>
-      <c r="I34" s="133"/>
-      <c r="J34" s="135"/>
+        <v>172</v>
+      </c>
+      <c r="G34" s="200"/>
+      <c r="H34" s="201"/>
+      <c r="I34" s="200"/>
+      <c r="J34" s="202"/>
     </row>
     <row r="35" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="109" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B35" s="69" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C35" s="67" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D35" s="68" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E35" s="70" t="s">
         <v>41</v>
       </c>
       <c r="F35" s="68" t="s">
-        <v>173</v>
-      </c>
-      <c r="G35" s="133"/>
-      <c r="H35" s="134"/>
-      <c r="I35" s="133"/>
-      <c r="J35" s="135"/>
+        <v>172</v>
+      </c>
+      <c r="G35" s="200"/>
+      <c r="H35" s="201"/>
+      <c r="I35" s="200"/>
+      <c r="J35" s="202"/>
     </row>
     <row r="36" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="107" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B36" s="108" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C36" s="72" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D36" s="71" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E36" s="71" t="s">
         <v>41</v>
       </c>
       <c r="F36" s="71" t="s">
-        <v>173</v>
-      </c>
-      <c r="G36" s="126"/>
-      <c r="H36" s="126"/>
-      <c r="I36" s="126"/>
-      <c r="J36" s="127"/>
+        <v>172</v>
+      </c>
+      <c r="G36" s="193"/>
+      <c r="H36" s="193"/>
+      <c r="I36" s="193"/>
+      <c r="J36" s="194"/>
     </row>
     <row r="37" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="73" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B37" s="94" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C37" s="72" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D37" s="71" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E37" s="71" t="s">
         <v>41</v>
       </c>
       <c r="F37" s="71" t="s">
-        <v>173</v>
-      </c>
-      <c r="G37" s="126"/>
-      <c r="H37" s="126"/>
-      <c r="I37" s="126"/>
-      <c r="J37" s="127"/>
+        <v>172</v>
+      </c>
+      <c r="G37" s="193"/>
+      <c r="H37" s="193"/>
+      <c r="I37" s="193"/>
+      <c r="J37" s="194"/>
     </row>
     <row r="38" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A38" s="74" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B38" s="93" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C38" s="72" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D38" s="75" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E38" s="75" t="s">
         <v>41</v>
       </c>
       <c r="F38" s="75" t="s">
-        <v>173</v>
-      </c>
-      <c r="G38" s="126"/>
-      <c r="H38" s="126"/>
-      <c r="I38" s="126"/>
-      <c r="J38" s="127"/>
+        <v>172</v>
+      </c>
+      <c r="G38" s="193"/>
+      <c r="H38" s="193"/>
+      <c r="I38" s="193"/>
+      <c r="J38" s="194"/>
     </row>
     <row r="39" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A39" s="58" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B39" s="58" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C39" s="58"/>
       <c r="D39" s="58" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E39" s="58" t="s">
         <v>41</v>
       </c>
       <c r="F39" s="58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G39" s="58"/>
       <c r="H39" s="58"/>
@@ -4674,20 +4674,20 @@
     </row>
     <row r="40" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A40" s="58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B40" s="58" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C40" s="58"/>
       <c r="D40" s="58" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E40" s="58" t="s">
         <v>41</v>
       </c>
       <c r="F40" s="58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G40" s="58"/>
       <c r="H40" s="58"/>
@@ -4695,23 +4695,23 @@
       <c r="J40" s="58"/>
     </row>
     <row r="41" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="219"/>
-      <c r="B41" s="219" t="s">
-        <v>303</v>
-      </c>
-      <c r="C41" s="219"/>
-      <c r="D41" s="219"/>
-      <c r="E41" s="219"/>
-      <c r="F41" s="219"/>
-      <c r="G41" s="219"/>
-      <c r="H41" s="219"/>
-      <c r="I41" s="219"/>
-      <c r="J41" s="219"/>
+      <c r="A41" s="115"/>
+      <c r="B41" s="115" t="s">
+        <v>302</v>
+      </c>
+      <c r="C41" s="115"/>
+      <c r="D41" s="115"/>
+      <c r="E41" s="115"/>
+      <c r="F41" s="115"/>
+      <c r="G41" s="115"/>
+      <c r="H41" s="115"/>
+      <c r="I41" s="115"/>
+      <c r="J41" s="115"/>
     </row>
     <row r="42" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A42" s="28"/>
       <c r="B42" s="109" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -4725,7 +4725,7 @@
     <row r="43" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A43" s="28"/>
       <c r="B43" s="109" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -4739,7 +4739,7 @@
     <row r="44" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A44" s="28"/>
       <c r="B44" s="109" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -4776,52 +4776,22 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="I30:J30"/>
@@ -4838,22 +4808,52 @@
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="A14:A21"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4865,8 +4865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27F8DC3-BDE0-43F3-979D-2CCDC5541D2C}">
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D36" sqref="D35:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4890,14 +4890,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -4918,14 +4918,14 @@
       <c r="F2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="209" t="s">
+      <c r="G2" s="214" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="209"/>
-      <c r="I2" s="209" t="s">
-        <v>152</v>
-      </c>
-      <c r="J2" s="209"/>
+      <c r="H2" s="214"/>
+      <c r="I2" s="214" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" s="214"/>
       <c r="N2" t="s">
         <v>77</v>
       </c>
@@ -4938,24 +4938,24 @@
       <c r="U2" s="21"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="208" t="s">
+      <c r="A3" s="215" t="s">
         <v>117</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="110" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D3" s="111" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E3" s="111" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F3" s="26"/>
-      <c r="G3" s="210"/>
-      <c r="H3" s="211"/>
-      <c r="I3" s="210"/>
-      <c r="J3" s="211"/>
+      <c r="G3" s="209"/>
+      <c r="H3" s="210"/>
+      <c r="I3" s="209"/>
+      <c r="J3" s="210"/>
       <c r="N3" s="35" t="s">
         <v>32</v>
       </c>
@@ -4982,22 +4982,22 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="208"/>
+      <c r="A4" s="215"/>
       <c r="B4" s="26"/>
       <c r="C4" s="110" t="s">
+        <v>291</v>
+      </c>
+      <c r="D4" s="112" t="s">
         <v>292</v>
       </c>
-      <c r="D4" s="112" t="s">
-        <v>293</v>
-      </c>
       <c r="E4" s="111" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F4" s="26"/>
-      <c r="G4" s="210"/>
-      <c r="H4" s="211"/>
-      <c r="I4" s="210"/>
-      <c r="J4" s="211"/>
+      <c r="G4" s="209"/>
+      <c r="H4" s="210"/>
+      <c r="I4" s="209"/>
+      <c r="J4" s="210"/>
       <c r="N4" s="22" t="s">
         <v>78</v>
       </c>
@@ -5024,22 +5024,22 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="208"/>
+      <c r="A5" s="215"/>
       <c r="B5" s="26"/>
       <c r="C5" s="110" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" s="112" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E5" s="112" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="26"/>
-      <c r="G5" s="210"/>
-      <c r="H5" s="211"/>
-      <c r="I5" s="210"/>
-      <c r="J5" s="211"/>
+      <c r="G5" s="209"/>
+      <c r="H5" s="210"/>
+      <c r="I5" s="209"/>
+      <c r="J5" s="210"/>
       <c r="N5" s="22" t="s">
         <v>82</v>
       </c>
@@ -5066,26 +5066,26 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="208" t="s">
+      <c r="A6" s="215" t="s">
         <v>118</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="110" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D6" s="112" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E6" s="112" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G6" s="210"/>
-      <c r="H6" s="211"/>
-      <c r="I6" s="210"/>
-      <c r="J6" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G6" s="209"/>
+      <c r="H6" s="210"/>
+      <c r="I6" s="209"/>
+      <c r="J6" s="210"/>
       <c r="N6" s="22" t="s">
         <v>86</v>
       </c>
@@ -5112,24 +5112,24 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="208"/>
+      <c r="A7" s="215"/>
       <c r="B7" s="26"/>
       <c r="C7" s="110" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D7" s="112" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E7" s="112" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G7" s="210"/>
-      <c r="H7" s="211"/>
-      <c r="I7" s="210"/>
-      <c r="J7" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G7" s="209"/>
+      <c r="H7" s="210"/>
+      <c r="I7" s="209"/>
+      <c r="J7" s="210"/>
       <c r="N7" s="22" t="s">
         <v>90</v>
       </c>
@@ -5156,26 +5156,26 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="208" t="s">
+      <c r="A8" s="215" t="s">
         <v>119</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="110" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D8" s="112" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E8" s="112" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G8" s="210"/>
-      <c r="H8" s="211"/>
-      <c r="I8" s="210"/>
-      <c r="J8" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G8" s="209"/>
+      <c r="H8" s="210"/>
+      <c r="I8" s="209"/>
+      <c r="J8" s="210"/>
       <c r="N8" s="29" t="s">
         <v>94</v>
       </c>
@@ -5202,24 +5202,24 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="208"/>
+      <c r="A9" s="215"/>
       <c r="B9" s="26"/>
       <c r="C9" s="110" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D9" s="112" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E9" s="112" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G9" s="210"/>
-      <c r="H9" s="211"/>
-      <c r="I9" s="210"/>
-      <c r="J9" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G9" s="209"/>
+      <c r="H9" s="210"/>
+      <c r="I9" s="209"/>
+      <c r="J9" s="210"/>
       <c r="L9" s="31"/>
       <c r="M9" s="32"/>
       <c r="N9" s="33" t="s">
@@ -5248,688 +5248,633 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="215"/>
       <c r="B10" s="26"/>
       <c r="C10" s="110" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D10" s="112" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E10" s="112" t="s">
         <v>44</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G10" s="210"/>
-      <c r="H10" s="211"/>
-      <c r="I10" s="210"/>
-      <c r="J10" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G10" s="209"/>
+      <c r="H10" s="210"/>
+      <c r="I10" s="209"/>
+      <c r="J10" s="210"/>
     </row>
     <row r="11" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="208" t="s">
+      <c r="A11" s="215" t="s">
         <v>120</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E11" s="23" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G11" s="210"/>
-      <c r="H11" s="211"/>
-      <c r="I11" s="210"/>
-      <c r="J11" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G11" s="209"/>
+      <c r="H11" s="210"/>
+      <c r="I11" s="209"/>
+      <c r="J11" s="210"/>
     </row>
     <row r="12" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="208"/>
+      <c r="A12" s="215"/>
       <c r="B12" s="26"/>
       <c r="C12" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G12" s="210"/>
-      <c r="H12" s="211"/>
-      <c r="I12" s="210"/>
-      <c r="J12" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G12" s="209"/>
+      <c r="H12" s="210"/>
+      <c r="I12" s="209"/>
+      <c r="J12" s="210"/>
     </row>
     <row r="13" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="208"/>
+      <c r="A13" s="215"/>
       <c r="B13" s="26"/>
       <c r="C13" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G13" s="210"/>
-      <c r="H13" s="211"/>
-      <c r="I13" s="210"/>
-      <c r="J13" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G13" s="209"/>
+      <c r="H13" s="210"/>
+      <c r="I13" s="209"/>
+      <c r="J13" s="210"/>
     </row>
     <row r="14" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="215" t="s">
+      <c r="A14" s="216" t="s">
         <v>121</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G14" s="210"/>
-      <c r="H14" s="211"/>
-      <c r="I14" s="210"/>
-      <c r="J14" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G14" s="209"/>
+      <c r="H14" s="210"/>
+      <c r="I14" s="209"/>
+      <c r="J14" s="210"/>
     </row>
     <row r="15" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="216"/>
+      <c r="A15" s="217"/>
       <c r="B15" s="26"/>
       <c r="C15" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G15" s="210"/>
-      <c r="H15" s="211"/>
-      <c r="I15" s="210"/>
-      <c r="J15" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G15" s="209"/>
+      <c r="H15" s="210"/>
+      <c r="I15" s="209"/>
+      <c r="J15" s="210"/>
     </row>
     <row r="16" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="216"/>
+      <c r="A16" s="217"/>
       <c r="B16" s="26"/>
       <c r="C16" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G16" s="210"/>
-      <c r="H16" s="211"/>
-      <c r="I16" s="210"/>
-      <c r="J16" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G16" s="209"/>
+      <c r="H16" s="210"/>
+      <c r="I16" s="209"/>
+      <c r="J16" s="210"/>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="216"/>
+      <c r="A17" s="217"/>
       <c r="B17" s="26"/>
       <c r="C17" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G17" s="210"/>
-      <c r="H17" s="211"/>
-      <c r="I17" s="210"/>
-      <c r="J17" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G17" s="209"/>
+      <c r="H17" s="210"/>
+      <c r="I17" s="209"/>
+      <c r="J17" s="210"/>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="216"/>
+      <c r="A18" s="217"/>
       <c r="B18" s="26"/>
       <c r="C18" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G18" s="210"/>
-      <c r="H18" s="211"/>
-      <c r="I18" s="210"/>
-      <c r="J18" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G18" s="209"/>
+      <c r="H18" s="210"/>
+      <c r="I18" s="209"/>
+      <c r="J18" s="210"/>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="216"/>
+      <c r="A19" s="217"/>
       <c r="B19" s="26"/>
       <c r="C19" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G19" s="210"/>
-      <c r="H19" s="211"/>
-      <c r="I19" s="210"/>
-      <c r="J19" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G19" s="209"/>
+      <c r="H19" s="210"/>
+      <c r="I19" s="209"/>
+      <c r="J19" s="210"/>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="217"/>
+      <c r="A20" s="218"/>
       <c r="B20" s="26"/>
       <c r="C20" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G20" s="210"/>
-      <c r="H20" s="211"/>
-      <c r="I20" s="210"/>
-      <c r="J20" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G20" s="209"/>
+      <c r="H20" s="210"/>
+      <c r="I20" s="209"/>
+      <c r="J20" s="210"/>
     </row>
     <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="212" t="s">
+      <c r="A21" s="211" t="s">
         <v>122</v>
       </c>
       <c r="B21" s="28"/>
       <c r="C21" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G21" s="210"/>
-      <c r="H21" s="211"/>
-      <c r="I21" s="210"/>
-      <c r="J21" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G21" s="209"/>
+      <c r="H21" s="210"/>
+      <c r="I21" s="209"/>
+      <c r="J21" s="210"/>
     </row>
     <row r="22" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="213"/>
+      <c r="A22" s="212"/>
       <c r="B22" s="28"/>
       <c r="C22" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G22" s="210"/>
-      <c r="H22" s="211"/>
-      <c r="I22" s="210"/>
-      <c r="J22" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G22" s="209"/>
+      <c r="H22" s="210"/>
+      <c r="I22" s="209"/>
+      <c r="J22" s="210"/>
     </row>
     <row r="23" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="213"/>
+      <c r="A23" s="212"/>
       <c r="B23" s="28"/>
       <c r="C23" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G23" s="210"/>
-      <c r="H23" s="211"/>
-      <c r="I23" s="210"/>
-      <c r="J23" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G23" s="209"/>
+      <c r="H23" s="210"/>
+      <c r="I23" s="209"/>
+      <c r="J23" s="210"/>
     </row>
     <row r="24" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="213"/>
+      <c r="A24" s="212"/>
       <c r="B24" s="28"/>
       <c r="C24" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E24" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G24" s="210"/>
-      <c r="H24" s="211"/>
-      <c r="I24" s="210"/>
-      <c r="J24" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G24" s="209"/>
+      <c r="H24" s="210"/>
+      <c r="I24" s="209"/>
+      <c r="J24" s="210"/>
     </row>
     <row r="25" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="213"/>
+      <c r="A25" s="212"/>
       <c r="B25" s="28"/>
       <c r="C25" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E25" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G25" s="210"/>
-      <c r="H25" s="211"/>
-      <c r="I25" s="210"/>
-      <c r="J25" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G25" s="209"/>
+      <c r="H25" s="210"/>
+      <c r="I25" s="209"/>
+      <c r="J25" s="210"/>
     </row>
     <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="213"/>
+      <c r="A26" s="212"/>
       <c r="B26" s="28"/>
       <c r="C26" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E26" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G26" s="210"/>
-      <c r="H26" s="211"/>
-      <c r="I26" s="210"/>
-      <c r="J26" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G26" s="209"/>
+      <c r="H26" s="210"/>
+      <c r="I26" s="209"/>
+      <c r="J26" s="210"/>
     </row>
     <row r="27" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="213"/>
+      <c r="A27" s="212"/>
       <c r="B27" s="28"/>
       <c r="C27" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G27" s="210"/>
-      <c r="H27" s="211"/>
-      <c r="I27" s="210"/>
-      <c r="J27" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G27" s="209"/>
+      <c r="H27" s="210"/>
+      <c r="I27" s="209"/>
+      <c r="J27" s="210"/>
     </row>
     <row r="28" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="214"/>
+      <c r="A28" s="213"/>
       <c r="B28" s="28"/>
       <c r="C28" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E28" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G28" s="210"/>
-      <c r="H28" s="211"/>
-      <c r="I28" s="210"/>
-      <c r="J28" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G28" s="209"/>
+      <c r="H28" s="210"/>
+      <c r="I28" s="209"/>
+      <c r="J28" s="210"/>
     </row>
     <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>123</v>
+        <v>303</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E29" s="23" t="s">
         <v>41</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G29" s="210"/>
-      <c r="H29" s="211"/>
-      <c r="I29" s="210"/>
-      <c r="J29" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G29" s="209"/>
+      <c r="H29" s="210"/>
+      <c r="I29" s="209"/>
+      <c r="J29" s="210"/>
     </row>
     <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D30" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="E30" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D30" s="112" t="s">
+        <v>212</v>
+      </c>
+      <c r="E30" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G30" s="210"/>
-      <c r="H30" s="211"/>
-      <c r="I30" s="210"/>
-      <c r="J30" s="211"/>
+      <c r="F30" s="112" t="s">
+        <v>182</v>
+      </c>
+      <c r="G30" s="209"/>
+      <c r="H30" s="210"/>
+      <c r="I30" s="209"/>
+      <c r="J30" s="210"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D31" s="23" t="s">
-        <v>200</v>
-      </c>
-      <c r="E31" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" s="112" t="s">
+        <v>199</v>
+      </c>
+      <c r="E31" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G31" s="210"/>
-      <c r="H31" s="211"/>
-      <c r="I31" s="210"/>
-      <c r="J31" s="211"/>
+      <c r="F31" s="112" t="s">
+        <v>182</v>
+      </c>
+      <c r="G31" s="209"/>
+      <c r="H31" s="210"/>
+      <c r="I31" s="209"/>
+      <c r="J31" s="210"/>
     </row>
     <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="E32" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D32" s="112" t="s">
+        <v>200</v>
+      </c>
+      <c r="E32" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G32" s="210"/>
-      <c r="H32" s="211"/>
-      <c r="I32" s="210"/>
-      <c r="J32" s="211"/>
+      <c r="F32" s="112" t="s">
+        <v>182</v>
+      </c>
+      <c r="G32" s="209"/>
+      <c r="H32" s="210"/>
+      <c r="I32" s="209"/>
+      <c r="J32" s="210"/>
     </row>
     <row r="33" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="E33" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" s="112" t="s">
+        <v>209</v>
+      </c>
+      <c r="E33" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G33" s="210"/>
-      <c r="H33" s="211"/>
-      <c r="I33" s="210"/>
-      <c r="J33" s="211"/>
+      <c r="F33" s="112" t="s">
+        <v>182</v>
+      </c>
+      <c r="G33" s="209"/>
+      <c r="H33" s="210"/>
+      <c r="I33" s="209"/>
+      <c r="J33" s="210"/>
     </row>
     <row r="34" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D34" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="E34" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" s="112" t="s">
+        <v>210</v>
+      </c>
+      <c r="E34" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="F34" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G34" s="210"/>
-      <c r="H34" s="211"/>
-      <c r="I34" s="210"/>
-      <c r="J34" s="211"/>
+      <c r="F34" s="112" t="s">
+        <v>182</v>
+      </c>
+      <c r="G34" s="209"/>
+      <c r="H34" s="210"/>
+      <c r="I34" s="209"/>
+      <c r="J34" s="210"/>
     </row>
     <row r="35" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D35" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="E35" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35" s="112" t="s">
+        <v>211</v>
+      </c>
+      <c r="E35" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="F35" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G35" s="210"/>
-      <c r="H35" s="211"/>
-      <c r="I35" s="210"/>
-      <c r="J35" s="211"/>
+      <c r="F35" s="112" t="s">
+        <v>182</v>
+      </c>
+      <c r="G35" s="209"/>
+      <c r="H35" s="210"/>
+      <c r="I35" s="209"/>
+      <c r="J35" s="210"/>
     </row>
     <row r="36" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="E36" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D36" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="E36" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="F36" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G36" s="210"/>
-      <c r="H36" s="211"/>
-      <c r="I36" s="210"/>
-      <c r="J36" s="211"/>
+      <c r="F36" s="112" t="s">
+        <v>182</v>
+      </c>
+      <c r="G36" s="209"/>
+      <c r="H36" s="210"/>
+      <c r="I36" s="209"/>
+      <c r="J36" s="210"/>
     </row>
     <row r="37" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="23"/>
       <c r="E37" s="23"/>
       <c r="F37" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G37" s="210"/>
-      <c r="H37" s="211"/>
-      <c r="I37" s="210"/>
-      <c r="J37" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G37" s="209"/>
+      <c r="H37" s="210"/>
+      <c r="I37" s="209"/>
+      <c r="J37" s="210"/>
     </row>
     <row r="38" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="23"/>
       <c r="E38" s="23"/>
       <c r="F38" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G38" s="210"/>
-      <c r="H38" s="211"/>
-      <c r="I38" s="210"/>
-      <c r="J38" s="211"/>
+        <v>182</v>
+      </c>
+      <c r="G38" s="209"/>
+      <c r="H38" s="210"/>
+      <c r="I38" s="209"/>
+      <c r="J38" s="210"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="210"/>
-      <c r="H39" s="211"/>
-      <c r="I39" s="210"/>
-      <c r="J39" s="211"/>
+      <c r="G39" s="209"/>
+      <c r="H39" s="210"/>
+      <c r="I39" s="209"/>
+      <c r="J39" s="210"/>
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="A21:A28"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="G3:H3"/>
@@ -5946,12 +5891,67 @@
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:J38"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5980,20 +5980,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="218" t="s">
-        <v>236</v>
-      </c>
-      <c r="B1" s="218"/>
-      <c r="C1" s="218"/>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
+      <c r="A1" s="219" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" s="219"/>
+      <c r="C1" s="219"/>
+      <c r="D1" s="219"/>
+      <c r="E1" s="219"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="218"/>
-      <c r="B2" s="218"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
+      <c r="A2" s="219"/>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -6023,7 +6023,7 @@
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B4" s="14">
         <v>2</v>
@@ -6032,24 +6032,24 @@
         <v>2</v>
       </c>
       <c r="D4" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="F4" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>241</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" s="14">
         <v>2</v>
@@ -6058,19 +6058,19 @@
         <v>2</v>
       </c>
       <c r="D5" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="G5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>244</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6084,19 +6084,19 @@
         <v>2</v>
       </c>
       <c r="D6" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="G6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>247</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
átalakítás Pozsony 2024.03.17 14:54
</commit_message>
<xml_diff>
--- a/IP_cim_kiosztas.xlsx
+++ b/IP_cim_kiosztas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tibi\Documents\GitHub\Uzemelteto_vizsgaremek_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Vizsgaremek\Uzemelteto_vizsgaremek_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41862206-BEF5-4FEB-911D-8ACA0433E1A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC4FACB-226C-42EB-BFED-CF329E09597B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21975" windowHeight="14130" xr2:uid="{5DEB228F-9A24-4144-85FF-8E6948A8BA71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{5DEB228F-9A24-4144-85FF-8E6948A8BA71}"/>
   </bookViews>
   <sheets>
     <sheet name="Központi Iroda" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="308">
   <si>
     <t>Központi Iroda</t>
   </si>
@@ -956,6 +956,9 @@
   </si>
   <si>
     <t>Gyor_WiFi2</t>
+  </si>
+  <si>
+    <t>Pozsony_VLAN_19</t>
   </si>
 </sst>
 </file>
@@ -2181,33 +2184,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2247,154 +2223,79 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2421,6 +2322,12 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2439,59 +2346,161 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2507,12 +2516,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2856,7 +2859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00720853-46FD-4EE1-97EA-B1AFFEF5B41E}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -2881,20 +2884,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="108" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="60" t="s">
@@ -2903,7 +2906,7 @@
       <c r="D2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="122" t="s">
+      <c r="E2" s="113" t="s">
         <v>57</v>
       </c>
       <c r="F2" s="61" t="s">
@@ -2911,19 +2914,19 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="116"/>
-      <c r="B3" s="118"/>
-      <c r="C3" s="119" t="s">
+      <c r="A3" s="107"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="120"/>
-      <c r="E3" s="123"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="114"/>
       <c r="F3" s="62" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="112" t="s">
+      <c r="A4" s="103" t="s">
         <v>221</v>
       </c>
       <c r="B4" s="90" t="s">
@@ -2935,7 +2938,7 @@
       <c r="F4" s="91"/>
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="112"/>
+      <c r="A5" s="103"/>
       <c r="B5" s="92" t="s">
         <v>236</v>
       </c>
@@ -2961,7 +2964,7 @@
       <c r="S5" s="86"/>
     </row>
     <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="112"/>
+      <c r="A6" s="103"/>
       <c r="B6" s="92" t="s">
         <v>237</v>
       </c>
@@ -2987,7 +2990,7 @@
       <c r="S6" s="86"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="111" t="s">
+      <c r="A7" s="102" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="94"/>
@@ -3009,7 +3012,7 @@
       <c r="S7" s="86"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="121"/>
+      <c r="A8" s="112"/>
       <c r="B8" s="94"/>
       <c r="C8" s="93"/>
       <c r="D8" s="93"/>
@@ -3029,7 +3032,7 @@
       <c r="S8" s="86"/>
     </row>
     <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="111" t="s">
+      <c r="A9" s="102" t="s">
         <v>238</v>
       </c>
       <c r="B9" s="95" t="s">
@@ -3057,7 +3060,7 @@
       <c r="S9" s="86"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="112"/>
+      <c r="A10" s="103"/>
       <c r="B10" s="95" t="s">
         <v>241</v>
       </c>
@@ -3071,7 +3074,7 @@
       <c r="F10" s="93"/>
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="112"/>
+      <c r="A11" s="103"/>
       <c r="B11" s="95" t="s">
         <v>243</v>
       </c>
@@ -3083,39 +3086,39 @@
       </c>
       <c r="E11" s="96"/>
       <c r="F11" s="93"/>
-      <c r="I11" s="109" t="s">
+      <c r="I11" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="105" t="s">
+      <c r="J11" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="105" t="s">
+      <c r="K11" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="105" t="s">
+      <c r="L11" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="105" t="s">
+      <c r="M11" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="N11" s="105" t="s">
+      <c r="N11" s="120" t="s">
         <v>22</v>
       </c>
-      <c r="O11" s="105" t="s">
+      <c r="O11" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="P11" s="105" t="s">
+      <c r="P11" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="Q11" s="105" t="s">
+      <c r="Q11" s="120" t="s">
         <v>57</v>
       </c>
-      <c r="R11" s="107" t="s">
+      <c r="R11" s="122" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="112"/>
+      <c r="A12" s="103"/>
       <c r="B12" s="95" t="s">
         <v>245</v>
       </c>
@@ -3127,19 +3130,19 @@
       </c>
       <c r="E12" s="96"/>
       <c r="F12" s="93"/>
-      <c r="I12" s="110"/>
-      <c r="J12" s="106"/>
-      <c r="K12" s="106"/>
-      <c r="L12" s="106"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-      <c r="R12" s="108"/>
+      <c r="I12" s="119"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="121"/>
+      <c r="L12" s="121"/>
+      <c r="M12" s="121"/>
+      <c r="N12" s="121"/>
+      <c r="O12" s="121"/>
+      <c r="P12" s="121"/>
+      <c r="Q12" s="121"/>
+      <c r="R12" s="123"/>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="112"/>
+      <c r="A13" s="103"/>
       <c r="B13" s="95" t="s">
         <v>247</v>
       </c>
@@ -3151,113 +3154,113 @@
       </c>
       <c r="E13" s="96"/>
       <c r="F13" s="93"/>
-      <c r="I13" s="102" t="s">
+      <c r="I13" s="116" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="102">
+      <c r="J13" s="116">
         <v>7</v>
       </c>
-      <c r="K13" s="102">
+      <c r="K13" s="116">
         <v>30</v>
       </c>
-      <c r="L13" s="103" t="s">
+      <c r="L13" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="M13" s="102" t="s">
+      <c r="M13" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="N13" s="104" t="s">
+      <c r="N13" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="O13" s="103" t="s">
+      <c r="O13" s="115" t="s">
         <v>42</v>
       </c>
-      <c r="P13" s="103" t="s">
+      <c r="P13" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="Q13" s="103" t="s">
+      <c r="Q13" s="115" t="s">
         <v>53</v>
       </c>
-      <c r="R13" s="103" t="s">
+      <c r="R13" s="115" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="112"/>
+      <c r="A14" s="103"/>
       <c r="B14" s="95"/>
       <c r="C14" s="96"/>
       <c r="D14" s="96"/>
       <c r="E14" s="96"/>
       <c r="F14" s="93"/>
-      <c r="I14" s="102"/>
-      <c r="J14" s="102"/>
-      <c r="K14" s="102"/>
-      <c r="L14" s="103"/>
-      <c r="M14" s="102"/>
-      <c r="N14" s="104"/>
-      <c r="O14" s="103"/>
-      <c r="P14" s="103"/>
-      <c r="Q14" s="103"/>
-      <c r="R14" s="103"/>
+      <c r="I14" s="116"/>
+      <c r="J14" s="116"/>
+      <c r="K14" s="116"/>
+      <c r="L14" s="115"/>
+      <c r="M14" s="116"/>
+      <c r="N14" s="117"/>
+      <c r="O14" s="115"/>
+      <c r="P14" s="115"/>
+      <c r="Q14" s="115"/>
+      <c r="R14" s="115"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="112"/>
+      <c r="A15" s="103"/>
       <c r="B15" s="95"/>
       <c r="C15" s="96"/>
       <c r="D15" s="96"/>
       <c r="E15" s="96"/>
       <c r="F15" s="93"/>
-      <c r="I15" s="102" t="s">
+      <c r="I15" s="116" t="s">
         <v>36</v>
       </c>
-      <c r="J15" s="102">
+      <c r="J15" s="116">
         <v>5</v>
       </c>
-      <c r="K15" s="102">
+      <c r="K15" s="116">
         <v>30</v>
       </c>
-      <c r="L15" s="103" t="s">
+      <c r="L15" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="M15" s="102" t="s">
+      <c r="M15" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="N15" s="104" t="s">
+      <c r="N15" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="O15" s="103" t="s">
+      <c r="O15" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="P15" s="103" t="s">
+      <c r="P15" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="Q15" s="103" t="s">
+      <c r="Q15" s="115" t="s">
         <v>54</v>
       </c>
-      <c r="R15" s="103" t="s">
+      <c r="R15" s="115" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="112"/>
+      <c r="A16" s="103"/>
       <c r="B16" s="95"/>
       <c r="C16" s="96"/>
       <c r="D16" s="96"/>
       <c r="E16" s="96"/>
       <c r="F16" s="93"/>
-      <c r="I16" s="102"/>
-      <c r="J16" s="102"/>
-      <c r="K16" s="102"/>
-      <c r="L16" s="103"/>
-      <c r="M16" s="102"/>
-      <c r="N16" s="104"/>
-      <c r="O16" s="103"/>
-      <c r="P16" s="103"/>
-      <c r="Q16" s="103"/>
-      <c r="R16" s="103"/>
+      <c r="I16" s="116"/>
+      <c r="J16" s="116"/>
+      <c r="K16" s="116"/>
+      <c r="L16" s="115"/>
+      <c r="M16" s="116"/>
+      <c r="N16" s="117"/>
+      <c r="O16" s="115"/>
+      <c r="P16" s="115"/>
+      <c r="Q16" s="115"/>
+      <c r="R16" s="115"/>
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="111" t="s">
+      <c r="A17" s="102" t="s">
         <v>249</v>
       </c>
       <c r="B17" s="95" t="s">
@@ -3271,39 +3274,39 @@
       </c>
       <c r="E17" s="96"/>
       <c r="F17" s="93"/>
-      <c r="I17" s="102" t="s">
+      <c r="I17" s="116" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="102">
+      <c r="J17" s="116">
         <v>1</v>
       </c>
-      <c r="K17" s="102">
+      <c r="K17" s="116">
         <v>6</v>
       </c>
-      <c r="L17" s="103" t="s">
+      <c r="L17" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="M17" s="102" t="s">
+      <c r="M17" s="116" t="s">
         <v>28</v>
       </c>
-      <c r="N17" s="104" t="s">
+      <c r="N17" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="O17" s="103" t="s">
+      <c r="O17" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="P17" s="103" t="s">
+      <c r="P17" s="115" t="s">
         <v>49</v>
       </c>
-      <c r="Q17" s="103" t="s">
+      <c r="Q17" s="115" t="s">
         <v>55</v>
       </c>
-      <c r="R17" s="103" t="s">
+      <c r="R17" s="115" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="112"/>
+      <c r="A18" s="103"/>
       <c r="B18" s="95" t="s">
         <v>241</v>
       </c>
@@ -3315,19 +3318,19 @@
       </c>
       <c r="E18" s="96"/>
       <c r="F18" s="93"/>
-      <c r="I18" s="102"/>
-      <c r="J18" s="102"/>
-      <c r="K18" s="102"/>
-      <c r="L18" s="103"/>
-      <c r="M18" s="102"/>
-      <c r="N18" s="104"/>
-      <c r="O18" s="103"/>
-      <c r="P18" s="103"/>
-      <c r="Q18" s="103"/>
-      <c r="R18" s="103"/>
+      <c r="I18" s="116"/>
+      <c r="J18" s="116"/>
+      <c r="K18" s="116"/>
+      <c r="L18" s="115"/>
+      <c r="M18" s="116"/>
+      <c r="N18" s="117"/>
+      <c r="O18" s="115"/>
+      <c r="P18" s="115"/>
+      <c r="Q18" s="115"/>
+      <c r="R18" s="115"/>
     </row>
     <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="112"/>
+      <c r="A19" s="103"/>
       <c r="B19" s="95" t="s">
         <v>243</v>
       </c>
@@ -3339,39 +3342,39 @@
       </c>
       <c r="E19" s="96"/>
       <c r="F19" s="93"/>
-      <c r="I19" s="102" t="s">
+      <c r="I19" s="116" t="s">
         <v>38</v>
       </c>
-      <c r="J19" s="102">
+      <c r="J19" s="116">
         <v>1</v>
       </c>
-      <c r="K19" s="102">
+      <c r="K19" s="116">
         <v>6</v>
       </c>
-      <c r="L19" s="103" t="s">
+      <c r="L19" s="115" t="s">
         <v>50</v>
       </c>
-      <c r="M19" s="102" t="s">
+      <c r="M19" s="116" t="s">
         <v>28</v>
       </c>
-      <c r="N19" s="104" t="s">
+      <c r="N19" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="O19" s="103" t="s">
+      <c r="O19" s="115" t="s">
         <v>51</v>
       </c>
-      <c r="P19" s="103" t="s">
+      <c r="P19" s="115" t="s">
         <v>52</v>
       </c>
-      <c r="Q19" s="103" t="s">
+      <c r="Q19" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="R19" s="103" t="s">
+      <c r="R19" s="115" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="112"/>
+      <c r="A20" s="103"/>
       <c r="B20" s="95" t="s">
         <v>245</v>
       </c>
@@ -3383,19 +3386,19 @@
       </c>
       <c r="E20" s="96"/>
       <c r="F20" s="93"/>
-      <c r="I20" s="102"/>
-      <c r="J20" s="102"/>
-      <c r="K20" s="102"/>
-      <c r="L20" s="103"/>
-      <c r="M20" s="102"/>
-      <c r="N20" s="104"/>
-      <c r="O20" s="103"/>
-      <c r="P20" s="103"/>
-      <c r="Q20" s="103"/>
-      <c r="R20" s="103"/>
+      <c r="I20" s="116"/>
+      <c r="J20" s="116"/>
+      <c r="K20" s="116"/>
+      <c r="L20" s="115"/>
+      <c r="M20" s="116"/>
+      <c r="N20" s="117"/>
+      <c r="O20" s="115"/>
+      <c r="P20" s="115"/>
+      <c r="Q20" s="115"/>
+      <c r="R20" s="115"/>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="112"/>
+      <c r="A21" s="103"/>
       <c r="B21" s="95" t="s">
         <v>247</v>
       </c>
@@ -3407,57 +3410,57 @@
       </c>
       <c r="E21" s="96"/>
       <c r="F21" s="93"/>
-      <c r="I21" s="102" t="s">
+      <c r="I21" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="J21" s="102">
+      <c r="J21" s="116">
         <v>3</v>
       </c>
-      <c r="K21" s="102">
+      <c r="K21" s="116">
         <v>6</v>
       </c>
-      <c r="L21" s="103" t="s">
+      <c r="L21" s="115" t="s">
         <v>261</v>
       </c>
-      <c r="M21" s="102" t="s">
+      <c r="M21" s="116" t="s">
         <v>28</v>
       </c>
-      <c r="N21" s="104" t="s">
+      <c r="N21" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="O21" s="103" t="s">
+      <c r="O21" s="115" t="s">
         <v>262</v>
       </c>
-      <c r="P21" s="103" t="s">
+      <c r="P21" s="115" t="s">
         <v>263</v>
       </c>
-      <c r="Q21" s="103" t="s">
+      <c r="Q21" s="115" t="s">
         <v>264</v>
       </c>
-      <c r="R21" s="103" t="s">
+      <c r="R21" s="115" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="112"/>
+      <c r="A22" s="103"/>
       <c r="B22" s="95"/>
       <c r="C22" s="96"/>
       <c r="D22" s="96"/>
       <c r="E22" s="96"/>
       <c r="F22" s="93"/>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
-      <c r="K22" s="102"/>
-      <c r="L22" s="103"/>
-      <c r="M22" s="102"/>
-      <c r="N22" s="104"/>
-      <c r="O22" s="103"/>
-      <c r="P22" s="103"/>
-      <c r="Q22" s="103"/>
-      <c r="R22" s="103"/>
+      <c r="I22" s="116"/>
+      <c r="J22" s="116"/>
+      <c r="K22" s="116"/>
+      <c r="L22" s="115"/>
+      <c r="M22" s="116"/>
+      <c r="N22" s="117"/>
+      <c r="O22" s="115"/>
+      <c r="P22" s="115"/>
+      <c r="Q22" s="115"/>
+      <c r="R22" s="115"/>
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="112"/>
+      <c r="A23" s="103"/>
       <c r="B23" s="95"/>
       <c r="C23" s="96"/>
       <c r="D23" s="96"/>
@@ -3465,7 +3468,7 @@
       <c r="F23" s="93"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="112"/>
+      <c r="A24" s="103"/>
       <c r="B24" s="95"/>
       <c r="C24" s="96"/>
       <c r="D24" s="96"/>
@@ -3489,7 +3492,7 @@
       <c r="F25" s="96" t="s">
         <v>265</v>
       </c>
-      <c r="N25" s="102"/>
+      <c r="N25" s="116"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="97" t="s">
@@ -3508,7 +3511,7 @@
       <c r="F26" s="96" t="s">
         <v>265</v>
       </c>
-      <c r="N26" s="102"/>
+      <c r="N26" s="116"/>
     </row>
     <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="97" t="s">
@@ -3690,36 +3693,29 @@
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="A17:A24"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="R17:R18"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="R19:R20"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="R21:R22"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="Q17:Q18"/>
     <mergeCell ref="O21:O22"/>
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="J15:J16"/>
@@ -3734,32 +3730,39 @@
     <mergeCell ref="O15:O16"/>
     <mergeCell ref="O17:O18"/>
     <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="Q17:Q18"/>
     <mergeCell ref="N19:N20"/>
     <mergeCell ref="N21:N22"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="R17:R18"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="R19:R20"/>
-    <mergeCell ref="Q21:Q22"/>
-    <mergeCell ref="R21:R22"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="A17:A24"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3770,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B769BC50-9623-4726-8971-E5FD68E08F76}">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3796,18 +3799,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="140" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
     </row>
     <row r="2" spans="1:19" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
@@ -3828,14 +3831,14 @@
       <c r="F2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="124" t="s">
+      <c r="G2" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="125"/>
-      <c r="I2" s="124" t="s">
+      <c r="H2" s="193"/>
+      <c r="I2" s="192" t="s">
         <v>136</v>
       </c>
-      <c r="J2" s="125"/>
+      <c r="J2" s="193"/>
       <c r="L2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3862,7 +3865,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="194" t="s">
         <v>137</v>
       </c>
       <c r="B3" s="21"/>
@@ -3876,10 +3879,10 @@
         <v>224</v>
       </c>
       <c r="F3" s="21"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="129"/>
-      <c r="J3" s="131"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="198"/>
+      <c r="I3" s="197"/>
+      <c r="J3" s="199"/>
       <c r="L3" s="3" t="s">
         <v>90</v>
       </c>
@@ -3906,7 +3909,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="127"/>
+      <c r="A4" s="195"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23" t="s">
         <v>118</v>
@@ -3918,10 +3921,10 @@
         <v>224</v>
       </c>
       <c r="F4" s="23"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="132"/>
-      <c r="J4" s="134"/>
+      <c r="G4" s="200"/>
+      <c r="H4" s="201"/>
+      <c r="I4" s="200"/>
+      <c r="J4" s="202"/>
       <c r="L4" s="3" t="s">
         <v>91</v>
       </c>
@@ -3948,7 +3951,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="128"/>
+      <c r="A5" s="196"/>
       <c r="B5" s="24"/>
       <c r="C5" s="24" t="s">
         <v>119</v>
@@ -3960,10 +3963,10 @@
         <v>34</v>
       </c>
       <c r="F5" s="24"/>
-      <c r="G5" s="135"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="135"/>
-      <c r="J5" s="137"/>
+      <c r="G5" s="203"/>
+      <c r="H5" s="204"/>
+      <c r="I5" s="203"/>
+      <c r="J5" s="205"/>
       <c r="L5" s="3" t="s">
         <v>95</v>
       </c>
@@ -3990,7 +3993,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="162" t="s">
+      <c r="A6" s="190" t="s">
         <v>140</v>
       </c>
       <c r="B6" s="26"/>
@@ -4006,10 +4009,10 @@
       <c r="F6" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="G6" s="141"/>
-      <c r="H6" s="142"/>
-      <c r="I6" s="141"/>
-      <c r="J6" s="143"/>
+      <c r="G6" s="169"/>
+      <c r="H6" s="170"/>
+      <c r="I6" s="169"/>
+      <c r="J6" s="171"/>
       <c r="L6" s="3" t="s">
         <v>99</v>
       </c>
@@ -4036,7 +4039,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="163"/>
+      <c r="A7" s="191"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28" t="s">
         <v>123</v>
@@ -4050,10 +4053,10 @@
       <c r="F7" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="G7" s="144"/>
-      <c r="H7" s="145"/>
-      <c r="I7" s="144"/>
-      <c r="J7" s="146"/>
+      <c r="G7" s="172"/>
+      <c r="H7" s="173"/>
+      <c r="I7" s="172"/>
+      <c r="J7" s="174"/>
       <c r="L7" s="67" t="s">
         <v>87</v>
       </c>
@@ -4080,7 +4083,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="147" t="s">
+      <c r="A8" s="175" t="s">
         <v>139</v>
       </c>
       <c r="B8" s="29"/>
@@ -4096,10 +4099,10 @@
       <c r="F8" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="G8" s="159"/>
-      <c r="H8" s="161"/>
-      <c r="I8" s="159"/>
-      <c r="J8" s="160"/>
+      <c r="G8" s="187"/>
+      <c r="H8" s="189"/>
+      <c r="I8" s="187"/>
+      <c r="J8" s="188"/>
       <c r="L8" s="3" t="s">
         <v>281</v>
       </c>
@@ -4126,7 +4129,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="148"/>
+      <c r="A9" s="176"/>
       <c r="B9" s="30"/>
       <c r="C9" s="30" t="s">
         <v>123</v>
@@ -4146,7 +4149,7 @@
       <c r="J9" s="71"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="149"/>
+      <c r="A10" s="177"/>
       <c r="B10" s="31"/>
       <c r="C10" s="31" t="s">
         <v>269</v>
@@ -4166,7 +4169,7 @@
       <c r="J10" s="74"/>
     </row>
     <row r="11" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="138" t="s">
+      <c r="A11" s="166" t="s">
         <v>138</v>
       </c>
       <c r="B11" s="32"/>
@@ -4182,13 +4185,13 @@
       <c r="F11" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="G11" s="153"/>
-      <c r="H11" s="154"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="155"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="182"/>
+      <c r="I11" s="181"/>
+      <c r="J11" s="183"/>
     </row>
     <row r="12" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="139"/>
+      <c r="A12" s="167"/>
       <c r="B12" s="33"/>
       <c r="C12" s="33" t="s">
         <v>121</v>
@@ -4202,10 +4205,10 @@
       <c r="F12" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="G12" s="156"/>
-      <c r="H12" s="157"/>
-      <c r="I12" s="156"/>
-      <c r="J12" s="158"/>
+      <c r="G12" s="184"/>
+      <c r="H12" s="185"/>
+      <c r="I12" s="184"/>
+      <c r="J12" s="186"/>
       <c r="L12" s="65"/>
       <c r="M12" s="65"/>
       <c r="N12" s="65"/>
@@ -4216,7 +4219,7 @@
       <c r="S12" s="65"/>
     </row>
     <row r="13" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="140"/>
+      <c r="A13" s="168"/>
       <c r="B13" s="34"/>
       <c r="C13" s="34" t="s">
         <v>122</v>
@@ -4230,10 +4233,10 @@
       <c r="F13" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="G13" s="150"/>
-      <c r="H13" s="151"/>
-      <c r="I13" s="150"/>
-      <c r="J13" s="152"/>
+      <c r="G13" s="178"/>
+      <c r="H13" s="179"/>
+      <c r="I13" s="178"/>
+      <c r="J13" s="180"/>
       <c r="L13" s="66"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
@@ -4244,7 +4247,7 @@
       <c r="S13" s="6"/>
     </row>
     <row r="14" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="192" t="s">
+      <c r="A14" s="126" t="s">
         <v>141</v>
       </c>
       <c r="B14" s="35"/>
@@ -4260,10 +4263,10 @@
       <c r="F14" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="G14" s="164"/>
-      <c r="H14" s="164"/>
-      <c r="I14" s="164"/>
-      <c r="J14" s="164"/>
+      <c r="G14" s="165"/>
+      <c r="H14" s="165"/>
+      <c r="I14" s="165"/>
+      <c r="J14" s="165"/>
       <c r="L14" s="66"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
@@ -4274,7 +4277,7 @@
       <c r="S14" s="6"/>
     </row>
     <row r="15" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="193"/>
+      <c r="A15" s="127"/>
       <c r="B15" s="36"/>
       <c r="C15" s="36" t="s">
         <v>124</v>
@@ -4288,10 +4291,10 @@
       <c r="F15" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="G15" s="165"/>
-      <c r="H15" s="165"/>
-      <c r="I15" s="165"/>
-      <c r="J15" s="165"/>
+      <c r="G15" s="156"/>
+      <c r="H15" s="156"/>
+      <c r="I15" s="156"/>
+      <c r="J15" s="156"/>
       <c r="L15" s="66"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
@@ -4302,7 +4305,7 @@
       <c r="S15" s="6"/>
     </row>
     <row r="16" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="193"/>
+      <c r="A16" s="127"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36" t="s">
         <v>125</v>
@@ -4316,10 +4319,10 @@
       <c r="F16" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="G16" s="165"/>
-      <c r="H16" s="165"/>
-      <c r="I16" s="165"/>
-      <c r="J16" s="165"/>
+      <c r="G16" s="156"/>
+      <c r="H16" s="156"/>
+      <c r="I16" s="156"/>
+      <c r="J16" s="156"/>
       <c r="L16" s="66"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
@@ -4330,7 +4333,7 @@
       <c r="S16" s="6"/>
     </row>
     <row r="17" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="193"/>
+      <c r="A17" s="127"/>
       <c r="B17" s="36"/>
       <c r="C17" s="36" t="s">
         <v>126</v>
@@ -4344,10 +4347,10 @@
       <c r="F17" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="G17" s="165"/>
-      <c r="H17" s="165"/>
-      <c r="I17" s="165"/>
-      <c r="J17" s="165"/>
+      <c r="G17" s="156"/>
+      <c r="H17" s="156"/>
+      <c r="I17" s="156"/>
+      <c r="J17" s="156"/>
       <c r="L17" s="66"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
@@ -4358,7 +4361,7 @@
       <c r="S17" s="6"/>
     </row>
     <row r="18" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="193"/>
+      <c r="A18" s="127"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36" t="s">
         <v>127</v>
@@ -4372,13 +4375,13 @@
       <c r="F18" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="G18" s="165"/>
-      <c r="H18" s="165"/>
-      <c r="I18" s="165"/>
-      <c r="J18" s="165"/>
+      <c r="G18" s="156"/>
+      <c r="H18" s="156"/>
+      <c r="I18" s="156"/>
+      <c r="J18" s="156"/>
     </row>
     <row r="19" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="193"/>
+      <c r="A19" s="127"/>
       <c r="B19" s="36"/>
       <c r="C19" s="36" t="s">
         <v>128</v>
@@ -4392,13 +4395,13 @@
       <c r="F19" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165"/>
-      <c r="J19" s="165"/>
+      <c r="G19" s="156"/>
+      <c r="H19" s="156"/>
+      <c r="I19" s="156"/>
+      <c r="J19" s="156"/>
     </row>
     <row r="20" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="193"/>
+      <c r="A20" s="127"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36" t="s">
         <v>129</v>
@@ -4412,13 +4415,13 @@
       <c r="F20" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165"/>
-      <c r="J20" s="165"/>
+      <c r="G20" s="156"/>
+      <c r="H20" s="156"/>
+      <c r="I20" s="156"/>
+      <c r="J20" s="156"/>
     </row>
     <row r="21" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="194"/>
+      <c r="A21" s="128"/>
       <c r="B21" s="38"/>
       <c r="C21" s="39" t="s">
         <v>130</v>
@@ -4432,13 +4435,13 @@
       <c r="F21" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="G21" s="188"/>
-      <c r="H21" s="188"/>
-      <c r="I21" s="188"/>
-      <c r="J21" s="188"/>
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157"/>
+      <c r="J21" s="157"/>
     </row>
     <row r="22" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="166" t="s">
+      <c r="A22" s="161" t="s">
         <v>142</v>
       </c>
       <c r="B22" s="40"/>
@@ -4454,13 +4457,13 @@
       <c r="F22" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="189"/>
-      <c r="I22" s="172"/>
-      <c r="J22" s="173"/>
+      <c r="G22" s="158"/>
+      <c r="H22" s="159"/>
+      <c r="I22" s="158"/>
+      <c r="J22" s="164"/>
     </row>
     <row r="23" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="167"/>
+      <c r="A23" s="162"/>
       <c r="B23" s="42"/>
       <c r="C23" s="43" t="s">
         <v>124</v>
@@ -4474,13 +4477,13 @@
       <c r="F23" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="G23" s="169"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="169"/>
-      <c r="J23" s="171"/>
+      <c r="G23" s="148"/>
+      <c r="H23" s="160"/>
+      <c r="I23" s="148"/>
+      <c r="J23" s="149"/>
     </row>
     <row r="24" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="167"/>
+      <c r="A24" s="162"/>
       <c r="B24" s="42"/>
       <c r="C24" s="43" t="s">
         <v>125</v>
@@ -4494,13 +4497,13 @@
       <c r="F24" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="G24" s="169"/>
-      <c r="H24" s="170"/>
-      <c r="I24" s="169"/>
-      <c r="J24" s="171"/>
+      <c r="G24" s="148"/>
+      <c r="H24" s="160"/>
+      <c r="I24" s="148"/>
+      <c r="J24" s="149"/>
     </row>
     <row r="25" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="167"/>
+      <c r="A25" s="162"/>
       <c r="B25" s="42"/>
       <c r="C25" s="43" t="s">
         <v>126</v>
@@ -4514,13 +4517,13 @@
       <c r="F25" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="G25" s="169"/>
-      <c r="H25" s="170"/>
-      <c r="I25" s="169"/>
-      <c r="J25" s="171"/>
+      <c r="G25" s="148"/>
+      <c r="H25" s="160"/>
+      <c r="I25" s="148"/>
+      <c r="J25" s="149"/>
     </row>
     <row r="26" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="167"/>
+      <c r="A26" s="162"/>
       <c r="B26" s="42"/>
       <c r="C26" s="43" t="s">
         <v>127</v>
@@ -4534,13 +4537,13 @@
       <c r="F26" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="G26" s="169"/>
-      <c r="H26" s="170"/>
-      <c r="I26" s="169"/>
-      <c r="J26" s="171"/>
+      <c r="G26" s="148"/>
+      <c r="H26" s="160"/>
+      <c r="I26" s="148"/>
+      <c r="J26" s="149"/>
     </row>
     <row r="27" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="167"/>
+      <c r="A27" s="162"/>
       <c r="B27" s="42"/>
       <c r="C27" s="43" t="s">
         <v>128</v>
@@ -4554,13 +4557,13 @@
       <c r="F27" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="G27" s="169"/>
-      <c r="H27" s="170"/>
-      <c r="I27" s="169"/>
-      <c r="J27" s="171"/>
+      <c r="G27" s="148"/>
+      <c r="H27" s="160"/>
+      <c r="I27" s="148"/>
+      <c r="J27" s="149"/>
     </row>
     <row r="28" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="168"/>
+      <c r="A28" s="163"/>
       <c r="B28" s="44"/>
       <c r="C28" s="45" t="s">
         <v>129</v>
@@ -4574,13 +4577,13 @@
       <c r="F28" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="G28" s="182"/>
-      <c r="H28" s="183"/>
-      <c r="I28" s="182"/>
-      <c r="J28" s="184"/>
+      <c r="G28" s="150"/>
+      <c r="H28" s="151"/>
+      <c r="I28" s="150"/>
+      <c r="J28" s="152"/>
     </row>
     <row r="29" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="195" t="s">
+      <c r="A29" s="129" t="s">
         <v>145</v>
       </c>
       <c r="B29" s="46"/>
@@ -4596,13 +4599,13 @@
       <c r="F29" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="G29" s="185"/>
-      <c r="H29" s="186"/>
-      <c r="I29" s="185"/>
-      <c r="J29" s="187"/>
+      <c r="G29" s="153"/>
+      <c r="H29" s="154"/>
+      <c r="I29" s="153"/>
+      <c r="J29" s="155"/>
     </row>
     <row r="30" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="196"/>
+      <c r="A30" s="130"/>
       <c r="B30" s="47"/>
       <c r="C30" s="48" t="s">
         <v>143</v>
@@ -4616,10 +4619,10 @@
       <c r="F30" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="G30" s="176"/>
-      <c r="H30" s="177"/>
-      <c r="I30" s="176"/>
-      <c r="J30" s="178"/>
+      <c r="G30" s="142"/>
+      <c r="H30" s="143"/>
+      <c r="I30" s="142"/>
+      <c r="J30" s="144"/>
     </row>
     <row r="31" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="75" t="s">
@@ -4638,10 +4641,10 @@
       <c r="F31" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="G31" s="179"/>
-      <c r="H31" s="180"/>
-      <c r="I31" s="179"/>
-      <c r="J31" s="181"/>
+      <c r="G31" s="145"/>
+      <c r="H31" s="146"/>
+      <c r="I31" s="145"/>
+      <c r="J31" s="147"/>
     </row>
     <row r="32" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="53" t="s">
@@ -4662,10 +4665,10 @@
       <c r="F32" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="G32" s="200"/>
-      <c r="H32" s="201"/>
-      <c r="I32" s="200"/>
-      <c r="J32" s="202"/>
+      <c r="G32" s="134"/>
+      <c r="H32" s="135"/>
+      <c r="I32" s="134"/>
+      <c r="J32" s="136"/>
     </row>
     <row r="33" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="53" t="s">
@@ -4686,10 +4689,10 @@
       <c r="F33" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="G33" s="203"/>
-      <c r="H33" s="204"/>
-      <c r="I33" s="203"/>
-      <c r="J33" s="205"/>
+      <c r="G33" s="137"/>
+      <c r="H33" s="138"/>
+      <c r="I33" s="137"/>
+      <c r="J33" s="139"/>
     </row>
     <row r="34" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="53" t="s">
@@ -4710,10 +4713,10 @@
       <c r="F34" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="G34" s="197"/>
-      <c r="H34" s="198"/>
-      <c r="I34" s="197"/>
-      <c r="J34" s="199"/>
+      <c r="G34" s="131"/>
+      <c r="H34" s="132"/>
+      <c r="I34" s="131"/>
+      <c r="J34" s="133"/>
     </row>
     <row r="35" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="79" t="s">
@@ -4734,10 +4737,10 @@
       <c r="F35" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="G35" s="197"/>
-      <c r="H35" s="198"/>
-      <c r="I35" s="197"/>
-      <c r="J35" s="199"/>
+      <c r="G35" s="131"/>
+      <c r="H35" s="132"/>
+      <c r="I35" s="131"/>
+      <c r="J35" s="133"/>
     </row>
     <row r="36" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="77" t="s">
@@ -4758,10 +4761,10 @@
       <c r="F36" s="55" t="s">
         <v>157</v>
       </c>
-      <c r="G36" s="190"/>
-      <c r="H36" s="190"/>
-      <c r="I36" s="190"/>
-      <c r="J36" s="191"/>
+      <c r="G36" s="124"/>
+      <c r="H36" s="124"/>
+      <c r="I36" s="124"/>
+      <c r="J36" s="125"/>
     </row>
     <row r="37" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="57" t="s">
@@ -4782,10 +4785,10 @@
       <c r="F37" s="55" t="s">
         <v>157</v>
       </c>
-      <c r="G37" s="190"/>
-      <c r="H37" s="190"/>
-      <c r="I37" s="190"/>
-      <c r="J37" s="191"/>
+      <c r="G37" s="124"/>
+      <c r="H37" s="124"/>
+      <c r="I37" s="124"/>
+      <c r="J37" s="125"/>
     </row>
     <row r="38" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A38" s="58" t="s">
@@ -4806,17 +4809,17 @@
       <c r="F38" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="G38" s="190"/>
-      <c r="H38" s="190"/>
-      <c r="I38" s="190"/>
-      <c r="J38" s="191"/>
+      <c r="G38" s="124"/>
+      <c r="H38" s="124"/>
+      <c r="I38" s="124"/>
+      <c r="J38" s="125"/>
     </row>
     <row r="39" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A39" s="42" t="s">
         <v>156</v>
       </c>
       <c r="B39" s="42" t="s">
-        <v>154</v>
+        <v>307</v>
       </c>
       <c r="C39" s="42"/>
       <c r="D39" s="42" t="s">
@@ -4872,7 +4875,7 @@
     <row r="42" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A42" s="12"/>
       <c r="B42" s="79" t="s">
-        <v>152</v>
+        <v>307</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -4899,9 +4902,7 @@
     </row>
     <row r="44" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A44" s="12"/>
-      <c r="B44" s="79" t="s">
-        <v>154</v>
-      </c>
+      <c r="B44" s="79"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -4937,6 +4938,68 @@
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G27:H27"/>
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="I37:J37"/>
@@ -4953,68 +5016,6 @@
     <mergeCell ref="I33:J33"/>
     <mergeCell ref="G35:H35"/>
     <mergeCell ref="I35:J35"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5051,14 +5052,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="104" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -5079,14 +5080,14 @@
       <c r="F2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="211" t="s">
+      <c r="G2" s="207" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="211"/>
-      <c r="I2" s="211" t="s">
+      <c r="H2" s="207"/>
+      <c r="I2" s="207" t="s">
         <v>136</v>
       </c>
-      <c r="J2" s="211"/>
+      <c r="J2" s="207"/>
       <c r="N2" t="s">
         <v>62</v>
       </c>
@@ -5099,7 +5100,7 @@
       <c r="U2" s="6"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="212" t="s">
+      <c r="A3" s="206" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="10"/>
@@ -5113,10 +5114,10 @@
         <v>224</v>
       </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="206"/>
-      <c r="H3" s="207"/>
-      <c r="I3" s="206"/>
-      <c r="J3" s="207"/>
+      <c r="G3" s="208"/>
+      <c r="H3" s="209"/>
+      <c r="I3" s="208"/>
+      <c r="J3" s="209"/>
       <c r="N3" s="19" t="s">
         <v>17</v>
       </c>
@@ -5143,7 +5144,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="212"/>
+      <c r="A4" s="206"/>
       <c r="B4" s="10"/>
       <c r="C4" s="80" t="s">
         <v>276</v>
@@ -5155,10 +5156,10 @@
         <v>224</v>
       </c>
       <c r="F4" s="10"/>
-      <c r="G4" s="206"/>
-      <c r="H4" s="207"/>
-      <c r="I4" s="206"/>
-      <c r="J4" s="207"/>
+      <c r="G4" s="208"/>
+      <c r="H4" s="209"/>
+      <c r="I4" s="208"/>
+      <c r="J4" s="209"/>
       <c r="N4" s="7" t="s">
         <v>63</v>
       </c>
@@ -5185,7 +5186,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="212"/>
+      <c r="A5" s="206"/>
       <c r="B5" s="10"/>
       <c r="C5" s="80" t="s">
         <v>119</v>
@@ -5197,10 +5198,10 @@
         <v>7</v>
       </c>
       <c r="F5" s="10"/>
-      <c r="G5" s="206"/>
-      <c r="H5" s="207"/>
-      <c r="I5" s="206"/>
-      <c r="J5" s="207"/>
+      <c r="G5" s="208"/>
+      <c r="H5" s="209"/>
+      <c r="I5" s="208"/>
+      <c r="J5" s="209"/>
       <c r="N5" s="7" t="s">
         <v>67</v>
       </c>
@@ -5227,7 +5228,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="212" t="s">
+      <c r="A6" s="206" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="10"/>
@@ -5243,10 +5244,10 @@
       <c r="F6" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G6" s="206"/>
-      <c r="H6" s="207"/>
-      <c r="I6" s="206"/>
-      <c r="J6" s="207"/>
+      <c r="G6" s="208"/>
+      <c r="H6" s="209"/>
+      <c r="I6" s="208"/>
+      <c r="J6" s="209"/>
       <c r="N6" s="7" t="s">
         <v>71</v>
       </c>
@@ -5273,7 +5274,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="212"/>
+      <c r="A7" s="206"/>
       <c r="B7" s="10"/>
       <c r="C7" s="80" t="s">
         <v>123</v>
@@ -5287,10 +5288,10 @@
       <c r="F7" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G7" s="206"/>
-      <c r="H7" s="207"/>
-      <c r="I7" s="206"/>
-      <c r="J7" s="207"/>
+      <c r="G7" s="208"/>
+      <c r="H7" s="209"/>
+      <c r="I7" s="208"/>
+      <c r="J7" s="209"/>
       <c r="N7" s="7" t="s">
         <v>75</v>
       </c>
@@ -5317,7 +5318,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="212" t="s">
+      <c r="A8" s="206" t="s">
         <v>104</v>
       </c>
       <c r="B8" s="10"/>
@@ -5333,10 +5334,10 @@
       <c r="F8" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G8" s="206"/>
-      <c r="H8" s="207"/>
-      <c r="I8" s="206"/>
-      <c r="J8" s="207"/>
+      <c r="G8" s="208"/>
+      <c r="H8" s="209"/>
+      <c r="I8" s="208"/>
+      <c r="J8" s="209"/>
       <c r="N8" s="13" t="s">
         <v>79</v>
       </c>
@@ -5363,7 +5364,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="212"/>
+      <c r="A9" s="206"/>
       <c r="B9" s="10"/>
       <c r="C9" s="80" t="s">
         <v>123</v>
@@ -5377,10 +5378,10 @@
       <c r="F9" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G9" s="206"/>
-      <c r="H9" s="207"/>
-      <c r="I9" s="206"/>
-      <c r="J9" s="207"/>
+      <c r="G9" s="208"/>
+      <c r="H9" s="209"/>
+      <c r="I9" s="208"/>
+      <c r="J9" s="209"/>
       <c r="L9" s="15"/>
       <c r="M9" s="16"/>
       <c r="N9" s="17" t="s">
@@ -5409,7 +5410,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="212"/>
+      <c r="A10" s="206"/>
       <c r="B10" s="10"/>
       <c r="C10" s="80" t="s">
         <v>269</v>
@@ -5423,13 +5424,13 @@
       <c r="F10" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G10" s="206"/>
-      <c r="H10" s="207"/>
-      <c r="I10" s="206"/>
-      <c r="J10" s="207"/>
+      <c r="G10" s="208"/>
+      <c r="H10" s="209"/>
+      <c r="I10" s="208"/>
+      <c r="J10" s="209"/>
     </row>
     <row r="11" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="212" t="s">
+      <c r="A11" s="206" t="s">
         <v>105</v>
       </c>
       <c r="B11" s="10"/>
@@ -5445,13 +5446,13 @@
       <c r="F11" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G11" s="206"/>
-      <c r="H11" s="207"/>
-      <c r="I11" s="206"/>
-      <c r="J11" s="207"/>
+      <c r="G11" s="208"/>
+      <c r="H11" s="209"/>
+      <c r="I11" s="208"/>
+      <c r="J11" s="209"/>
     </row>
     <row r="12" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="212"/>
+      <c r="A12" s="206"/>
       <c r="B12" s="10"/>
       <c r="C12" s="9" t="s">
         <v>121</v>
@@ -5465,13 +5466,13 @@
       <c r="F12" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G12" s="206"/>
-      <c r="H12" s="207"/>
-      <c r="I12" s="206"/>
-      <c r="J12" s="207"/>
+      <c r="G12" s="208"/>
+      <c r="H12" s="209"/>
+      <c r="I12" s="208"/>
+      <c r="J12" s="209"/>
     </row>
     <row r="13" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="212"/>
+      <c r="A13" s="206"/>
       <c r="B13" s="10"/>
       <c r="C13" s="9" t="s">
         <v>122</v>
@@ -5485,10 +5486,10 @@
       <c r="F13" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G13" s="206"/>
-      <c r="H13" s="207"/>
-      <c r="I13" s="206"/>
-      <c r="J13" s="207"/>
+      <c r="G13" s="208"/>
+      <c r="H13" s="209"/>
+      <c r="I13" s="208"/>
+      <c r="J13" s="209"/>
     </row>
     <row r="14" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="213" t="s">
@@ -5507,10 +5508,10 @@
       <c r="F14" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G14" s="206"/>
-      <c r="H14" s="207"/>
-      <c r="I14" s="206"/>
-      <c r="J14" s="207"/>
+      <c r="G14" s="208"/>
+      <c r="H14" s="209"/>
+      <c r="I14" s="208"/>
+      <c r="J14" s="209"/>
     </row>
     <row r="15" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="214"/>
@@ -5527,10 +5528,10 @@
       <c r="F15" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G15" s="206"/>
-      <c r="H15" s="207"/>
-      <c r="I15" s="206"/>
-      <c r="J15" s="207"/>
+      <c r="G15" s="208"/>
+      <c r="H15" s="209"/>
+      <c r="I15" s="208"/>
+      <c r="J15" s="209"/>
     </row>
     <row r="16" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="214"/>
@@ -5547,10 +5548,10 @@
       <c r="F16" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G16" s="206"/>
-      <c r="H16" s="207"/>
-      <c r="I16" s="206"/>
-      <c r="J16" s="207"/>
+      <c r="G16" s="208"/>
+      <c r="H16" s="209"/>
+      <c r="I16" s="208"/>
+      <c r="J16" s="209"/>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="214"/>
@@ -5567,10 +5568,10 @@
       <c r="F17" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G17" s="206"/>
-      <c r="H17" s="207"/>
-      <c r="I17" s="206"/>
-      <c r="J17" s="207"/>
+      <c r="G17" s="208"/>
+      <c r="H17" s="209"/>
+      <c r="I17" s="208"/>
+      <c r="J17" s="209"/>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="214"/>
@@ -5587,10 +5588,10 @@
       <c r="F18" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G18" s="206"/>
-      <c r="H18" s="207"/>
-      <c r="I18" s="206"/>
-      <c r="J18" s="207"/>
+      <c r="G18" s="208"/>
+      <c r="H18" s="209"/>
+      <c r="I18" s="208"/>
+      <c r="J18" s="209"/>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="214"/>
@@ -5607,10 +5608,10 @@
       <c r="F19" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G19" s="206"/>
-      <c r="H19" s="207"/>
-      <c r="I19" s="206"/>
-      <c r="J19" s="207"/>
+      <c r="G19" s="208"/>
+      <c r="H19" s="209"/>
+      <c r="I19" s="208"/>
+      <c r="J19" s="209"/>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="215"/>
@@ -5627,13 +5628,13 @@
       <c r="F20" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G20" s="206"/>
-      <c r="H20" s="207"/>
-      <c r="I20" s="206"/>
-      <c r="J20" s="207"/>
+      <c r="G20" s="208"/>
+      <c r="H20" s="209"/>
+      <c r="I20" s="208"/>
+      <c r="J20" s="209"/>
     </row>
     <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="208" t="s">
+      <c r="A21" s="210" t="s">
         <v>107</v>
       </c>
       <c r="B21" s="12"/>
@@ -5649,13 +5650,13 @@
       <c r="F21" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G21" s="206"/>
-      <c r="H21" s="207"/>
-      <c r="I21" s="206"/>
-      <c r="J21" s="207"/>
+      <c r="G21" s="208"/>
+      <c r="H21" s="209"/>
+      <c r="I21" s="208"/>
+      <c r="J21" s="209"/>
     </row>
     <row r="22" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="209"/>
+      <c r="A22" s="211"/>
       <c r="B22" s="12"/>
       <c r="C22" s="9" t="s">
         <v>124</v>
@@ -5669,13 +5670,13 @@
       <c r="F22" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G22" s="206"/>
-      <c r="H22" s="207"/>
-      <c r="I22" s="206"/>
-      <c r="J22" s="207"/>
+      <c r="G22" s="208"/>
+      <c r="H22" s="209"/>
+      <c r="I22" s="208"/>
+      <c r="J22" s="209"/>
     </row>
     <row r="23" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="209"/>
+      <c r="A23" s="211"/>
       <c r="B23" s="12"/>
       <c r="C23" s="9" t="s">
         <v>125</v>
@@ -5689,13 +5690,13 @@
       <c r="F23" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G23" s="206"/>
-      <c r="H23" s="207"/>
-      <c r="I23" s="206"/>
-      <c r="J23" s="207"/>
+      <c r="G23" s="208"/>
+      <c r="H23" s="209"/>
+      <c r="I23" s="208"/>
+      <c r="J23" s="209"/>
     </row>
     <row r="24" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="209"/>
+      <c r="A24" s="211"/>
       <c r="B24" s="12"/>
       <c r="C24" s="9" t="s">
         <v>126</v>
@@ -5709,13 +5710,13 @@
       <c r="F24" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G24" s="206"/>
-      <c r="H24" s="207"/>
-      <c r="I24" s="206"/>
-      <c r="J24" s="207"/>
+      <c r="G24" s="208"/>
+      <c r="H24" s="209"/>
+      <c r="I24" s="208"/>
+      <c r="J24" s="209"/>
     </row>
     <row r="25" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="209"/>
+      <c r="A25" s="211"/>
       <c r="B25" s="12"/>
       <c r="C25" s="9" t="s">
         <v>127</v>
@@ -5729,13 +5730,13 @@
       <c r="F25" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G25" s="206"/>
-      <c r="H25" s="207"/>
-      <c r="I25" s="206"/>
-      <c r="J25" s="207"/>
+      <c r="G25" s="208"/>
+      <c r="H25" s="209"/>
+      <c r="I25" s="208"/>
+      <c r="J25" s="209"/>
     </row>
     <row r="26" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="209"/>
+      <c r="A26" s="211"/>
       <c r="B26" s="12"/>
       <c r="C26" s="9" t="s">
         <v>128</v>
@@ -5749,13 +5750,13 @@
       <c r="F26" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G26" s="206"/>
-      <c r="H26" s="207"/>
-      <c r="I26" s="206"/>
-      <c r="J26" s="207"/>
+      <c r="G26" s="208"/>
+      <c r="H26" s="209"/>
+      <c r="I26" s="208"/>
+      <c r="J26" s="209"/>
     </row>
     <row r="27" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="209"/>
+      <c r="A27" s="211"/>
       <c r="B27" s="12"/>
       <c r="C27" s="9" t="s">
         <v>129</v>
@@ -5769,13 +5770,13 @@
       <c r="F27" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G27" s="206"/>
-      <c r="H27" s="207"/>
-      <c r="I27" s="206"/>
-      <c r="J27" s="207"/>
+      <c r="G27" s="208"/>
+      <c r="H27" s="209"/>
+      <c r="I27" s="208"/>
+      <c r="J27" s="209"/>
     </row>
     <row r="28" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="210"/>
+      <c r="A28" s="212"/>
       <c r="B28" s="12"/>
       <c r="C28" s="9" t="s">
         <v>130</v>
@@ -5789,10 +5790,10 @@
       <c r="F28" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G28" s="206"/>
-      <c r="H28" s="207"/>
-      <c r="I28" s="206"/>
-      <c r="J28" s="207"/>
+      <c r="G28" s="208"/>
+      <c r="H28" s="209"/>
+      <c r="I28" s="208"/>
+      <c r="J28" s="209"/>
     </row>
     <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -5811,10 +5812,10 @@
       <c r="F29" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G29" s="206"/>
-      <c r="H29" s="207"/>
-      <c r="I29" s="206"/>
-      <c r="J29" s="207"/>
+      <c r="G29" s="208"/>
+      <c r="H29" s="209"/>
+      <c r="I29" s="208"/>
+      <c r="J29" s="209"/>
     </row>
     <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -5833,10 +5834,10 @@
       <c r="F30" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="G30" s="206"/>
-      <c r="H30" s="207"/>
-      <c r="I30" s="206"/>
-      <c r="J30" s="207"/>
+      <c r="G30" s="208"/>
+      <c r="H30" s="209"/>
+      <c r="I30" s="208"/>
+      <c r="J30" s="209"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -5857,10 +5858,10 @@
       <c r="F31" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="G31" s="206"/>
-      <c r="H31" s="207"/>
-      <c r="I31" s="206"/>
-      <c r="J31" s="207"/>
+      <c r="G31" s="208"/>
+      <c r="H31" s="209"/>
+      <c r="I31" s="208"/>
+      <c r="J31" s="209"/>
     </row>
     <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -5881,10 +5882,10 @@
       <c r="F32" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="G32" s="206"/>
-      <c r="H32" s="207"/>
-      <c r="I32" s="206"/>
-      <c r="J32" s="207"/>
+      <c r="G32" s="208"/>
+      <c r="H32" s="209"/>
+      <c r="I32" s="208"/>
+      <c r="J32" s="209"/>
     </row>
     <row r="33" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -5905,10 +5906,10 @@
       <c r="F33" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="G33" s="206"/>
-      <c r="H33" s="207"/>
-      <c r="I33" s="206"/>
-      <c r="J33" s="207"/>
+      <c r="G33" s="208"/>
+      <c r="H33" s="209"/>
+      <c r="I33" s="208"/>
+      <c r="J33" s="209"/>
     </row>
     <row r="34" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -5929,10 +5930,10 @@
       <c r="F34" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="G34" s="206"/>
-      <c r="H34" s="207"/>
-      <c r="I34" s="206"/>
-      <c r="J34" s="207"/>
+      <c r="G34" s="208"/>
+      <c r="H34" s="209"/>
+      <c r="I34" s="208"/>
+      <c r="J34" s="209"/>
     </row>
     <row r="35" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -5953,10 +5954,10 @@
       <c r="F35" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="G35" s="206"/>
-      <c r="H35" s="207"/>
-      <c r="I35" s="206"/>
-      <c r="J35" s="207"/>
+      <c r="G35" s="208"/>
+      <c r="H35" s="209"/>
+      <c r="I35" s="208"/>
+      <c r="J35" s="209"/>
     </row>
     <row r="36" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -5977,10 +5978,10 @@
       <c r="F36" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="G36" s="206"/>
-      <c r="H36" s="207"/>
-      <c r="I36" s="206"/>
-      <c r="J36" s="207"/>
+      <c r="G36" s="208"/>
+      <c r="H36" s="209"/>
+      <c r="I36" s="208"/>
+      <c r="J36" s="209"/>
     </row>
     <row r="37" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -5993,10 +5994,10 @@
       <c r="F37" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G37" s="206"/>
-      <c r="H37" s="207"/>
-      <c r="I37" s="206"/>
-      <c r="J37" s="207"/>
+      <c r="G37" s="208"/>
+      <c r="H37" s="209"/>
+      <c r="I37" s="208"/>
+      <c r="J37" s="209"/>
     </row>
     <row r="38" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -6009,10 +6010,10 @@
       <c r="F38" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G38" s="206"/>
-      <c r="H38" s="207"/>
-      <c r="I38" s="206"/>
-      <c r="J38" s="207"/>
+      <c r="G38" s="208"/>
+      <c r="H38" s="209"/>
+      <c r="I38" s="208"/>
+      <c r="J38" s="209"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
@@ -6023,19 +6024,74 @@
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="206"/>
-      <c r="H39" s="207"/>
-      <c r="I39" s="206"/>
-      <c r="J39" s="207"/>
+      <c r="G39" s="208"/>
+      <c r="H39" s="209"/>
+      <c r="I39" s="208"/>
+      <c r="J39" s="209"/>
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
     <mergeCell ref="A21:A28"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="G3:H3"/>
@@ -6052,67 +6108,12 @@
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A20"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="G9:H9"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
switchek, vlanok beállítása, etherchannel
</commit_message>
<xml_diff>
--- a/IP_cim_kiosztas.xlsx
+++ b/IP_cim_kiosztas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tibi\Documents\GitHub\Uzemelteto_vizsgaremek_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Üzemeltető\vizsgaremek\Uzemelteto_vizsgaremek_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41862206-BEF5-4FEB-911D-8ACA0433E1A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFAEF53-5610-4E2B-98B4-4FAE1133DBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21975" windowHeight="14130" xr2:uid="{5DEB228F-9A24-4144-85FF-8E6948A8BA71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5DEB228F-9A24-4144-85FF-8E6948A8BA71}"/>
   </bookViews>
   <sheets>
     <sheet name="Központi Iroda" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="309">
   <si>
     <t>Központi Iroda</t>
   </si>
@@ -627,9 +627,6 @@
     <t>192.168.0.76</t>
   </si>
   <si>
-    <t>192.168.0.178</t>
-  </si>
-  <si>
     <t>192.168.0.77</t>
   </si>
   <si>
@@ -956,6 +953,15 @@
   </si>
   <si>
     <t>Gyor_WiFi2</t>
+  </si>
+  <si>
+    <t>G0</t>
+  </si>
+  <si>
+    <t>192.168.0.78</t>
+  </si>
+  <si>
+    <t>192.168.0.79</t>
   </si>
 </sst>
 </file>
@@ -1892,7 +1898,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="215">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2147,71 +2153,42 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2238,7 +2215,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2247,154 +2224,79 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2421,6 +2323,12 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2439,59 +2347,161 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2507,12 +2517,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2854,10 +2858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00720853-46FD-4EE1-97EA-B1AFFEF5B41E}">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2880,21 +2884,21 @@
     <col min="18" max="18" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="113" t="s">
+    <row r="1" spans="1:18" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="115" t="s">
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+    </row>
+    <row r="2" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="106" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="60" t="s">
@@ -2903,823 +2907,801 @@
       <c r="D2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="122" t="s">
+      <c r="E2" s="111" t="s">
         <v>57</v>
       </c>
       <c r="F2" s="61" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="116"/>
-      <c r="B3" s="118"/>
-      <c r="C3" s="119" t="s">
+    <row r="3" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="105"/>
+      <c r="B3" s="107"/>
+      <c r="C3" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="120"/>
-      <c r="E3" s="123"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="112"/>
       <c r="F3" s="62" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="112" t="s">
-        <v>221</v>
-      </c>
-      <c r="B4" s="90" t="s">
+    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="101" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="88" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="89"/>
+    </row>
+    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="101"/>
+      <c r="B5" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="91"/>
-    </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="112"/>
-      <c r="B5" s="92" t="s">
+      <c r="C5" s="92" t="s">
+        <v>278</v>
+      </c>
+      <c r="D5" s="92" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="92"/>
+      <c r="F5" s="18"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
+    </row>
+    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="101"/>
+      <c r="B6" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C5" s="96" t="s">
+      <c r="C6" s="92" t="s">
         <v>279</v>
       </c>
-      <c r="D5" s="96" t="s">
-        <v>224</v>
-      </c>
-      <c r="E5" s="96"/>
-      <c r="F5" s="93"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="87"/>
-      <c r="M5" s="87"/>
-      <c r="N5" s="87"/>
-      <c r="O5" s="87"/>
-      <c r="P5" s="87"/>
-      <c r="Q5" s="87"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="86"/>
-    </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="112"/>
-      <c r="B6" s="92" t="s">
+      <c r="D6" s="92" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" s="92"/>
+      <c r="F6" s="18"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65"/>
+    </row>
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="100" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="90"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="65"/>
+    </row>
+    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="110"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="86"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="65"/>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="65"/>
+    </row>
+    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="100" t="s">
         <v>237</v>
       </c>
-      <c r="C6" s="96" t="s">
-        <v>280</v>
-      </c>
-      <c r="D6" s="96" t="s">
-        <v>224</v>
-      </c>
-      <c r="E6" s="96"/>
-      <c r="F6" s="93"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88"/>
-      <c r="L6" s="87"/>
-      <c r="M6" s="88"/>
-      <c r="N6" s="89"/>
-      <c r="O6" s="87"/>
-      <c r="P6" s="87"/>
-      <c r="Q6" s="87"/>
-      <c r="R6" s="86"/>
-      <c r="S6" s="86"/>
-    </row>
-    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="111" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="96"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="88"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="88"/>
-      <c r="N7" s="89"/>
-      <c r="O7" s="87"/>
-      <c r="P7" s="87"/>
-      <c r="Q7" s="87"/>
-      <c r="R7" s="86"/>
-      <c r="S7" s="86"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="121"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="87"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="89"/>
-      <c r="O8" s="87"/>
-      <c r="P8" s="87"/>
-      <c r="Q8" s="87"/>
-      <c r="R8" s="86"/>
-      <c r="S8" s="86"/>
-    </row>
-    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="111" t="s">
+      <c r="B9" s="91" t="s">
         <v>238</v>
       </c>
-      <c r="B9" s="95" t="s">
+      <c r="C9" s="92" t="s">
         <v>239</v>
       </c>
-      <c r="C9" s="96" t="s">
+      <c r="D9" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="92"/>
+      <c r="F9" s="18"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="65"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65"/>
+    </row>
+    <row r="10" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="101"/>
+      <c r="B10" s="91" t="s">
         <v>240</v>
       </c>
-      <c r="D9" s="96" t="s">
+      <c r="C10" s="92" t="s">
+        <v>241</v>
+      </c>
+      <c r="D10" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="96"/>
-      <c r="F9" s="93"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="88"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="88"/>
-      <c r="L9" s="87"/>
-      <c r="M9" s="88"/>
-      <c r="N9" s="89"/>
-      <c r="O9" s="87"/>
-      <c r="P9" s="87"/>
-      <c r="Q9" s="87"/>
-      <c r="R9" s="86"/>
-      <c r="S9" s="86"/>
-    </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="112"/>
-      <c r="B10" s="95" t="s">
-        <v>241</v>
-      </c>
-      <c r="C10" s="96" t="s">
+      <c r="E10" s="92"/>
+      <c r="F10" s="18"/>
+    </row>
+    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="101"/>
+      <c r="B11" s="91" t="s">
         <v>242</v>
       </c>
-      <c r="D10" s="96" t="s">
+      <c r="C11" s="92" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="92"/>
+      <c r="F11" s="18"/>
+      <c r="I11" s="116" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="118" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="118" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="118" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="118" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="118" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="118" t="s">
+        <v>23</v>
+      </c>
+      <c r="P11" s="118" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11" s="118" t="s">
+        <v>57</v>
+      </c>
+      <c r="R11" s="120" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="101"/>
+      <c r="B12" s="91" t="s">
+        <v>244</v>
+      </c>
+      <c r="C12" s="92" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="92"/>
+      <c r="F12" s="18"/>
+      <c r="I12" s="117"/>
+      <c r="J12" s="119"/>
+      <c r="K12" s="119"/>
+      <c r="L12" s="119"/>
+      <c r="M12" s="119"/>
+      <c r="N12" s="119"/>
+      <c r="O12" s="119"/>
+      <c r="P12" s="119"/>
+      <c r="Q12" s="119"/>
+      <c r="R12" s="121"/>
+    </row>
+    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="101"/>
+      <c r="B13" s="91" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" s="92" t="s">
+        <v>247</v>
+      </c>
+      <c r="D13" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="92"/>
+      <c r="F13" s="18"/>
+      <c r="I13" s="114" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="114">
+        <v>7</v>
+      </c>
+      <c r="K13" s="114">
+        <v>30</v>
+      </c>
+      <c r="L13" s="113" t="s">
+        <v>41</v>
+      </c>
+      <c r="M13" s="114" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="115" t="s">
+        <v>40</v>
+      </c>
+      <c r="O13" s="113" t="s">
+        <v>42</v>
+      </c>
+      <c r="P13" s="113" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q13" s="113" t="s">
+        <v>53</v>
+      </c>
+      <c r="R13" s="113" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="101"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="18"/>
+      <c r="I14" s="114"/>
+      <c r="J14" s="114"/>
+      <c r="K14" s="114"/>
+      <c r="L14" s="113"/>
+      <c r="M14" s="114"/>
+      <c r="N14" s="115"/>
+      <c r="O14" s="113"/>
+      <c r="P14" s="113"/>
+      <c r="Q14" s="113"/>
+      <c r="R14" s="113"/>
+    </row>
+    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="101"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="18"/>
+      <c r="I15" s="114" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="114">
+        <v>5</v>
+      </c>
+      <c r="K15" s="114">
+        <v>30</v>
+      </c>
+      <c r="L15" s="113" t="s">
+        <v>44</v>
+      </c>
+      <c r="M15" s="114" t="s">
+        <v>33</v>
+      </c>
+      <c r="N15" s="115" t="s">
+        <v>40</v>
+      </c>
+      <c r="O15" s="113" t="s">
+        <v>45</v>
+      </c>
+      <c r="P15" s="113" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q15" s="113" t="s">
+        <v>54</v>
+      </c>
+      <c r="R15" s="113" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="101"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="18"/>
+      <c r="I16" s="114"/>
+      <c r="J16" s="114"/>
+      <c r="K16" s="114"/>
+      <c r="L16" s="113"/>
+      <c r="M16" s="114"/>
+      <c r="N16" s="115"/>
+      <c r="O16" s="113"/>
+      <c r="P16" s="113"/>
+      <c r="Q16" s="113"/>
+      <c r="R16" s="113"/>
+    </row>
+    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="100" t="s">
+        <v>248</v>
+      </c>
+      <c r="B17" s="91" t="s">
+        <v>238</v>
+      </c>
+      <c r="C17" s="92" t="s">
+        <v>249</v>
+      </c>
+      <c r="D17" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="96"/>
-      <c r="F10" s="93"/>
-    </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="112"/>
-      <c r="B11" s="95" t="s">
-        <v>243</v>
-      </c>
-      <c r="C11" s="96" t="s">
+      <c r="E17" s="92"/>
+      <c r="F17" s="18"/>
+      <c r="I17" s="114" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" s="114">
+        <v>1</v>
+      </c>
+      <c r="K17" s="114">
+        <v>6</v>
+      </c>
+      <c r="L17" s="113" t="s">
+        <v>47</v>
+      </c>
+      <c r="M17" s="114" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" s="115" t="s">
+        <v>39</v>
+      </c>
+      <c r="O17" s="113" t="s">
+        <v>48</v>
+      </c>
+      <c r="P17" s="113" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q17" s="113" t="s">
+        <v>55</v>
+      </c>
+      <c r="R17" s="113" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="101"/>
+      <c r="B18" s="91" t="s">
+        <v>240</v>
+      </c>
+      <c r="C18" s="92" t="s">
+        <v>250</v>
+      </c>
+      <c r="D18" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="92"/>
+      <c r="F18" s="18"/>
+      <c r="I18" s="114"/>
+      <c r="J18" s="114"/>
+      <c r="K18" s="114"/>
+      <c r="L18" s="113"/>
+      <c r="M18" s="114"/>
+      <c r="N18" s="115"/>
+      <c r="O18" s="113"/>
+      <c r="P18" s="113"/>
+      <c r="Q18" s="113"/>
+      <c r="R18" s="113"/>
+    </row>
+    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="101"/>
+      <c r="B19" s="91" t="s">
+        <v>242</v>
+      </c>
+      <c r="C19" s="92" t="s">
+        <v>251</v>
+      </c>
+      <c r="D19" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="92"/>
+      <c r="F19" s="18"/>
+      <c r="I19" s="114" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="114">
+        <v>1</v>
+      </c>
+      <c r="K19" s="114">
+        <v>6</v>
+      </c>
+      <c r="L19" s="113" t="s">
+        <v>50</v>
+      </c>
+      <c r="M19" s="114" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" s="115" t="s">
+        <v>39</v>
+      </c>
+      <c r="O19" s="113" t="s">
+        <v>51</v>
+      </c>
+      <c r="P19" s="113" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q19" s="113" t="s">
+        <v>56</v>
+      </c>
+      <c r="R19" s="113" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="101"/>
+      <c r="B20" s="91" t="s">
         <v>244</v>
       </c>
-      <c r="D11" s="96" t="s">
+      <c r="C20" s="92" t="s">
+        <v>252</v>
+      </c>
+      <c r="D20" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="96"/>
-      <c r="F11" s="93"/>
-      <c r="I11" s="109" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="105" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="105" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="105" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="105" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="105" t="s">
-        <v>22</v>
-      </c>
-      <c r="O11" s="105" t="s">
-        <v>23</v>
-      </c>
-      <c r="P11" s="105" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q11" s="105" t="s">
-        <v>57</v>
-      </c>
-      <c r="R11" s="107" t="s">
+      <c r="E20" s="92"/>
+      <c r="F20" s="18"/>
+      <c r="I20" s="114"/>
+      <c r="J20" s="114"/>
+      <c r="K20" s="114"/>
+      <c r="L20" s="113"/>
+      <c r="M20" s="114"/>
+      <c r="N20" s="115"/>
+      <c r="O20" s="113"/>
+      <c r="P20" s="113"/>
+      <c r="Q20" s="113"/>
+      <c r="R20" s="113"/>
+    </row>
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="101"/>
+      <c r="B21" s="91" t="s">
+        <v>246</v>
+      </c>
+      <c r="C21" s="92" t="s">
+        <v>253</v>
+      </c>
+      <c r="D21" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="92"/>
+      <c r="F21" s="18"/>
+      <c r="I21" s="114" t="s">
+        <v>259</v>
+      </c>
+      <c r="J21" s="114">
+        <v>3</v>
+      </c>
+      <c r="K21" s="114">
+        <v>6</v>
+      </c>
+      <c r="L21" s="113" t="s">
+        <v>260</v>
+      </c>
+      <c r="M21" s="114" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" s="115" t="s">
+        <v>39</v>
+      </c>
+      <c r="O21" s="113" t="s">
+        <v>261</v>
+      </c>
+      <c r="P21" s="113" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q21" s="113" t="s">
+        <v>263</v>
+      </c>
+      <c r="R21" s="113" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="101"/>
+      <c r="B22" s="91"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="92"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="18"/>
+      <c r="I22" s="114"/>
+      <c r="J22" s="114"/>
+      <c r="K22" s="114"/>
+      <c r="L22" s="113"/>
+      <c r="M22" s="114"/>
+      <c r="N22" s="115"/>
+      <c r="O22" s="113"/>
+      <c r="P22" s="113"/>
+      <c r="Q22" s="113"/>
+      <c r="R22" s="113"/>
+    </row>
+    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="101"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="101"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="92"/>
+    </row>
+    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="93" t="s">
+        <v>288</v>
+      </c>
+      <c r="B25" s="91"/>
+      <c r="C25" s="92" t="s">
+        <v>289</v>
+      </c>
+      <c r="D25" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="F25" s="92" t="s">
+        <v>264</v>
+      </c>
+      <c r="N25" s="114"/>
+    </row>
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="93" t="s">
+        <v>293</v>
+      </c>
+      <c r="B26" s="92"/>
+      <c r="C26" s="92" t="s">
+        <v>290</v>
+      </c>
+      <c r="D26" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="F26" s="92" t="s">
+        <v>264</v>
+      </c>
+      <c r="N26" s="114"/>
+    </row>
+    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="93" t="s">
+        <v>294</v>
+      </c>
+      <c r="B27" s="92"/>
+      <c r="C27" s="92" t="s">
+        <v>291</v>
+      </c>
+      <c r="D27" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="92" t="s">
+        <v>292</v>
+      </c>
+      <c r="F27" s="92" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="93" t="s">
+        <v>296</v>
+      </c>
+      <c r="B28" s="92" t="s">
+        <v>297</v>
+      </c>
+      <c r="C28" s="92" t="s">
+        <v>301</v>
+      </c>
+      <c r="D28" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="92"/>
+      <c r="F28" s="92" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="93" t="s">
+        <v>295</v>
+      </c>
+      <c r="B29" s="92" t="s">
+        <v>297</v>
+      </c>
+      <c r="C29" s="92" t="s">
+        <v>300</v>
+      </c>
+      <c r="D29" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="92"/>
+      <c r="F29" s="92"/>
+    </row>
+    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="93" t="s">
+        <v>299</v>
+      </c>
+      <c r="B30" s="92" t="s">
+        <v>297</v>
+      </c>
+      <c r="C30" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="D30" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="92"/>
+      <c r="F30" s="92" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="93" t="s">
+        <v>298</v>
+      </c>
+      <c r="B31" s="92" t="s">
+        <v>297</v>
+      </c>
+      <c r="C31" s="92" t="s">
+        <v>303</v>
+      </c>
+      <c r="D31" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="92"/>
+      <c r="F31" s="92" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="112"/>
-      <c r="B12" s="95" t="s">
-        <v>245</v>
-      </c>
-      <c r="C12" s="96" t="s">
-        <v>246</v>
-      </c>
-      <c r="D12" s="96" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="96"/>
-      <c r="F12" s="93"/>
-      <c r="I12" s="110"/>
-      <c r="J12" s="106"/>
-      <c r="K12" s="106"/>
-      <c r="L12" s="106"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-      <c r="R12" s="108"/>
-    </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="112"/>
-      <c r="B13" s="95" t="s">
-        <v>247</v>
-      </c>
-      <c r="C13" s="96" t="s">
-        <v>248</v>
-      </c>
-      <c r="D13" s="96" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="96"/>
-      <c r="F13" s="93"/>
-      <c r="I13" s="102" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="102">
-        <v>7</v>
-      </c>
-      <c r="K13" s="102">
-        <v>30</v>
-      </c>
-      <c r="L13" s="103" t="s">
-        <v>41</v>
-      </c>
-      <c r="M13" s="102" t="s">
-        <v>33</v>
-      </c>
-      <c r="N13" s="104" t="s">
-        <v>40</v>
-      </c>
-      <c r="O13" s="103" t="s">
-        <v>42</v>
-      </c>
-      <c r="P13" s="103" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q13" s="103" t="s">
-        <v>53</v>
-      </c>
-      <c r="R13" s="103" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="112"/>
-      <c r="B14" s="95"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="93"/>
-      <c r="I14" s="102"/>
-      <c r="J14" s="102"/>
-      <c r="K14" s="102"/>
-      <c r="L14" s="103"/>
-      <c r="M14" s="102"/>
-      <c r="N14" s="104"/>
-      <c r="O14" s="103"/>
-      <c r="P14" s="103"/>
-      <c r="Q14" s="103"/>
-      <c r="R14" s="103"/>
-    </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="112"/>
-      <c r="B15" s="95"/>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="93"/>
-      <c r="I15" s="102" t="s">
-        <v>36</v>
-      </c>
-      <c r="J15" s="102">
-        <v>5</v>
-      </c>
-      <c r="K15" s="102">
-        <v>30</v>
-      </c>
-      <c r="L15" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="M15" s="102" t="s">
-        <v>33</v>
-      </c>
-      <c r="N15" s="104" t="s">
-        <v>40</v>
-      </c>
-      <c r="O15" s="103" t="s">
-        <v>45</v>
-      </c>
-      <c r="P15" s="103" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q15" s="103" t="s">
-        <v>54</v>
-      </c>
-      <c r="R15" s="103" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="112"/>
-      <c r="B16" s="95"/>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="93"/>
-      <c r="I16" s="102"/>
-      <c r="J16" s="102"/>
-      <c r="K16" s="102"/>
-      <c r="L16" s="103"/>
-      <c r="M16" s="102"/>
-      <c r="N16" s="104"/>
-      <c r="O16" s="103"/>
-      <c r="P16" s="103"/>
-      <c r="Q16" s="103"/>
-      <c r="R16" s="103"/>
-    </row>
-    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="111" t="s">
-        <v>249</v>
-      </c>
-      <c r="B17" s="95" t="s">
-        <v>239</v>
-      </c>
-      <c r="C17" s="96" t="s">
-        <v>250</v>
-      </c>
-      <c r="D17" s="96" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="96"/>
-      <c r="F17" s="93"/>
-      <c r="I17" s="102" t="s">
-        <v>37</v>
-      </c>
-      <c r="J17" s="102">
-        <v>1</v>
-      </c>
-      <c r="K17" s="102">
-        <v>6</v>
-      </c>
-      <c r="L17" s="103" t="s">
-        <v>47</v>
-      </c>
-      <c r="M17" s="102" t="s">
-        <v>28</v>
-      </c>
-      <c r="N17" s="104" t="s">
-        <v>39</v>
-      </c>
-      <c r="O17" s="103" t="s">
-        <v>48</v>
-      </c>
-      <c r="P17" s="103" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q17" s="103" t="s">
-        <v>55</v>
-      </c>
-      <c r="R17" s="103" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="112"/>
-      <c r="B18" s="95" t="s">
-        <v>241</v>
-      </c>
-      <c r="C18" s="96" t="s">
-        <v>251</v>
-      </c>
-      <c r="D18" s="96" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="96"/>
-      <c r="F18" s="93"/>
-      <c r="I18" s="102"/>
-      <c r="J18" s="102"/>
-      <c r="K18" s="102"/>
-      <c r="L18" s="103"/>
-      <c r="M18" s="102"/>
-      <c r="N18" s="104"/>
-      <c r="O18" s="103"/>
-      <c r="P18" s="103"/>
-      <c r="Q18" s="103"/>
-      <c r="R18" s="103"/>
-    </row>
-    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="112"/>
-      <c r="B19" s="95" t="s">
-        <v>243</v>
-      </c>
-      <c r="C19" s="96" t="s">
-        <v>252</v>
-      </c>
-      <c r="D19" s="96" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="96"/>
-      <c r="F19" s="93"/>
-      <c r="I19" s="102" t="s">
-        <v>38</v>
-      </c>
-      <c r="J19" s="102">
-        <v>1</v>
-      </c>
-      <c r="K19" s="102">
-        <v>6</v>
-      </c>
-      <c r="L19" s="103" t="s">
-        <v>50</v>
-      </c>
-      <c r="M19" s="102" t="s">
-        <v>28</v>
-      </c>
-      <c r="N19" s="104" t="s">
-        <v>39</v>
-      </c>
-      <c r="O19" s="103" t="s">
-        <v>51</v>
-      </c>
-      <c r="P19" s="103" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q19" s="103" t="s">
-        <v>56</v>
-      </c>
-      <c r="R19" s="103" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="112"/>
-      <c r="B20" s="95" t="s">
-        <v>245</v>
-      </c>
-      <c r="C20" s="96" t="s">
-        <v>253</v>
-      </c>
-      <c r="D20" s="96" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="96"/>
-      <c r="F20" s="93"/>
-      <c r="I20" s="102"/>
-      <c r="J20" s="102"/>
-      <c r="K20" s="102"/>
-      <c r="L20" s="103"/>
-      <c r="M20" s="102"/>
-      <c r="N20" s="104"/>
-      <c r="O20" s="103"/>
-      <c r="P20" s="103"/>
-      <c r="Q20" s="103"/>
-      <c r="R20" s="103"/>
-    </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="112"/>
-      <c r="B21" s="95" t="s">
-        <v>247</v>
-      </c>
-      <c r="C21" s="96" t="s">
-        <v>254</v>
-      </c>
-      <c r="D21" s="96" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="96"/>
-      <c r="F21" s="93"/>
-      <c r="I21" s="102" t="s">
-        <v>260</v>
-      </c>
-      <c r="J21" s="102">
-        <v>3</v>
-      </c>
-      <c r="K21" s="102">
-        <v>6</v>
-      </c>
-      <c r="L21" s="103" t="s">
-        <v>261</v>
-      </c>
-      <c r="M21" s="102" t="s">
-        <v>28</v>
-      </c>
-      <c r="N21" s="104" t="s">
-        <v>39</v>
-      </c>
-      <c r="O21" s="103" t="s">
-        <v>262</v>
-      </c>
-      <c r="P21" s="103" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q21" s="103" t="s">
-        <v>264</v>
-      </c>
-      <c r="R21" s="103" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="112"/>
-      <c r="B22" s="95"/>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="93"/>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
-      <c r="K22" s="102"/>
-      <c r="L22" s="103"/>
-      <c r="M22" s="102"/>
-      <c r="N22" s="104"/>
-      <c r="O22" s="103"/>
-      <c r="P22" s="103"/>
-      <c r="Q22" s="103"/>
-      <c r="R22" s="103"/>
-    </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="112"/>
-      <c r="B23" s="95"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="93"/>
-    </row>
-    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="112"/>
-      <c r="B24" s="95"/>
-      <c r="C24" s="96"/>
-      <c r="D24" s="96"/>
-      <c r="E24" s="96"/>
-      <c r="F24" s="96"/>
-    </row>
-    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="97" t="s">
-        <v>289</v>
-      </c>
-      <c r="B25" s="95"/>
-      <c r="C25" s="96" t="s">
-        <v>290</v>
-      </c>
-      <c r="D25" s="96" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="96" t="s">
-        <v>293</v>
-      </c>
-      <c r="F25" s="96" t="s">
-        <v>265</v>
-      </c>
-      <c r="N25" s="102"/>
-    </row>
-    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="97" t="s">
-        <v>294</v>
-      </c>
-      <c r="B26" s="96"/>
-      <c r="C26" s="96" t="s">
-        <v>291</v>
-      </c>
-      <c r="D26" s="96" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="96" t="s">
-        <v>293</v>
-      </c>
-      <c r="F26" s="96" t="s">
-        <v>265</v>
-      </c>
-      <c r="N26" s="102"/>
-    </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="97" t="s">
-        <v>295</v>
-      </c>
-      <c r="B27" s="96"/>
-      <c r="C27" s="96" t="s">
-        <v>292</v>
-      </c>
-      <c r="D27" s="96" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="96" t="s">
-        <v>293</v>
-      </c>
-      <c r="F27" s="96" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="97" t="s">
-        <v>297</v>
-      </c>
-      <c r="B28" s="96" t="s">
-        <v>298</v>
-      </c>
-      <c r="C28" s="96" t="s">
-        <v>302</v>
-      </c>
-      <c r="D28" s="96" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="96"/>
-      <c r="F28" s="96" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="97" t="s">
-        <v>296</v>
-      </c>
-      <c r="B29" s="96" t="s">
-        <v>298</v>
-      </c>
-      <c r="C29" s="96" t="s">
-        <v>301</v>
-      </c>
-      <c r="D29" s="96" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="96"/>
-      <c r="F29" s="96"/>
-    </row>
-    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="97" t="s">
-        <v>300</v>
-      </c>
-      <c r="B30" s="96" t="s">
-        <v>298</v>
-      </c>
-      <c r="C30" s="96" t="s">
-        <v>303</v>
-      </c>
-      <c r="D30" s="96" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="96"/>
-      <c r="F30" s="96" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="97" t="s">
-        <v>299</v>
-      </c>
-      <c r="B31" s="96" t="s">
-        <v>298</v>
-      </c>
-      <c r="C31" s="96" t="s">
+    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="93" t="s">
         <v>304</v>
       </c>
-      <c r="D31" s="96" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="96"/>
-      <c r="F31" s="96" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="97" t="s">
+      <c r="B32" s="92"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="95"/>
+    </row>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="93" t="s">
         <v>305</v>
       </c>
-      <c r="B32" s="96"/>
-      <c r="C32" s="92"/>
-      <c r="D32" s="92"/>
-      <c r="E32" s="98"/>
-      <c r="F32" s="99"/>
-    </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="97" t="s">
-        <v>306</v>
-      </c>
-      <c r="B33" s="100"/>
-      <c r="C33" s="92"/>
-      <c r="D33" s="92"/>
-      <c r="E33" s="98"/>
-      <c r="F33" s="99"/>
+      <c r="B33" s="96"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="95"/>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="97" t="s">
+      <c r="A34" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="100"/>
-      <c r="C34" s="92"/>
-      <c r="D34" s="92"/>
-      <c r="E34" s="98"/>
-      <c r="F34" s="99"/>
+      <c r="B34" s="96"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="94"/>
+      <c r="F34" s="95"/>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="97" t="s">
+      <c r="A35" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="100"/>
-      <c r="C35" s="92"/>
-      <c r="D35" s="92"/>
-      <c r="E35" s="98"/>
-      <c r="F35" s="99"/>
+      <c r="B35" s="96"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="95"/>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="97" t="s">
+      <c r="A36" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="100"/>
-      <c r="C36" s="92"/>
-      <c r="D36" s="92"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="99"/>
+      <c r="B36" s="96"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="94"/>
+      <c r="F36" s="95"/>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="97" t="s">
+      <c r="A37" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="100"/>
-      <c r="C37" s="92"/>
-      <c r="D37" s="92"/>
-      <c r="E37" s="98"/>
-      <c r="F37" s="99"/>
+      <c r="B37" s="96"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="95"/>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="97" t="s">
+      <c r="A38" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="100"/>
-      <c r="C38" s="92"/>
-      <c r="D38" s="92"/>
-      <c r="E38" s="98"/>
-      <c r="F38" s="99"/>
+      <c r="B38" s="96"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="94"/>
+      <c r="F38" s="95"/>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="97" t="s">
+      <c r="A39" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="100"/>
-      <c r="C39" s="92"/>
-      <c r="D39" s="92"/>
-      <c r="E39" s="98"/>
-      <c r="F39" s="99"/>
+      <c r="B39" s="96"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="94"/>
+      <c r="F39" s="95"/>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="97" t="s">
+      <c r="A40" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="100"/>
-      <c r="C40" s="92"/>
-      <c r="D40" s="92"/>
-      <c r="E40" s="98"/>
-      <c r="F40" s="99"/>
+      <c r="B40" s="96"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="A17:A24"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="R17:R18"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="R19:R20"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="R21:R22"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="Q17:Q18"/>
     <mergeCell ref="O21:O22"/>
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="J15:J16"/>
@@ -3734,32 +3716,39 @@
     <mergeCell ref="O15:O16"/>
     <mergeCell ref="O17:O18"/>
     <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="Q17:Q18"/>
     <mergeCell ref="N19:N20"/>
     <mergeCell ref="N21:N22"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="R17:R18"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="R19:R20"/>
-    <mergeCell ref="Q21:Q22"/>
-    <mergeCell ref="R21:R22"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="A17:A24"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3796,18 +3785,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="138" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
     </row>
     <row r="2" spans="1:19" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
@@ -3828,14 +3817,14 @@
       <c r="F2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="124" t="s">
+      <c r="G2" s="190" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="125"/>
-      <c r="I2" s="124" t="s">
+      <c r="H2" s="191"/>
+      <c r="I2" s="190" t="s">
         <v>136</v>
       </c>
-      <c r="J2" s="125"/>
+      <c r="J2" s="191"/>
       <c r="L2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3862,7 +3851,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="192" t="s">
         <v>137</v>
       </c>
       <c r="B3" s="21"/>
@@ -3870,16 +3859,16 @@
         <v>117</v>
       </c>
       <c r="D3" s="84" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F3" s="21"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="129"/>
-      <c r="J3" s="131"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="196"/>
+      <c r="I3" s="195"/>
+      <c r="J3" s="197"/>
       <c r="L3" s="3" t="s">
         <v>90</v>
       </c>
@@ -3906,22 +3895,22 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="127"/>
+      <c r="A4" s="193"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23" t="s">
         <v>118</v>
       </c>
       <c r="D4" s="83" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F4" s="23"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="132"/>
-      <c r="J4" s="134"/>
+      <c r="G4" s="198"/>
+      <c r="H4" s="199"/>
+      <c r="I4" s="198"/>
+      <c r="J4" s="200"/>
       <c r="L4" s="3" t="s">
         <v>91</v>
       </c>
@@ -3948,7 +3937,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="128"/>
+      <c r="A5" s="194"/>
       <c r="B5" s="24"/>
       <c r="C5" s="24" t="s">
         <v>119</v>
@@ -3960,10 +3949,10 @@
         <v>34</v>
       </c>
       <c r="F5" s="24"/>
-      <c r="G5" s="135"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="135"/>
-      <c r="J5" s="137"/>
+      <c r="G5" s="201"/>
+      <c r="H5" s="202"/>
+      <c r="I5" s="201"/>
+      <c r="J5" s="203"/>
       <c r="L5" s="3" t="s">
         <v>95</v>
       </c>
@@ -3990,7 +3979,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="162" t="s">
+      <c r="A6" s="188" t="s">
         <v>140</v>
       </c>
       <c r="B6" s="26"/>
@@ -4006,10 +3995,10 @@
       <c r="F6" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="G6" s="141"/>
-      <c r="H6" s="142"/>
-      <c r="I6" s="141"/>
-      <c r="J6" s="143"/>
+      <c r="G6" s="167"/>
+      <c r="H6" s="168"/>
+      <c r="I6" s="167"/>
+      <c r="J6" s="169"/>
       <c r="L6" s="3" t="s">
         <v>99</v>
       </c>
@@ -4036,7 +4025,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="163"/>
+      <c r="A7" s="189"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28" t="s">
         <v>123</v>
@@ -4050,10 +4039,10 @@
       <c r="F7" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="G7" s="144"/>
-      <c r="H7" s="145"/>
-      <c r="I7" s="144"/>
-      <c r="J7" s="146"/>
+      <c r="G7" s="170"/>
+      <c r="H7" s="171"/>
+      <c r="I7" s="170"/>
+      <c r="J7" s="172"/>
       <c r="L7" s="67" t="s">
         <v>87</v>
       </c>
@@ -4080,7 +4069,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="147" t="s">
+      <c r="A8" s="173" t="s">
         <v>139</v>
       </c>
       <c r="B8" s="29"/>
@@ -4096,12 +4085,12 @@
       <c r="F8" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="G8" s="159"/>
-      <c r="H8" s="161"/>
-      <c r="I8" s="159"/>
-      <c r="J8" s="160"/>
+      <c r="G8" s="185"/>
+      <c r="H8" s="187"/>
+      <c r="I8" s="185"/>
+      <c r="J8" s="186"/>
       <c r="L8" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M8" s="4">
         <v>15</v>
@@ -4110,7 +4099,7 @@
         <v>30</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P8" s="4" t="s">
         <v>33</v>
@@ -4119,14 +4108,14 @@
         <v>34</v>
       </c>
       <c r="R8" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="S8" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="S8" s="4" t="s">
-        <v>286</v>
-      </c>
     </row>
     <row r="9" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="148"/>
+      <c r="A9" s="174"/>
       <c r="B9" s="30"/>
       <c r="C9" s="30" t="s">
         <v>123</v>
@@ -4146,13 +4135,13 @@
       <c r="J9" s="71"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="149"/>
+      <c r="A10" s="175"/>
       <c r="B10" s="31"/>
       <c r="C10" s="31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E10" s="31" t="s">
         <v>29</v>
@@ -4166,7 +4155,7 @@
       <c r="J10" s="74"/>
     </row>
     <row r="11" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="138" t="s">
+      <c r="A11" s="164" t="s">
         <v>138</v>
       </c>
       <c r="B11" s="32"/>
@@ -4182,13 +4171,13 @@
       <c r="F11" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="G11" s="153"/>
-      <c r="H11" s="154"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="155"/>
+      <c r="G11" s="179"/>
+      <c r="H11" s="180"/>
+      <c r="I11" s="179"/>
+      <c r="J11" s="181"/>
     </row>
     <row r="12" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="139"/>
+      <c r="A12" s="165"/>
       <c r="B12" s="33"/>
       <c r="C12" s="33" t="s">
         <v>121</v>
@@ -4202,10 +4191,10 @@
       <c r="F12" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="G12" s="156"/>
-      <c r="H12" s="157"/>
-      <c r="I12" s="156"/>
-      <c r="J12" s="158"/>
+      <c r="G12" s="182"/>
+      <c r="H12" s="183"/>
+      <c r="I12" s="182"/>
+      <c r="J12" s="184"/>
       <c r="L12" s="65"/>
       <c r="M12" s="65"/>
       <c r="N12" s="65"/>
@@ -4216,7 +4205,7 @@
       <c r="S12" s="65"/>
     </row>
     <row r="13" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="140"/>
+      <c r="A13" s="166"/>
       <c r="B13" s="34"/>
       <c r="C13" s="34" t="s">
         <v>122</v>
@@ -4230,10 +4219,10 @@
       <c r="F13" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="G13" s="150"/>
-      <c r="H13" s="151"/>
-      <c r="I13" s="150"/>
-      <c r="J13" s="152"/>
+      <c r="G13" s="176"/>
+      <c r="H13" s="177"/>
+      <c r="I13" s="176"/>
+      <c r="J13" s="178"/>
       <c r="L13" s="66"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
@@ -4244,7 +4233,7 @@
       <c r="S13" s="6"/>
     </row>
     <row r="14" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="192" t="s">
+      <c r="A14" s="124" t="s">
         <v>141</v>
       </c>
       <c r="B14" s="35"/>
@@ -4260,10 +4249,10 @@
       <c r="F14" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="G14" s="164"/>
-      <c r="H14" s="164"/>
-      <c r="I14" s="164"/>
-      <c r="J14" s="164"/>
+      <c r="G14" s="163"/>
+      <c r="H14" s="163"/>
+      <c r="I14" s="163"/>
+      <c r="J14" s="163"/>
       <c r="L14" s="66"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
@@ -4274,13 +4263,13 @@
       <c r="S14" s="6"/>
     </row>
     <row r="15" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="193"/>
+      <c r="A15" s="125"/>
       <c r="B15" s="36"/>
       <c r="C15" s="36" t="s">
         <v>124</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E15" s="36" t="s">
         <v>26</v>
@@ -4288,10 +4277,10 @@
       <c r="F15" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="G15" s="165"/>
-      <c r="H15" s="165"/>
-      <c r="I15" s="165"/>
-      <c r="J15" s="165"/>
+      <c r="G15" s="154"/>
+      <c r="H15" s="154"/>
+      <c r="I15" s="154"/>
+      <c r="J15" s="154"/>
       <c r="L15" s="66"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
@@ -4302,13 +4291,13 @@
       <c r="S15" s="6"/>
     </row>
     <row r="16" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="193"/>
+      <c r="A16" s="125"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36" t="s">
         <v>125</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E16" s="36" t="s">
         <v>26</v>
@@ -4316,10 +4305,10 @@
       <c r="F16" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="G16" s="165"/>
-      <c r="H16" s="165"/>
-      <c r="I16" s="165"/>
-      <c r="J16" s="165"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
       <c r="L16" s="66"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
@@ -4330,13 +4319,13 @@
       <c r="S16" s="6"/>
     </row>
     <row r="17" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="193"/>
+      <c r="A17" s="125"/>
       <c r="B17" s="36"/>
       <c r="C17" s="36" t="s">
         <v>126</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E17" s="36" t="s">
         <v>26</v>
@@ -4344,10 +4333,10 @@
       <c r="F17" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="G17" s="165"/>
-      <c r="H17" s="165"/>
-      <c r="I17" s="165"/>
-      <c r="J17" s="165"/>
+      <c r="G17" s="154"/>
+      <c r="H17" s="154"/>
+      <c r="I17" s="154"/>
+      <c r="J17" s="154"/>
       <c r="L17" s="66"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
@@ -4358,13 +4347,13 @@
       <c r="S17" s="6"/>
     </row>
     <row r="18" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="193"/>
+      <c r="A18" s="125"/>
       <c r="B18" s="36"/>
       <c r="C18" s="36" t="s">
         <v>127</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E18" s="36" t="s">
         <v>26</v>
@@ -4372,19 +4361,19 @@
       <c r="F18" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="G18" s="165"/>
-      <c r="H18" s="165"/>
-      <c r="I18" s="165"/>
-      <c r="J18" s="165"/>
+      <c r="G18" s="154"/>
+      <c r="H18" s="154"/>
+      <c r="I18" s="154"/>
+      <c r="J18" s="154"/>
     </row>
     <row r="19" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="193"/>
+      <c r="A19" s="125"/>
       <c r="B19" s="36"/>
       <c r="C19" s="36" t="s">
         <v>128</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E19" s="36" t="s">
         <v>26</v>
@@ -4392,19 +4381,19 @@
       <c r="F19" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="G19" s="165"/>
-      <c r="H19" s="165"/>
-      <c r="I19" s="165"/>
-      <c r="J19" s="165"/>
+      <c r="G19" s="154"/>
+      <c r="H19" s="154"/>
+      <c r="I19" s="154"/>
+      <c r="J19" s="154"/>
     </row>
     <row r="20" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="193"/>
+      <c r="A20" s="125"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36" t="s">
         <v>129</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E20" s="36" t="s">
         <v>26</v>
@@ -4412,19 +4401,19 @@
       <c r="F20" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165"/>
-      <c r="J20" s="165"/>
+      <c r="G20" s="154"/>
+      <c r="H20" s="154"/>
+      <c r="I20" s="154"/>
+      <c r="J20" s="154"/>
     </row>
     <row r="21" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="194"/>
+      <c r="A21" s="126"/>
       <c r="B21" s="38"/>
       <c r="C21" s="39" t="s">
         <v>130</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E21" s="39" t="s">
         <v>26</v>
@@ -4432,13 +4421,13 @@
       <c r="F21" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="G21" s="188"/>
-      <c r="H21" s="188"/>
-      <c r="I21" s="188"/>
-      <c r="J21" s="188"/>
+      <c r="G21" s="155"/>
+      <c r="H21" s="155"/>
+      <c r="I21" s="155"/>
+      <c r="J21" s="155"/>
     </row>
     <row r="22" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="166" t="s">
+      <c r="A22" s="159" t="s">
         <v>142</v>
       </c>
       <c r="B22" s="40"/>
@@ -4454,19 +4443,19 @@
       <c r="F22" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="189"/>
-      <c r="I22" s="172"/>
-      <c r="J22" s="173"/>
+      <c r="G22" s="156"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="156"/>
+      <c r="J22" s="162"/>
     </row>
     <row r="23" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="167"/>
+      <c r="A23" s="160"/>
       <c r="B23" s="42"/>
       <c r="C23" s="43" t="s">
         <v>124</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E23" s="42" t="s">
         <v>26</v>
@@ -4474,19 +4463,19 @@
       <c r="F23" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="G23" s="169"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="169"/>
-      <c r="J23" s="171"/>
+      <c r="G23" s="146"/>
+      <c r="H23" s="158"/>
+      <c r="I23" s="146"/>
+      <c r="J23" s="147"/>
     </row>
     <row r="24" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="167"/>
+      <c r="A24" s="160"/>
       <c r="B24" s="42"/>
       <c r="C24" s="43" t="s">
         <v>125</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E24" s="42" t="s">
         <v>26</v>
@@ -4494,19 +4483,19 @@
       <c r="F24" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="G24" s="169"/>
-      <c r="H24" s="170"/>
-      <c r="I24" s="169"/>
-      <c r="J24" s="171"/>
+      <c r="G24" s="146"/>
+      <c r="H24" s="158"/>
+      <c r="I24" s="146"/>
+      <c r="J24" s="147"/>
     </row>
     <row r="25" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="167"/>
+      <c r="A25" s="160"/>
       <c r="B25" s="42"/>
       <c r="C25" s="43" t="s">
         <v>126</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E25" s="42" t="s">
         <v>26</v>
@@ -4514,19 +4503,19 @@
       <c r="F25" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="G25" s="169"/>
-      <c r="H25" s="170"/>
-      <c r="I25" s="169"/>
-      <c r="J25" s="171"/>
+      <c r="G25" s="146"/>
+      <c r="H25" s="158"/>
+      <c r="I25" s="146"/>
+      <c r="J25" s="147"/>
     </row>
     <row r="26" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="167"/>
+      <c r="A26" s="160"/>
       <c r="B26" s="42"/>
       <c r="C26" s="43" t="s">
         <v>127</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E26" s="42" t="s">
         <v>26</v>
@@ -4534,19 +4523,19 @@
       <c r="F26" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="G26" s="169"/>
-      <c r="H26" s="170"/>
-      <c r="I26" s="169"/>
-      <c r="J26" s="171"/>
+      <c r="G26" s="146"/>
+      <c r="H26" s="158"/>
+      <c r="I26" s="146"/>
+      <c r="J26" s="147"/>
     </row>
     <row r="27" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="167"/>
+      <c r="A27" s="160"/>
       <c r="B27" s="42"/>
       <c r="C27" s="43" t="s">
         <v>128</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E27" s="42" t="s">
         <v>26</v>
@@ -4554,19 +4543,19 @@
       <c r="F27" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="G27" s="169"/>
-      <c r="H27" s="170"/>
-      <c r="I27" s="169"/>
-      <c r="J27" s="171"/>
+      <c r="G27" s="146"/>
+      <c r="H27" s="158"/>
+      <c r="I27" s="146"/>
+      <c r="J27" s="147"/>
     </row>
     <row r="28" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="168"/>
+      <c r="A28" s="161"/>
       <c r="B28" s="44"/>
       <c r="C28" s="45" t="s">
         <v>129</v>
       </c>
       <c r="D28" s="44" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E28" s="44" t="s">
         <v>26</v>
@@ -4574,41 +4563,41 @@
       <c r="F28" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="G28" s="182"/>
-      <c r="H28" s="183"/>
-      <c r="I28" s="182"/>
-      <c r="J28" s="184"/>
+      <c r="G28" s="148"/>
+      <c r="H28" s="149"/>
+      <c r="I28" s="148"/>
+      <c r="J28" s="150"/>
     </row>
     <row r="29" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="195" t="s">
+      <c r="A29" s="127" t="s">
         <v>145</v>
       </c>
       <c r="B29" s="46"/>
       <c r="C29" s="46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D29" s="46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E29" s="46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F29" s="46" t="s">
-        <v>219</v>
-      </c>
-      <c r="G29" s="185"/>
-      <c r="H29" s="186"/>
-      <c r="I29" s="185"/>
-      <c r="J29" s="187"/>
+        <v>218</v>
+      </c>
+      <c r="G29" s="151"/>
+      <c r="H29" s="152"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="153"/>
     </row>
     <row r="30" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="196"/>
+      <c r="A30" s="128"/>
       <c r="B30" s="47"/>
       <c r="C30" s="48" t="s">
         <v>143</v>
       </c>
       <c r="D30" s="47" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E30" s="47" t="s">
         <v>26</v>
@@ -4616,10 +4605,10 @@
       <c r="F30" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="G30" s="176"/>
-      <c r="H30" s="177"/>
-      <c r="I30" s="176"/>
-      <c r="J30" s="178"/>
+      <c r="G30" s="140"/>
+      <c r="H30" s="141"/>
+      <c r="I30" s="140"/>
+      <c r="J30" s="142"/>
     </row>
     <row r="31" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="75" t="s">
@@ -4630,7 +4619,7 @@
         <v>132</v>
       </c>
       <c r="D31" s="49" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E31" s="49" t="s">
         <v>34</v>
@@ -4638,10 +4627,10 @@
       <c r="F31" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="G31" s="179"/>
-      <c r="H31" s="180"/>
-      <c r="I31" s="179"/>
-      <c r="J31" s="181"/>
+      <c r="G31" s="143"/>
+      <c r="H31" s="144"/>
+      <c r="I31" s="143"/>
+      <c r="J31" s="145"/>
     </row>
     <row r="32" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="53" t="s">
@@ -4651,10 +4640,10 @@
         <v>152</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D32" s="52" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E32" s="52" t="s">
         <v>26</v>
@@ -4662,10 +4651,10 @@
       <c r="F32" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="G32" s="200"/>
-      <c r="H32" s="201"/>
-      <c r="I32" s="200"/>
-      <c r="J32" s="202"/>
+      <c r="G32" s="132"/>
+      <c r="H32" s="133"/>
+      <c r="I32" s="132"/>
+      <c r="J32" s="134"/>
     </row>
     <row r="33" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="53" t="s">
@@ -4675,10 +4664,10 @@
         <v>152</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D33" s="52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E33" s="53" t="s">
         <v>26</v>
@@ -4686,10 +4675,10 @@
       <c r="F33" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="G33" s="203"/>
-      <c r="H33" s="204"/>
-      <c r="I33" s="203"/>
-      <c r="J33" s="205"/>
+      <c r="G33" s="135"/>
+      <c r="H33" s="136"/>
+      <c r="I33" s="135"/>
+      <c r="J33" s="137"/>
     </row>
     <row r="34" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="53" t="s">
@@ -4699,10 +4688,10 @@
         <v>152</v>
       </c>
       <c r="C34" s="51" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D34" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E34" s="54" t="s">
         <v>26</v>
@@ -4710,23 +4699,23 @@
       <c r="F34" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="G34" s="197"/>
-      <c r="H34" s="198"/>
-      <c r="I34" s="197"/>
-      <c r="J34" s="199"/>
+      <c r="G34" s="129"/>
+      <c r="H34" s="130"/>
+      <c r="I34" s="129"/>
+      <c r="J34" s="131"/>
     </row>
     <row r="35" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="79" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B35" s="53" t="s">
         <v>152</v>
       </c>
       <c r="C35" s="51" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E35" s="54" t="s">
         <v>26</v>
@@ -4734,10 +4723,10 @@
       <c r="F35" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="G35" s="197"/>
-      <c r="H35" s="198"/>
-      <c r="I35" s="197"/>
-      <c r="J35" s="199"/>
+      <c r="G35" s="129"/>
+      <c r="H35" s="130"/>
+      <c r="I35" s="129"/>
+      <c r="J35" s="131"/>
     </row>
     <row r="36" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="77" t="s">
@@ -4747,10 +4736,10 @@
         <v>153</v>
       </c>
       <c r="C36" s="56" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D36" s="55" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E36" s="55" t="s">
         <v>26</v>
@@ -4758,10 +4747,10 @@
       <c r="F36" s="55" t="s">
         <v>157</v>
       </c>
-      <c r="G36" s="190"/>
-      <c r="H36" s="190"/>
-      <c r="I36" s="190"/>
-      <c r="J36" s="191"/>
+      <c r="G36" s="122"/>
+      <c r="H36" s="122"/>
+      <c r="I36" s="122"/>
+      <c r="J36" s="123"/>
     </row>
     <row r="37" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="57" t="s">
@@ -4771,10 +4760,10 @@
         <v>153</v>
       </c>
       <c r="C37" s="56" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D37" s="55" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E37" s="55" t="s">
         <v>26</v>
@@ -4782,10 +4771,10 @@
       <c r="F37" s="55" t="s">
         <v>157</v>
       </c>
-      <c r="G37" s="190"/>
-      <c r="H37" s="190"/>
-      <c r="I37" s="190"/>
-      <c r="J37" s="191"/>
+      <c r="G37" s="122"/>
+      <c r="H37" s="122"/>
+      <c r="I37" s="122"/>
+      <c r="J37" s="123"/>
     </row>
     <row r="38" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A38" s="58" t="s">
@@ -4795,10 +4784,10 @@
         <v>153</v>
       </c>
       <c r="C38" s="56" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D38" s="59" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E38" s="59" t="s">
         <v>26</v>
@@ -4806,10 +4795,10 @@
       <c r="F38" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="G38" s="190"/>
-      <c r="H38" s="190"/>
-      <c r="I38" s="190"/>
-      <c r="J38" s="191"/>
+      <c r="G38" s="122"/>
+      <c r="H38" s="122"/>
+      <c r="I38" s="122"/>
+      <c r="J38" s="123"/>
     </row>
     <row r="39" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A39" s="42" t="s">
@@ -4820,7 +4809,7 @@
       </c>
       <c r="C39" s="42"/>
       <c r="D39" s="42" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E39" s="42" t="s">
         <v>26</v>
@@ -4842,7 +4831,7 @@
       </c>
       <c r="C40" s="42"/>
       <c r="D40" s="42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E40" s="42" t="s">
         <v>26</v>
@@ -4858,7 +4847,7 @@
     <row r="41" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A41" s="85"/>
       <c r="B41" s="85" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C41" s="85"/>
       <c r="D41" s="85"/>
@@ -4937,6 +4926,68 @@
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G27:H27"/>
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="I37:J37"/>
@@ -4953,68 +5004,6 @@
     <mergeCell ref="I33:J33"/>
     <mergeCell ref="G35:H35"/>
     <mergeCell ref="I35:J35"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5024,10 +5013,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27F8DC3-BDE0-43F3-979D-2CCDC5541D2C}">
-  <dimension ref="A1:U39"/>
+  <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D36" sqref="D35:F36"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5051,14 +5040,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="102" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -5079,14 +5068,14 @@
       <c r="F2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="211" t="s">
+      <c r="G2" s="205" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="211"/>
-      <c r="I2" s="211" t="s">
+      <c r="H2" s="205"/>
+      <c r="I2" s="205" t="s">
         <v>136</v>
       </c>
-      <c r="J2" s="211"/>
+      <c r="J2" s="205"/>
       <c r="N2" t="s">
         <v>62</v>
       </c>
@@ -5099,18 +5088,18 @@
       <c r="U2" s="6"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="212" t="s">
+      <c r="A3" s="204" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D3" s="81" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E3" s="81" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="206"/>
@@ -5143,16 +5132,16 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="212"/>
+      <c r="A4" s="204"/>
       <c r="B4" s="10"/>
       <c r="C4" s="80" t="s">
+        <v>275</v>
+      </c>
+      <c r="D4" s="82" t="s">
         <v>276</v>
       </c>
-      <c r="D4" s="82" t="s">
-        <v>277</v>
-      </c>
       <c r="E4" s="81" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="206"/>
@@ -5185,7 +5174,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="212"/>
+      <c r="A5" s="204"/>
       <c r="B5" s="10"/>
       <c r="C5" s="80" t="s">
         <v>119</v>
@@ -5227,7 +5216,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="212" t="s">
+      <c r="A6" s="204" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="10"/>
@@ -5273,7 +5262,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="212"/>
+      <c r="A7" s="204"/>
       <c r="B7" s="10"/>
       <c r="C7" s="80" t="s">
         <v>123</v>
@@ -5317,7 +5306,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="212" t="s">
+      <c r="A8" s="204" t="s">
         <v>104</v>
       </c>
       <c r="B8" s="10"/>
@@ -5363,7 +5352,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="212"/>
+      <c r="A9" s="204"/>
       <c r="B9" s="10"/>
       <c r="C9" s="80" t="s">
         <v>123</v>
@@ -5409,10 +5398,10 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="212"/>
+      <c r="A10" s="204"/>
       <c r="B10" s="10"/>
       <c r="C10" s="80" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D10" s="82" t="s">
         <v>174</v>
@@ -5429,7 +5418,7 @@
       <c r="J10" s="207"/>
     </row>
     <row r="11" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="212" t="s">
+      <c r="A11" s="204" t="s">
         <v>105</v>
       </c>
       <c r="B11" s="10"/>
@@ -5451,7 +5440,7 @@
       <c r="J11" s="207"/>
     </row>
     <row r="12" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="212"/>
+      <c r="A12" s="204"/>
       <c r="B12" s="10"/>
       <c r="C12" s="9" t="s">
         <v>121</v>
@@ -5471,7 +5460,7 @@
       <c r="J12" s="207"/>
     </row>
     <row r="13" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="212"/>
+      <c r="A13" s="204"/>
       <c r="B13" s="10"/>
       <c r="C13" s="9" t="s">
         <v>122</v>
@@ -5491,7 +5480,7 @@
       <c r="J13" s="207"/>
     </row>
     <row r="14" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="213" t="s">
+      <c r="A14" s="211" t="s">
         <v>106</v>
       </c>
       <c r="B14" s="10"/>
@@ -5513,7 +5502,7 @@
       <c r="J14" s="207"/>
     </row>
     <row r="15" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="214"/>
+      <c r="A15" s="212"/>
       <c r="B15" s="10"/>
       <c r="C15" s="9" t="s">
         <v>124</v>
@@ -5533,7 +5522,7 @@
       <c r="J15" s="207"/>
     </row>
     <row r="16" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="214"/>
+      <c r="A16" s="212"/>
       <c r="B16" s="10"/>
       <c r="C16" s="9" t="s">
         <v>125</v>
@@ -5553,7 +5542,7 @@
       <c r="J16" s="207"/>
     </row>
     <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="214"/>
+      <c r="A17" s="212"/>
       <c r="B17" s="10"/>
       <c r="C17" s="9" t="s">
         <v>126</v>
@@ -5573,7 +5562,7 @@
       <c r="J17" s="207"/>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="214"/>
+      <c r="A18" s="212"/>
       <c r="B18" s="10"/>
       <c r="C18" s="9" t="s">
         <v>127</v>
@@ -5593,7 +5582,7 @@
       <c r="J18" s="207"/>
     </row>
     <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="214"/>
+      <c r="A19" s="212"/>
       <c r="B19" s="10"/>
       <c r="C19" s="9" t="s">
         <v>128</v>
@@ -5613,7 +5602,7 @@
       <c r="J19" s="207"/>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="215"/>
+      <c r="A20" s="212"/>
       <c r="B20" s="10"/>
       <c r="C20" s="9" t="s">
         <v>129</v>
@@ -5627,27 +5616,21 @@
       <c r="F20" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G20" s="206"/>
-      <c r="H20" s="207"/>
-      <c r="I20" s="206"/>
-      <c r="J20" s="207"/>
+      <c r="G20" s="98"/>
+      <c r="H20" s="99"/>
+      <c r="I20" s="98"/>
+      <c r="J20" s="99"/>
     </row>
     <row r="21" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="208" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="9" t="s">
-        <v>123</v>
+      <c r="A21" s="213"/>
+      <c r="B21" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>186</v>
+        <v>308</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>167</v>
       </c>
       <c r="G21" s="206"/>
       <c r="H21" s="207"/>
@@ -5655,13 +5638,15 @@
       <c r="J21" s="207"/>
     </row>
     <row r="22" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="209"/>
+      <c r="A22" s="208" t="s">
+        <v>107</v>
+      </c>
       <c r="B22" s="12"/>
       <c r="C22" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>26</v>
@@ -5678,10 +5663,10 @@
       <c r="A23" s="209"/>
       <c r="B23" s="12"/>
       <c r="C23" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>26</v>
@@ -5698,10 +5683,10 @@
       <c r="A24" s="209"/>
       <c r="B24" s="12"/>
       <c r="C24" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>26</v>
@@ -5718,10 +5703,10 @@
       <c r="A25" s="209"/>
       <c r="B25" s="12"/>
       <c r="C25" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>26</v>
@@ -5738,10 +5723,10 @@
       <c r="A26" s="209"/>
       <c r="B26" s="12"/>
       <c r="C26" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>26</v>
@@ -5758,10 +5743,10 @@
       <c r="A27" s="209"/>
       <c r="B27" s="12"/>
       <c r="C27" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>26</v>
@@ -5775,13 +5760,13 @@
       <c r="J27" s="207"/>
     </row>
     <row r="28" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="210"/>
+      <c r="A28" s="209"/>
       <c r="B28" s="12"/>
       <c r="C28" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>26</v>
@@ -5795,15 +5780,13 @@
       <c r="J28" s="207"/>
     </row>
     <row r="29" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1" t="s">
-        <v>131</v>
+      <c r="A29" s="209"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>26</v>
@@ -5811,27 +5794,21 @@
       <c r="F29" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G29" s="206"/>
-      <c r="H29" s="207"/>
-      <c r="I29" s="206"/>
-      <c r="J29" s="207"/>
+      <c r="G29" s="98"/>
+      <c r="H29" s="99"/>
+      <c r="I29" s="98"/>
+      <c r="J29" s="99"/>
     </row>
     <row r="30" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="D30" s="82" t="s">
-        <v>197</v>
-      </c>
-      <c r="E30" s="82" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="82" t="s">
-        <v>167</v>
+      <c r="A30" s="210"/>
+      <c r="B30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="G30" s="206"/>
       <c r="H30" s="207"/>
@@ -5840,21 +5817,19 @@
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" t="s">
-        <v>134</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="D31" s="82" t="s">
-        <v>184</v>
-      </c>
-      <c r="E31" s="82" t="s">
+        <v>287</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="82" t="s">
+      <c r="F31" s="8" t="s">
         <v>167</v>
       </c>
       <c r="G31" s="206"/>
@@ -5864,19 +5839,17 @@
     </row>
     <row r="32" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B32" t="s">
-        <v>134</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="B32" s="1"/>
       <c r="C32" s="9" t="s">
-        <v>132</v>
+        <v>306</v>
       </c>
       <c r="D32" s="82" t="s">
-        <v>185</v>
+        <v>307</v>
       </c>
       <c r="E32" s="82" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F32" s="82" t="s">
         <v>167</v>
@@ -5888,16 +5861,16 @@
     </row>
     <row r="33" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>132</v>
       </c>
       <c r="D33" s="82" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="E33" s="82" t="s">
         <v>26</v>
@@ -5912,16 +5885,16 @@
     </row>
     <row r="34" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B34" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>132</v>
       </c>
       <c r="D34" s="82" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="E34" s="82" t="s">
         <v>26</v>
@@ -5936,7 +5909,7 @@
     </row>
     <row r="35" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B35" t="s">
         <v>133</v>
@@ -5945,7 +5918,7 @@
         <v>132</v>
       </c>
       <c r="D35" s="82" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E35" s="82" t="s">
         <v>26</v>
@@ -5958,18 +5931,18 @@
       <c r="I35" s="206"/>
       <c r="J35" s="207"/>
     </row>
-    <row r="36" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>132</v>
       </c>
       <c r="D36" s="82" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="E36" s="82" t="s">
         <v>26</v>
@@ -5984,13 +5957,21 @@
     </row>
     <row r="37" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="82" t="s">
+        <v>196</v>
+      </c>
+      <c r="E37" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" s="82" t="s">
         <v>167</v>
       </c>
       <c r="G37" s="206"/>
@@ -5998,15 +5979,23 @@
       <c r="I37" s="206"/>
       <c r="J37" s="207"/>
     </row>
-    <row r="38" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D38" s="82" t="s">
+        <v>183</v>
+      </c>
+      <c r="E38" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="82" t="s">
         <v>167</v>
       </c>
       <c r="G38" s="206"/>
@@ -6014,29 +6003,116 @@
       <c r="I38" s="206"/>
       <c r="J38" s="207"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1" t="s">
-        <v>135</v>
-      </c>
+    <row r="39" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8" t="s">
+        <v>167</v>
+      </c>
       <c r="G39" s="206"/>
       <c r="H39" s="207"/>
       <c r="I39" s="206"/>
       <c r="J39" s="207"/>
     </row>
+    <row r="40" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G40" s="206"/>
+      <c r="H40" s="207"/>
+      <c r="I40" s="206"/>
+      <c r="J40" s="207"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="206"/>
+      <c r="H41" s="207"/>
+      <c r="I41" s="206"/>
+      <c r="J41" s="207"/>
+    </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A21:A28"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A22:A30"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
@@ -6051,68 +6127,13 @@
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="G9:H9"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6141,20 +6162,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="216" t="s">
-        <v>220</v>
-      </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
+      <c r="A1" s="214" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" s="214"/>
+      <c r="C1" s="214"/>
+      <c r="D1" s="214"/>
+      <c r="E1" s="214"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="216"/>
-      <c r="B2" s="216"/>
-      <c r="C2" s="216"/>
-      <c r="D2" s="216"/>
-      <c r="E2" s="216"/>
+      <c r="A2" s="214"/>
+      <c r="B2" s="214"/>
+      <c r="C2" s="214"/>
+      <c r="D2" s="214"/>
+      <c r="E2" s="214"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -6184,7 +6205,7 @@
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
@@ -6193,19 +6214,19 @@
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>225</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6219,19 +6240,19 @@
         <v>2</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6245,19 +6266,19 @@
         <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>231</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>